<commit_message>
Added notes on database and use cases.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -2,20 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\finap\git\cs480\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtrepani\git\cs480\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Base" sheetId="1" r:id="rId1"/>
+    <sheet name="Databases" sheetId="2" r:id="rId2"/>
+    <sheet name="Use Cases" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,8 +25,268 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Administrator</author>
+  </authors>
+  <commentList>
+    <comment ref="E2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Administrator:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Hashed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Administrator:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Relative path; NOT absolute</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Administrator:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Relative path; NOT absolute</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Administrator</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Administrator:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Admin</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Administrator:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+User</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Administrator:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Server</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Administrator:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Google</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Administrator:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Admin</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Administrator:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Database</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Administrator:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Client</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="140">
   <si>
     <t>Design</t>
   </si>
@@ -214,13 +475,284 @@
   </si>
   <si>
     <t xml:space="preserve"> &gt;= 94</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>Dependencies</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Subtask</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>user id</t>
+  </si>
+  <si>
+    <t>calendar id</t>
+  </si>
+  <si>
+    <t>label id</t>
+  </si>
+  <si>
+    <t>task id</t>
+  </si>
+  <si>
+    <t>id UNIQUE AUTO_INCREMENT</t>
+  </si>
+  <si>
+    <t>admin BOOL</t>
+  </si>
+  <si>
+    <t>completed BOOL</t>
+  </si>
+  <si>
+    <t>description TEXT</t>
+  </si>
+  <si>
+    <t>name TEXT</t>
+  </si>
+  <si>
+    <t>name UNIQUE TEXT</t>
+  </si>
+  <si>
+    <t>active BOOL</t>
+  </si>
+  <si>
+    <t>notes TEXT</t>
+  </si>
+  <si>
+    <t>location TEXT</t>
+  </si>
+  <si>
+    <t>color TEXT</t>
+  </si>
+  <si>
+    <t>How to implement shareable labels and calendars?</t>
+  </si>
+  <si>
+    <t>reminder DATE</t>
+  </si>
+  <si>
+    <t>start time DATE</t>
+  </si>
+  <si>
+    <t>end time DATE</t>
+  </si>
+  <si>
+    <t>due date DATE</t>
+  </si>
+  <si>
+    <t>avatar TEXT</t>
+  </si>
+  <si>
+    <t>picture TEXT</t>
+  </si>
+  <si>
+    <t>Optimistic Concurrency for multiple users editting data at same time</t>
+  </si>
+  <si>
+    <t>http://www.asp.net/web-forms/overview/data-access/editing-inserting-and-deleting-data/implementing-optimistic-concurrency-cs</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>Notes: Client</t>
+  </si>
+  <si>
+    <t>Notes: Server</t>
+  </si>
+  <si>
+    <t>Use Case: Server</t>
+  </si>
+  <si>
+    <t>Use Case: Client</t>
+  </si>
+  <si>
+    <t>Conversation: Client</t>
+  </si>
+  <si>
+    <t>Conversation: Server</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>End Session</t>
+  </si>
+  <si>
+    <t>Start Session</t>
+  </si>
+  <si>
+    <t>1.
+2. Enter username and password</t>
+  </si>
+  <si>
+    <t>email TEXT</t>
+  </si>
+  <si>
+    <t>Create New User</t>
+  </si>
+  <si>
+    <t>Register New User/Self</t>
+  </si>
+  <si>
+    <t>1. Prompt client for credentials
+2.
+3. Compare username to database
+4. If no such username, notify client, reprompt client, and do not continue
+5. Else, hash the password and compare it against the password in the data and reprompt client
+6. If passwords do not much, notify client
+7. Else, Start Session*</t>
+  </si>
+  <si>
+    <t>Need to securely send information between client and server</t>
+  </si>
+  <si>
+    <t>1.
+2. Terminate session with corresponding id
+3. Notify client of successful termination</t>
+  </si>
+  <si>
+    <t>Can termination fail?</t>
+  </si>
+  <si>
+    <t>Sync Tasks/Events</t>
+  </si>
+  <si>
+    <t>Sync Tests/Events</t>
+  </si>
+  <si>
+    <t>Change Password</t>
+  </si>
+  <si>
+    <t>1. Prompt server to end session with session id</t>
+  </si>
+  <si>
+    <t>1.
+2. Enter old and new password
+3. Check that both new password fields match
+4. If not, restart from beginning
+5. Else, send to server</t>
+  </si>
+  <si>
+    <t>1. Prompt client to enter old password and new password (twice)
+2.
+3.
+4.
+5.
+6. Hash old password and compare against user's stored password
+7. If password does not match, notify client and do not continue
+8. Else, hash new password, replace old password, and notify client</t>
+  </si>
+  <si>
+    <t>1.
+2. Enter credentials
+3. Check that both password fields match
+4. If not, restart from beginning
+5. Else, send to server</t>
+  </si>
+  <si>
+    <t>1. Prompt client for username, password (twice), and email address
+2.
+3.
+4.
+5.
+6. Verify username is unique by comparing against database
+7. If username already exists, notify client
+8. Else, create user in database and notify client</t>
+  </si>
+  <si>
+    <t>Spin icon while syncing</t>
+  </si>
+  <si>
+    <t>Return cookie?</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Will sync calendars with google calendar</t>
+  </si>
+  <si>
+    <t>Share Label</t>
+  </si>
+  <si>
+    <t>Share Calendar</t>
+  </si>
+  <si>
+    <t>View-only option?</t>
+  </si>
+  <si>
+    <t>Update User(s) Access For Label</t>
+  </si>
+  <si>
+    <t>Update User(s) Access for Calendar</t>
+  </si>
+  <si>
+    <t>Add timeout on session based on inactivity</t>
+  </si>
+  <si>
+    <t>CRUDs: Calendar, Label, Task, Event, Subtask, ReminderTask, ReminderCalendar, Pictures, Notes</t>
+  </si>
+  <si>
+    <t>CRUD User</t>
+  </si>
+  <si>
+    <t>Local storage until Sync* instead of directly to server?</t>
+  </si>
+  <si>
+    <t>1.
+2. Enter information</t>
+  </si>
+  <si>
+    <t>1. Prompt client to CRUD users and enter information where applicable
+2.
+3. Sanitize input
+4. If invalid input, notify client
+5. Else, parse information and CRUD users accordingly</t>
+  </si>
+  <si>
+    <t>1. Prompt client to CRUD and enter information where applicable
+2.
+3. Sanitize input
+4. If input invalid, notify client 
+5. Else, parse information and CRUD accordingly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +768,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -245,10 +819,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -257,7 +840,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -267,11 +850,122 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -282,6 +976,31 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:M109" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A2:M109"/>
+  <sortState ref="A3:M109">
+    <sortCondition ref="F2:F109"/>
+  </sortState>
+  <tableColumns count="13">
+    <tableColumn id="1" name="Notes: Client" dataDxfId="14"/>
+    <tableColumn id="2" name="A" dataDxfId="13"/>
+    <tableColumn id="3" name="U" dataDxfId="12"/>
+    <tableColumn id="4" name="S" dataDxfId="11"/>
+    <tableColumn id="5" name="Use Case: Client" dataDxfId="10"/>
+    <tableColumn id="6" name="Conversation: Client" dataDxfId="9"/>
+    <tableColumn id="7" name="Conversation: Server" dataDxfId="8"/>
+    <tableColumn id="8" name="Use Case: Server" dataDxfId="7"/>
+    <tableColumn id="13" name="G" dataDxfId="6"/>
+    <tableColumn id="9" name="A2" dataDxfId="5"/>
+    <tableColumn id="10" name="D" dataDxfId="4"/>
+    <tableColumn id="11" name="C" dataDxfId="3"/>
+    <tableColumn id="12" name="Notes: Server" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -549,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,4 +1683,2084 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="12" width="16.7109375" customWidth="1"/>
+    <col min="13" max="14" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M109"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" style="9" customWidth="1"/>
+    <col min="2" max="4" width="5.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" style="9" customWidth="1"/>
+    <col min="10" max="12" width="5.85546875" customWidth="1"/>
+    <col min="13" max="13" width="25.140625" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+    </row>
+    <row r="2" spans="1:13" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" spans="1:13" ht="240" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M5" s="14"/>
+    </row>
+    <row r="6" spans="1:13" ht="225" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M10" s="14"/>
+    </row>
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M11" s="14"/>
+    </row>
+    <row r="12" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M12" s="14"/>
+    </row>
+    <row r="13" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M13" s="14"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="14"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="14"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="14"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="14"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="14"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="14"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="14"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="14"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="14"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="14"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="14"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="14"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="14"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="14"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="14"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="14"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="14"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="14"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="14"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="14"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="14"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="14"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="14"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="14"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="14"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="14"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="14"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="14"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="14"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="14"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="14"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="14"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="14"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="14"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="14"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="14"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="14"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="14"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="14"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="15"/>
+      <c r="M49" s="14"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="14"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
+      <c r="K50" s="15"/>
+      <c r="L50" s="15"/>
+      <c r="M50" s="14"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="15"/>
+      <c r="M51" s="14"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="14"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="15"/>
+      <c r="M52" s="14"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="14"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="14"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="14"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="14"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="15"/>
+      <c r="M55" s="14"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="14"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15"/>
+      <c r="L56" s="15"/>
+      <c r="M56" s="14"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="14"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="15"/>
+      <c r="M57" s="14"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="14"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="15"/>
+      <c r="L58" s="15"/>
+      <c r="M58" s="14"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="14"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="15"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="15"/>
+      <c r="M59" s="14"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="14"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="15"/>
+      <c r="J60" s="15"/>
+      <c r="K60" s="15"/>
+      <c r="L60" s="15"/>
+      <c r="M60" s="14"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="15"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="15"/>
+      <c r="M61" s="14"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="14"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="15"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="15"/>
+      <c r="M62" s="14"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="14"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="15"/>
+      <c r="M63" s="14"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="14"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="15"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="15"/>
+      <c r="M64" s="14"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="14"/>
+      <c r="B65" s="15"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="15"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="15"/>
+      <c r="M65" s="14"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="14"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="15"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="15"/>
+      <c r="M66" s="14"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="14"/>
+      <c r="B67" s="15"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="15"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="15"/>
+      <c r="M67" s="14"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="14"/>
+      <c r="B68" s="15"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="15"/>
+      <c r="J68" s="15"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="15"/>
+      <c r="M68" s="14"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="14"/>
+      <c r="B69" s="15"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="15"/>
+      <c r="J69" s="15"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="15"/>
+      <c r="M69" s="14"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="14"/>
+      <c r="B70" s="15"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="15"/>
+      <c r="J70" s="15"/>
+      <c r="K70" s="15"/>
+      <c r="L70" s="15"/>
+      <c r="M70" s="14"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" s="14"/>
+      <c r="B71" s="15"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="15"/>
+      <c r="J71" s="15"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="15"/>
+      <c r="M71" s="14"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="14"/>
+      <c r="B72" s="15"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="15"/>
+      <c r="J72" s="15"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="15"/>
+      <c r="M72" s="14"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="14"/>
+      <c r="B73" s="15"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="15"/>
+      <c r="J73" s="15"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="15"/>
+      <c r="M73" s="14"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="14"/>
+      <c r="B74" s="15"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="14"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="15"/>
+      <c r="J74" s="15"/>
+      <c r="K74" s="15"/>
+      <c r="L74" s="15"/>
+      <c r="M74" s="14"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="14"/>
+      <c r="B75" s="15"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="15"/>
+      <c r="J75" s="15"/>
+      <c r="K75" s="15"/>
+      <c r="L75" s="15"/>
+      <c r="M75" s="14"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="14"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="14"/>
+      <c r="H76" s="14"/>
+      <c r="I76" s="15"/>
+      <c r="J76" s="15"/>
+      <c r="K76" s="15"/>
+      <c r="L76" s="15"/>
+      <c r="M76" s="14"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="14"/>
+      <c r="B77" s="15"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="15"/>
+      <c r="J77" s="15"/>
+      <c r="K77" s="15"/>
+      <c r="L77" s="15"/>
+      <c r="M77" s="14"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" s="14"/>
+      <c r="B78" s="15"/>
+      <c r="C78" s="15"/>
+      <c r="D78" s="15"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="14"/>
+      <c r="I78" s="15"/>
+      <c r="J78" s="15"/>
+      <c r="K78" s="15"/>
+      <c r="L78" s="15"/>
+      <c r="M78" s="14"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" s="14"/>
+      <c r="B79" s="15"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="14"/>
+      <c r="I79" s="15"/>
+      <c r="J79" s="15"/>
+      <c r="K79" s="15"/>
+      <c r="L79" s="15"/>
+      <c r="M79" s="14"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" s="14"/>
+      <c r="B80" s="15"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="15"/>
+      <c r="J80" s="15"/>
+      <c r="K80" s="15"/>
+      <c r="L80" s="15"/>
+      <c r="M80" s="14"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" s="14"/>
+      <c r="B81" s="15"/>
+      <c r="C81" s="15"/>
+      <c r="D81" s="15"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="14"/>
+      <c r="H81" s="14"/>
+      <c r="I81" s="15"/>
+      <c r="J81" s="15"/>
+      <c r="K81" s="15"/>
+      <c r="L81" s="15"/>
+      <c r="M81" s="14"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" s="14"/>
+      <c r="B82" s="15"/>
+      <c r="C82" s="15"/>
+      <c r="D82" s="15"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="14"/>
+      <c r="H82" s="14"/>
+      <c r="I82" s="15"/>
+      <c r="J82" s="15"/>
+      <c r="K82" s="15"/>
+      <c r="L82" s="15"/>
+      <c r="M82" s="14"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83" s="14"/>
+      <c r="B83" s="15"/>
+      <c r="C83" s="15"/>
+      <c r="D83" s="15"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="12"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
+      <c r="I83" s="15"/>
+      <c r="J83" s="15"/>
+      <c r="K83" s="15"/>
+      <c r="L83" s="15"/>
+      <c r="M83" s="14"/>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84" s="14"/>
+      <c r="B84" s="15"/>
+      <c r="C84" s="15"/>
+      <c r="D84" s="15"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="14"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="15"/>
+      <c r="J84" s="15"/>
+      <c r="K84" s="15"/>
+      <c r="L84" s="15"/>
+      <c r="M84" s="14"/>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85" s="14"/>
+      <c r="B85" s="15"/>
+      <c r="C85" s="15"/>
+      <c r="D85" s="15"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="14"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="15"/>
+      <c r="J85" s="15"/>
+      <c r="K85" s="15"/>
+      <c r="L85" s="15"/>
+      <c r="M85" s="14"/>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86" s="14"/>
+      <c r="B86" s="15"/>
+      <c r="C86" s="15"/>
+      <c r="D86" s="15"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="12"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="15"/>
+      <c r="J86" s="15"/>
+      <c r="K86" s="15"/>
+      <c r="L86" s="15"/>
+      <c r="M86" s="14"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87" s="14"/>
+      <c r="B87" s="15"/>
+      <c r="C87" s="15"/>
+      <c r="D87" s="15"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="12"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="15"/>
+      <c r="J87" s="15"/>
+      <c r="K87" s="15"/>
+      <c r="L87" s="15"/>
+      <c r="M87" s="14"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88" s="14"/>
+      <c r="B88" s="15"/>
+      <c r="C88" s="15"/>
+      <c r="D88" s="15"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="14"/>
+      <c r="H88" s="14"/>
+      <c r="I88" s="15"/>
+      <c r="J88" s="15"/>
+      <c r="K88" s="15"/>
+      <c r="L88" s="15"/>
+      <c r="M88" s="14"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89" s="14"/>
+      <c r="B89" s="15"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="12"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="15"/>
+      <c r="J89" s="15"/>
+      <c r="K89" s="15"/>
+      <c r="L89" s="15"/>
+      <c r="M89" s="14"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90" s="14"/>
+      <c r="B90" s="15"/>
+      <c r="C90" s="15"/>
+      <c r="D90" s="15"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="12"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="15"/>
+      <c r="J90" s="15"/>
+      <c r="K90" s="15"/>
+      <c r="L90" s="15"/>
+      <c r="M90" s="14"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91" s="14"/>
+      <c r="B91" s="15"/>
+      <c r="C91" s="15"/>
+      <c r="D91" s="15"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="15"/>
+      <c r="J91" s="15"/>
+      <c r="K91" s="15"/>
+      <c r="L91" s="15"/>
+      <c r="M91" s="14"/>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92" s="14"/>
+      <c r="B92" s="15"/>
+      <c r="C92" s="15"/>
+      <c r="D92" s="15"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="12"/>
+      <c r="G92" s="14"/>
+      <c r="H92" s="14"/>
+      <c r="I92" s="15"/>
+      <c r="J92" s="15"/>
+      <c r="K92" s="15"/>
+      <c r="L92" s="15"/>
+      <c r="M92" s="14"/>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93" s="14"/>
+      <c r="B93" s="15"/>
+      <c r="C93" s="15"/>
+      <c r="D93" s="15"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="12"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="14"/>
+      <c r="I93" s="15"/>
+      <c r="J93" s="15"/>
+      <c r="K93" s="15"/>
+      <c r="L93" s="15"/>
+      <c r="M93" s="14"/>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94" s="14"/>
+      <c r="B94" s="15"/>
+      <c r="C94" s="15"/>
+      <c r="D94" s="15"/>
+      <c r="E94" s="14"/>
+      <c r="F94" s="12"/>
+      <c r="G94" s="14"/>
+      <c r="H94" s="14"/>
+      <c r="I94" s="15"/>
+      <c r="J94" s="15"/>
+      <c r="K94" s="15"/>
+      <c r="L94" s="15"/>
+      <c r="M94" s="14"/>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95" s="14"/>
+      <c r="B95" s="15"/>
+      <c r="C95" s="15"/>
+      <c r="D95" s="15"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="12"/>
+      <c r="G95" s="14"/>
+      <c r="H95" s="14"/>
+      <c r="I95" s="15"/>
+      <c r="J95" s="15"/>
+      <c r="K95" s="15"/>
+      <c r="L95" s="15"/>
+      <c r="M95" s="14"/>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A96" s="14"/>
+      <c r="B96" s="15"/>
+      <c r="C96" s="15"/>
+      <c r="D96" s="15"/>
+      <c r="E96" s="14"/>
+      <c r="F96" s="12"/>
+      <c r="G96" s="14"/>
+      <c r="H96" s="14"/>
+      <c r="I96" s="15"/>
+      <c r="J96" s="15"/>
+      <c r="K96" s="15"/>
+      <c r="L96" s="15"/>
+      <c r="M96" s="14"/>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A97" s="14"/>
+      <c r="B97" s="15"/>
+      <c r="C97" s="15"/>
+      <c r="D97" s="15"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="12"/>
+      <c r="G97" s="14"/>
+      <c r="H97" s="14"/>
+      <c r="I97" s="15"/>
+      <c r="J97" s="15"/>
+      <c r="K97" s="15"/>
+      <c r="L97" s="15"/>
+      <c r="M97" s="14"/>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A98" s="14"/>
+      <c r="B98" s="15"/>
+      <c r="C98" s="15"/>
+      <c r="D98" s="15"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="14"/>
+      <c r="H98" s="14"/>
+      <c r="I98" s="15"/>
+      <c r="J98" s="15"/>
+      <c r="K98" s="15"/>
+      <c r="L98" s="15"/>
+      <c r="M98" s="14"/>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A99" s="14"/>
+      <c r="B99" s="15"/>
+      <c r="C99" s="15"/>
+      <c r="D99" s="15"/>
+      <c r="E99" s="14"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="14"/>
+      <c r="H99" s="14"/>
+      <c r="I99" s="15"/>
+      <c r="J99" s="15"/>
+      <c r="K99" s="15"/>
+      <c r="L99" s="15"/>
+      <c r="M99" s="14"/>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A100" s="14"/>
+      <c r="B100" s="15"/>
+      <c r="C100" s="15"/>
+      <c r="D100" s="15"/>
+      <c r="E100" s="14"/>
+      <c r="F100" s="12"/>
+      <c r="G100" s="14"/>
+      <c r="H100" s="14"/>
+      <c r="I100" s="15"/>
+      <c r="J100" s="15"/>
+      <c r="K100" s="15"/>
+      <c r="L100" s="15"/>
+      <c r="M100" s="14"/>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A101" s="14"/>
+      <c r="B101" s="15"/>
+      <c r="C101" s="15"/>
+      <c r="D101" s="15"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="12"/>
+      <c r="G101" s="14"/>
+      <c r="H101" s="14"/>
+      <c r="I101" s="15"/>
+      <c r="J101" s="15"/>
+      <c r="K101" s="15"/>
+      <c r="L101" s="15"/>
+      <c r="M101" s="14"/>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A102" s="14"/>
+      <c r="B102" s="15"/>
+      <c r="C102" s="15"/>
+      <c r="D102" s="15"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="12"/>
+      <c r="G102" s="14"/>
+      <c r="H102" s="14"/>
+      <c r="I102" s="15"/>
+      <c r="J102" s="15"/>
+      <c r="K102" s="15"/>
+      <c r="L102" s="15"/>
+      <c r="M102" s="14"/>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103" s="14"/>
+      <c r="B103" s="15"/>
+      <c r="C103" s="15"/>
+      <c r="D103" s="15"/>
+      <c r="E103" s="14"/>
+      <c r="F103" s="12"/>
+      <c r="G103" s="14"/>
+      <c r="H103" s="14"/>
+      <c r="I103" s="15"/>
+      <c r="J103" s="15"/>
+      <c r="K103" s="15"/>
+      <c r="L103" s="15"/>
+      <c r="M103" s="14"/>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A104" s="14"/>
+      <c r="B104" s="15"/>
+      <c r="C104" s="15"/>
+      <c r="D104" s="15"/>
+      <c r="E104" s="14"/>
+      <c r="F104" s="12"/>
+      <c r="G104" s="14"/>
+      <c r="H104" s="14"/>
+      <c r="I104" s="15"/>
+      <c r="J104" s="15"/>
+      <c r="K104" s="15"/>
+      <c r="L104" s="15"/>
+      <c r="M104" s="14"/>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A105" s="14"/>
+      <c r="B105" s="15"/>
+      <c r="C105" s="15"/>
+      <c r="D105" s="15"/>
+      <c r="E105" s="14"/>
+      <c r="F105" s="12"/>
+      <c r="G105" s="14"/>
+      <c r="H105" s="14"/>
+      <c r="I105" s="15"/>
+      <c r="J105" s="15"/>
+      <c r="K105" s="15"/>
+      <c r="L105" s="15"/>
+      <c r="M105" s="14"/>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A106" s="14"/>
+      <c r="B106" s="15"/>
+      <c r="C106" s="15"/>
+      <c r="D106" s="15"/>
+      <c r="E106" s="14"/>
+      <c r="F106" s="12"/>
+      <c r="G106" s="14"/>
+      <c r="H106" s="14"/>
+      <c r="I106" s="15"/>
+      <c r="J106" s="15"/>
+      <c r="K106" s="15"/>
+      <c r="L106" s="15"/>
+      <c r="M106" s="14"/>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A107" s="14"/>
+      <c r="B107" s="15"/>
+      <c r="C107" s="15"/>
+      <c r="D107" s="15"/>
+      <c r="E107" s="14"/>
+      <c r="F107" s="12"/>
+      <c r="G107" s="14"/>
+      <c r="H107" s="14"/>
+      <c r="I107" s="15"/>
+      <c r="J107" s="15"/>
+      <c r="K107" s="15"/>
+      <c r="L107" s="15"/>
+      <c r="M107" s="14"/>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A108" s="14"/>
+      <c r="B108" s="15"/>
+      <c r="C108" s="15"/>
+      <c r="D108" s="15"/>
+      <c r="E108" s="14"/>
+      <c r="F108" s="12"/>
+      <c r="G108" s="14"/>
+      <c r="H108" s="14"/>
+      <c r="I108" s="15"/>
+      <c r="J108" s="15"/>
+      <c r="K108" s="15"/>
+      <c r="L108" s="15"/>
+      <c r="M108" s="14"/>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A109" s="14"/>
+      <c r="B109" s="15"/>
+      <c r="C109" s="15"/>
+      <c r="D109" s="15"/>
+      <c r="E109" s="14"/>
+      <c r="F109" s="12"/>
+      <c r="G109" s="14"/>
+      <c r="H109" s="14"/>
+      <c r="I109" s="15"/>
+      <c r="J109" s="15"/>
+      <c r="K109" s="15"/>
+      <c r="L109" s="15"/>
+      <c r="M109" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Notes, structure change, added tables sql and database class.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,8 @@
     <sheet name="Reminders" sheetId="4" r:id="rId3"/>
     <sheet name="Databases" sheetId="2" r:id="rId4"/>
     <sheet name="Use Cases" sheetId="3" r:id="rId5"/>
-    <sheet name="AngularJS" sheetId="6" r:id="rId6"/>
+    <sheet name="Classes" sheetId="7" r:id="rId6"/>
+    <sheet name="AngularJS" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="Slicer_Category">#N/A</definedName>
@@ -26,17 +27,18 @@
     <definedName name="Slicer_Done1">#N/A</definedName>
     <definedName name="Slicer_Look_Into">#N/A</definedName>
     <definedName name="Slicer_Look_Into1">#N/A</definedName>
+    <definedName name="Slicer_Remember">#N/A</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
-        <x14:slicerCache r:id="rId8"/>
         <x14:slicerCache r:id="rId9"/>
         <x14:slicerCache r:id="rId10"/>
+        <x14:slicerCache r:id="rId11"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -44,9 +46,10 @@
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
       <x15:slicerCaches xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicerCache r:id="rId11"/>
         <x14:slicerCache r:id="rId12"/>
         <x14:slicerCache r:id="rId13"/>
+        <x14:slicerCache r:id="rId14"/>
+        <x14:slicerCache r:id="rId15"/>
       </x15:slicerCaches>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -57,6 +60,40 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Fina Jo</author>
+  </authors>
+  <commentList>
+    <comment ref="D2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fina Jo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Things to remember near or at end of project</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Administrator</author>
@@ -135,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="0" shapeId="0">
+    <comment ref="H8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -159,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="1" shapeId="0">
+    <comment ref="A12" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -180,7 +217,8 @@
           </rPr>
           <t xml:space="preserve">
 Uses RRule standard
-Day ENUM('su', 'mo', 'tu', 'we', 'th', 'fr', 'sa')</t>
+Day ENUM('su', 'mo', 'tu', 'we', 'th', 'fr', 'sa')
+by_(?!set_pos).* stored in serialized arrays</t>
         </r>
       </text>
     </comment>
@@ -188,7 +226,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Administrator</author>
@@ -366,7 +404,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Administrator</author>
@@ -475,7 +513,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="252">
   <si>
     <t>Design</t>
   </si>
@@ -645,9 +683,6 @@
     <t>description TEXT</t>
   </si>
   <si>
-    <t>location TEXT</t>
-  </si>
-  <si>
     <t>avatar TEXT</t>
   </si>
   <si>
@@ -694,9 +729,6 @@
   </si>
   <si>
     <t>Start Session</t>
-  </si>
-  <si>
-    <t>email TEXT</t>
   </si>
   <si>
     <t>Create New User</t>
@@ -787,12 +819,6 @@
     <t>Column7</t>
   </si>
   <si>
-    <t>task(id) UNIQUE</t>
-  </si>
-  <si>
-    <t>event(id) UNIQUE</t>
-  </si>
-  <si>
     <t>Foreign Key1</t>
   </si>
   <si>
@@ -802,18 +828,9 @@
     <t>reminder DATETIME</t>
   </si>
   <si>
-    <t>color ENUM(/* colors here*/)</t>
-  </si>
-  <si>
     <t>Check if username and password is between 8 and 32 characters</t>
   </si>
   <si>
-    <t>name TEXT UNIQUE NOT NULL</t>
-  </si>
-  <si>
-    <t>name TEXT NOT NULL</t>
-  </si>
-  <si>
     <t>note TEXT</t>
   </si>
   <si>
@@ -841,15 +858,6 @@
     <t>recurrence</t>
   </si>
   <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>reminder</t>
-  </si>
-  <si>
     <t>calendar_user</t>
   </si>
   <si>
@@ -859,9 +867,6 @@
     <t>view_only BOOL</t>
   </si>
   <si>
-    <t>password TEXT NOT NULL</t>
-  </si>
-  <si>
     <t>admin BOOL DEFAULT false</t>
   </si>
   <si>
@@ -871,9 +876,6 @@
     <t>theme ENUM('light', 'dark') DEFAULT 'light'</t>
   </si>
   <si>
-    <t>user_id REFERENCES user(id)</t>
-  </si>
-  <si>
     <t>time_zone INT</t>
   </si>
   <si>
@@ -889,9 +891,6 @@
     <t>interval INT NOT_NULL DEFAULT 1</t>
   </si>
   <si>
-    <t xml:space="preserve">by_hour </t>
-  </si>
-  <si>
     <t>Column8</t>
   </si>
   <si>
@@ -901,12 +900,6 @@
     <t>Column10</t>
   </si>
   <si>
-    <t>by_month</t>
-  </si>
-  <si>
-    <t>by_day</t>
-  </si>
-  <si>
     <t>Column12</t>
   </si>
   <si>
@@ -919,24 +912,6 @@
     <t>Column14</t>
   </si>
   <si>
-    <t>by_second</t>
-  </si>
-  <si>
-    <t>by_minute</t>
-  </si>
-  <si>
-    <t>by_month_day</t>
-  </si>
-  <si>
-    <t>by_year_day</t>
-  </si>
-  <si>
-    <t>by_week_no</t>
-  </si>
-  <si>
-    <t>by_set_pos</t>
-  </si>
-  <si>
     <t>freq ENUM('secondly', 'minutely', 'hourly', 'daily', 'weekly', 'monthly', 'yearly') DEFAULT 'daily'</t>
   </si>
   <si>
@@ -958,9 +933,6 @@
     <t>Look into property bag pattern for user settings</t>
   </si>
   <si>
-    <t>summary TEXT NOT NULL</t>
-  </si>
-  <si>
     <t>Convert timezones as necessary</t>
   </si>
   <si>
@@ -988,9 +960,6 @@
     <t>Set utf8mb4 on PDO connection and database + tables?</t>
   </si>
   <si>
-    <t>REMEMBER!!</t>
-  </si>
-  <si>
     <t>Out-sourced files (FA and AngularJS) is for previously-cached versions</t>
   </si>
   <si>
@@ -1022,12 +991,6 @@
   </si>
   <si>
     <t>due DATETIME</t>
-  </si>
-  <si>
-    <t>start DATETIME</t>
-  </si>
-  <si>
-    <t>end DATETIME</t>
   </si>
   <si>
     <t>session</t>
@@ -1208,15 +1171,169 @@
     <t>Exception handler?</t>
   </si>
   <si>
-    <t>PHP: Convert $connection to main db vs test and set appropriate username and password</t>
-  </si>
-  <si>
-    <t>PHP: turn off error reporting off in php.ini when final product is done; set these:
+    <t>dt_end DATETIME</t>
+  </si>
+  <si>
+    <t>dt_start DATETIME</t>
+  </si>
+  <si>
+    <t>Implement transcations if necessary</t>
+  </si>
+  <si>
+    <t>Turn off error reporting off in php.ini when final product is done; set these:
   display_errors = Off
   display_startup_errors = Off</t>
   </si>
   <si>
-    <t>HTML/JS: Out-sourced files (FA and AngularJS) is for previously-cached versions</t>
+    <t>Convert $connection to main db vs test and set appropriate username and password</t>
+  </si>
+  <si>
+    <t>Remember</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>mb_internal_encoding('utf-8') AND mb_http_output('utf-8') in global include file</t>
+  </si>
+  <si>
+    <t>recurrence(id)</t>
+  </si>
+  <si>
+    <t>activity_prefs</t>
+  </si>
+  <si>
+    <t>activity_prefs(id)</t>
+  </si>
+  <si>
+    <t>color VARCHAR(32)</t>
+  </si>
+  <si>
+    <t>name VARCHAR(32) UNIQUE NOT NULL</t>
+  </si>
+  <si>
+    <t>password VARCHAR(512) NOT NULL</t>
+  </si>
+  <si>
+    <t>email VARCHAR(64)</t>
+  </si>
+  <si>
+    <t>by_second TEXT</t>
+  </si>
+  <si>
+    <t>by_minute TEXT</t>
+  </si>
+  <si>
+    <t>by_hour  TEXT</t>
+  </si>
+  <si>
+    <t>by_day TEXT</t>
+  </si>
+  <si>
+    <t>by_month_day TEXT</t>
+  </si>
+  <si>
+    <t>by_year_day TEXT</t>
+  </si>
+  <si>
+    <t>by_week_no TEXT</t>
+  </si>
+  <si>
+    <t>by_month TEXT</t>
+  </si>
+  <si>
+    <t>by_set_pos INT</t>
+  </si>
+  <si>
+    <t>name VARCHAR(64) NOT NULL</t>
+  </si>
+  <si>
+    <t>summary VARCHAR(256) NOT NULL</t>
+  </si>
+  <si>
+    <t>location VARCHAR(256)</t>
+  </si>
+  <si>
+    <t>Session</t>
+  </si>
+  <si>
+    <t>registrationController</t>
+  </si>
+  <si>
+    <t>Messages</t>
+  </si>
+  <si>
+    <t>Collaborators</t>
+  </si>
+  <si>
+    <t>registrationService</t>
+  </si>
+  <si>
+    <t>loginController</t>
+  </si>
+  <si>
+    <t>loginService</t>
+  </si>
+  <si>
+    <t>logoutController</t>
+  </si>
+  <si>
+    <t>logoutService</t>
+  </si>
+  <si>
+    <t>database</t>
+  </si>
+  <si>
+    <t>query</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>deleteEntry</t>
+  </si>
+  <si>
+    <t>createEntry</t>
+  </si>
+  <si>
+    <t>checkLogin</t>
+  </si>
+  <si>
+    <t>viewEntry</t>
+  </si>
+  <si>
+    <t>updateEntry</t>
+  </si>
+  <si>
+    <t>authenticateLogin</t>
+  </si>
+  <si>
+    <t>deleteSession</t>
+  </si>
+  <si>
+    <t>createSession</t>
+  </si>
+  <si>
+    <t>database
+createSession</t>
+  </si>
+  <si>
+    <t>database
+deleteSession</t>
+  </si>
+  <si>
+    <t>createEntry
+deleteEntry
+authenticateLogin</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>register</t>
   </si>
 </sst>
 </file>
@@ -1399,7 +1516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1449,9 +1566,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
@@ -1496,11 +1610,199 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="115">
+  <dxfs count="119">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1515,15 +1817,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1662,95 +1955,24 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1848,63 +2070,6 @@
     </dxf>
     <dxf>
       <alignment vertical="top" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2140,38 +2305,38 @@
   </dxfs>
   <tableStyles count="5" defaultTableStyle="Senior Project" defaultPivotStyle="PivotTable Style 1">
     <tableStyle name="PivotTable Style 1" table="0" count="6">
-      <tableStyleElement type="wholeTable" dxfId="114"/>
-      <tableStyleElement type="headerRow" dxfId="113"/>
-      <tableStyleElement type="firstRowStripe" dxfId="112"/>
-      <tableStyleElement type="secondRowStripe" dxfId="111"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="110"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="109"/>
+      <tableStyleElement type="wholeTable" dxfId="118"/>
+      <tableStyleElement type="headerRow" dxfId="117"/>
+      <tableStyleElement type="firstRowStripe" dxfId="116"/>
+      <tableStyleElement type="secondRowStripe" dxfId="115"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="114"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="113"/>
     </tableStyle>
     <tableStyle name="Senior Project" pivot="0" count="4">
+      <tableStyleElement type="wholeTable" dxfId="112"/>
+      <tableStyleElement type="headerRow" dxfId="111"/>
+      <tableStyleElement type="firstRowStripe" dxfId="110"/>
+      <tableStyleElement type="secondRowStripe" dxfId="109"/>
+    </tableStyle>
+    <tableStyle name="Senior Project: Red" pivot="0" count="4">
       <tableStyleElement type="wholeTable" dxfId="108"/>
       <tableStyleElement type="headerRow" dxfId="107"/>
       <tableStyleElement type="firstRowStripe" dxfId="106"/>
       <tableStyleElement type="secondRowStripe" dxfId="105"/>
     </tableStyle>
-    <tableStyle name="Senior Project: Red" pivot="0" count="4">
+    <tableStyle name="SlicerStyle1" pivot="0" table="0" count="10">
       <tableStyleElement type="wholeTable" dxfId="104"/>
       <tableStyleElement type="headerRow" dxfId="103"/>
-      <tableStyleElement type="firstRowStripe" dxfId="102"/>
-      <tableStyleElement type="secondRowStripe" dxfId="101"/>
-    </tableStyle>
-    <tableStyle name="SlicerStyle1" pivot="0" table="0" count="10">
-      <tableStyleElement type="wholeTable" dxfId="100"/>
-      <tableStyleElement type="headerRow" dxfId="99"/>
     </tableStyle>
     <tableStyle name="SlicerStyleDark1 2 2" pivot="0" table="0" count="10">
-      <tableStyleElement type="wholeTable" dxfId="98"/>
-      <tableStyleElement type="headerRow" dxfId="97"/>
+      <tableStyleElement type="wholeTable" dxfId="102"/>
+      <tableStyleElement type="headerRow" dxfId="101"/>
     </tableStyle>
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF76B64A"/>
       <color rgb="FFE03237"/>
-      <color rgb="FF76B64A"/>
       <color rgb="FFF5F5F5"/>
       <color rgb="FFFFFFFF"/>
       <color rgb="FF2685CC"/>
@@ -2847,19 +3012,19 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-      <mc:Choice Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Category 1"/>
@@ -2876,7 +3041,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2886,7 +3051,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5934075" y="190500"/>
+              <a:off x="6334125" y="190500"/>
               <a:ext cx="1457325" cy="2524125"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2919,19 +3084,19 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>523875</xdr:rowOff>
+      <xdr:rowOff>333375</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-      <mc:Choice Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Done 1"/>
@@ -2948,7 +3113,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2958,7 +3123,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7572376" y="190500"/>
+              <a:off x="7972426" y="190500"/>
               <a:ext cx="1314450" cy="904875"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2991,19 +3156,19 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>695325</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-      <mc:Choice Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="Look Into 1"/>
@@ -3020,7 +3185,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -3030,7 +3195,79 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7572376" y="1266825"/>
+              <a:off x="7972426" y="1143000"/>
+              <a:ext cx="1314450" cy="904875"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a table slicer. Table slicers are supported in Excel or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2007 or earlier, the slicer can't be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>333374</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Remember"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Remember"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7972425" y="2095499"/>
               <a:ext cx="1314450" cy="904875"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3380,7 +3617,7 @@
     <i/>
   </colItems>
   <formats count="33">
-    <format dxfId="90">
+    <format dxfId="100">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -3394,10 +3631,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="99">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="88">
+    <format dxfId="98">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -3407,6 +3644,109 @@
             <x v="3"/>
             <x v="4"/>
             <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="97">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="96">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="95">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="94">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="93">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="3">
+            <x v="3"/>
+            <x v="9"/>
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="92">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="2">
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="91">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="3" count="2">
+            <x v="1"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="90">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="3" count="5">
+            <x v="2"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="11"/>
+            <x v="13"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="89">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="3" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="88">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="3" count="1">
+            <x v="14"/>
           </reference>
         </references>
       </pivotArea>
@@ -3515,43 +3855,66 @@
       </pivotArea>
     </format>
     <format dxfId="77">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
     <format dxfId="76">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
     </format>
     <format dxfId="75">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
     </format>
     <format dxfId="74">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
-          <reference field="1" count="6">
-            <x v="0"/>
-            <x v="1"/>
+          <reference field="1" count="1">
             <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="73">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="72">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="71">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
             <x v="0"/>
           </reference>
-          <reference field="3" count="3">
-            <x v="3"/>
-            <x v="9"/>
+          <reference field="3" count="1">
             <x v="10"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="70">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3564,7 +3927,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="69">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3577,133 +3940,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="3" count="5">
-            <x v="2"/>
-            <x v="7"/>
-            <x v="8"/>
-            <x v="11"/>
-            <x v="13"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="69">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-          <reference field="3" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
     <format dxfId="68">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-          <reference field="3" count="1">
-            <x v="14"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="67">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
-    </format>
-    <format dxfId="66">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="65">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="64">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="63">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="62">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="61">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1">
-            <x v="10"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="60">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="3" count="2">
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="59">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="3" count="2">
-            <x v="1"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="58">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3811,6 +4048,16 @@
 </slicerCacheDefinition>
 </file>
 
+<file path=xl/slicerCaches/slicerCache7.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_Remember" sourceName="Remember">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="3" column="5"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <slicer name="Category" cache="Slicer_Category" caption="Category" rowHeight="241300"/>
@@ -3824,97 +4071,102 @@
   <slicer name="Category 1" cache="Slicer_Category1" caption="Category" rowHeight="241300"/>
   <slicer name="Done 1" cache="Slicer_Done1" caption="Done" rowHeight="241300"/>
   <slicer name="Look Into 1" cache="Slicer_Look_Into1" caption="Look Into" rowHeight="241300"/>
+  <slicer name="Remember" cache="Slicer_Remember" caption="Remember" rowHeight="241300"/>
 </slicers>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:E25" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
-  <autoFilter ref="B2:E25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F25" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+  <autoFilter ref="B2:F25">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
-  <sortState ref="B3:E25">
-    <sortCondition ref="C1:C24"/>
+  <sortState ref="B4:F25">
+    <sortCondition ref="C2:C25"/>
   </sortState>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Done" dataDxfId="48"/>
-    <tableColumn id="3" name="Category" dataDxfId="47"/>
-    <tableColumn id="4" name="Look Into" dataDxfId="46"/>
-    <tableColumn id="2" name="Task" dataDxfId="45"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Done" dataDxfId="65"/>
+    <tableColumn id="3" name="Category" dataDxfId="64"/>
+    <tableColumn id="5" name="Remember" dataDxfId="22"/>
+    <tableColumn id="4" name="Look Into" dataDxfId="63"/>
+    <tableColumn id="2" name="Task" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Remember_List" displayName="Remember_List" ref="K2:K25" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
-  <autoFilter ref="K2:K25"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="REMEMBER!!" dataDxfId="42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+  <autoFilter ref="A1:Q15"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="Name" dataDxfId="59"/>
+    <tableColumn id="2" name="Foreign Key1" dataDxfId="58"/>
+    <tableColumn id="3" name="Foreign Key2" dataDxfId="57"/>
+    <tableColumn id="4" name="Column1" dataDxfId="56"/>
+    <tableColumn id="5" name="Column2" dataDxfId="55"/>
+    <tableColumn id="6" name="Column3" dataDxfId="54"/>
+    <tableColumn id="7" name="Column4" dataDxfId="53"/>
+    <tableColumn id="8" name="Column5" dataDxfId="52"/>
+    <tableColumn id="9" name="Column6" dataDxfId="51"/>
+    <tableColumn id="13" name="Column7" dataDxfId="50"/>
+    <tableColumn id="12" name="Column8" dataDxfId="49"/>
+    <tableColumn id="11" name="Column9" dataDxfId="48"/>
+    <tableColumn id="17" name="Column10" dataDxfId="47"/>
+    <tableColumn id="16" name="Column11" dataDxfId="46"/>
+    <tableColumn id="15" name="Column12" dataDxfId="45"/>
+    <tableColumn id="14" name="Column13" dataDxfId="44"/>
+    <tableColumn id="10" name="Column14" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q17" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
-  <autoFilter ref="A1:Q17"/>
-  <tableColumns count="17">
-    <tableColumn id="1" name="Name" dataDxfId="39"/>
-    <tableColumn id="2" name="Foreign Key1" dataDxfId="38"/>
-    <tableColumn id="3" name="Foreign Key2" dataDxfId="37"/>
-    <tableColumn id="4" name="Column1" dataDxfId="36"/>
-    <tableColumn id="5" name="Column2" dataDxfId="35"/>
-    <tableColumn id="6" name="Column3" dataDxfId="34"/>
-    <tableColumn id="7" name="Column4" dataDxfId="33"/>
-    <tableColumn id="8" name="Column5" dataDxfId="32"/>
-    <tableColumn id="9" name="Column6" dataDxfId="31"/>
-    <tableColumn id="13" name="Column7" dataDxfId="30"/>
-    <tableColumn id="12" name="Column8" dataDxfId="29"/>
-    <tableColumn id="11" name="Column9" dataDxfId="28"/>
-    <tableColumn id="17" name="Column10" dataDxfId="27"/>
-    <tableColumn id="16" name="Column11" dataDxfId="26"/>
-    <tableColumn id="15" name="Column12" dataDxfId="25"/>
-    <tableColumn id="14" name="Column13" dataDxfId="24"/>
-    <tableColumn id="10" name="Column14" dataDxfId="23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+  <autoFilter ref="A2:L108"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="Notes: Client" dataDxfId="40"/>
+    <tableColumn id="2" name="A:C" dataDxfId="39"/>
+    <tableColumn id="3" name="U" dataDxfId="38"/>
+    <tableColumn id="4" name="S" dataDxfId="37"/>
+    <tableColumn id="5" name="Use Case: Client" dataDxfId="36"/>
+    <tableColumn id="6" name="Conversation" dataDxfId="35"/>
+    <tableColumn id="8" name="Use Case: Server" dataDxfId="34"/>
+    <tableColumn id="13" name="G" dataDxfId="33"/>
+    <tableColumn id="9" name="A:S" dataDxfId="32"/>
+    <tableColumn id="10" name="D" dataDxfId="31"/>
+    <tableColumn id="11" name="C" dataDxfId="30"/>
+    <tableColumn id="12" name="Notes: Server" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="A2:L108"/>
-  <tableColumns count="12">
-    <tableColumn id="1" name="Notes: Client" dataDxfId="20"/>
-    <tableColumn id="2" name="A:C" dataDxfId="19"/>
-    <tableColumn id="3" name="U" dataDxfId="18"/>
-    <tableColumn id="4" name="S" dataDxfId="17"/>
-    <tableColumn id="5" name="Use Case: Client" dataDxfId="16"/>
-    <tableColumn id="6" name="Conversation" dataDxfId="15"/>
-    <tableColumn id="8" name="Use Case: Server" dataDxfId="14"/>
-    <tableColumn id="13" name="G" dataDxfId="13"/>
-    <tableColumn id="9" name="A:S" dataDxfId="12"/>
-    <tableColumn id="10" name="D" dataDxfId="11"/>
-    <tableColumn id="11" name="C" dataDxfId="10"/>
-    <tableColumn id="12" name="Notes: Server" dataDxfId="9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="17" dataDxfId="20">
+  <autoFilter ref="A1:D21"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Type" dataDxfId="15"/>
+    <tableColumn id="6" name="Name" dataDxfId="13"/>
+    <tableColumn id="2" name="Messages" dataDxfId="14"/>
+    <tableColumn id="3" name="Collaborators" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G23" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="16" dataDxfId="28">
+  <autoFilter ref="A1:G25"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Name" dataDxfId="6"/>
-    <tableColumn id="7" name="Dependencies" dataDxfId="5"/>
-    <tableColumn id="6" name="Route" dataDxfId="4"/>
-    <tableColumn id="2" name="Controller" dataDxfId="3"/>
-    <tableColumn id="4" name="Directive" dataDxfId="2"/>
-    <tableColumn id="3" name="Factory" dataDxfId="1"/>
-    <tableColumn id="5" name="Service" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="18"/>
+    <tableColumn id="7" name="Dependencies" dataDxfId="19"/>
+    <tableColumn id="6" name="Route" dataDxfId="27"/>
+    <tableColumn id="2" name="Controller" dataDxfId="26"/>
+    <tableColumn id="4" name="Directive" dataDxfId="25"/>
+    <tableColumn id="3" name="Factory" dataDxfId="24"/>
+    <tableColumn id="5" name="Service" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project: Red" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4186,7 +4438,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -4202,396 +4454,396 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="23">
         <v>17</v>
       </c>
-      <c r="D2" s="24"/>
+      <c r="D2" s="23"/>
       <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="25">
         <v>5</v>
       </c>
-      <c r="D3" s="26" t="s">
-        <v>65</v>
+      <c r="D3" s="25" t="s">
+        <v>64</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="25">
         <v>2</v>
       </c>
-      <c r="D4" s="26"/>
+      <c r="D4" s="25"/>
       <c r="F4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="25">
         <v>5</v>
       </c>
-      <c r="D5" s="26"/>
+      <c r="D5" s="25"/>
       <c r="F5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="25">
         <v>5</v>
       </c>
-      <c r="D6" s="26"/>
+      <c r="D6" s="25"/>
       <c r="F6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="27">
         <v>15</v>
       </c>
-      <c r="D7" s="28"/>
+      <c r="D7" s="27"/>
       <c r="F7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="25">
         <v>5</v>
       </c>
-      <c r="D8" s="26"/>
+      <c r="D8" s="25"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="25">
         <v>2</v>
       </c>
-      <c r="D9" s="26"/>
+      <c r="D9" s="25"/>
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="25">
         <v>5</v>
       </c>
-      <c r="D10" s="26"/>
+      <c r="D10" s="25"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="25">
         <v>3</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="F11" s="29" t="s">
+      <c r="D11" s="25"/>
+      <c r="F11" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="I11" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="J11" s="24" t="s">
+      <c r="J11" s="23" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12" s="27">
         <v>6</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="F12" s="30" t="s">
+      <c r="D12" s="27"/>
+      <c r="F12" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="26">
+      <c r="G12" s="25">
         <v>84</v>
       </c>
-      <c r="H12" s="26">
+      <c r="H12" s="25">
         <v>74</v>
       </c>
-      <c r="I12" s="26">
-        <v>64</v>
-      </c>
-      <c r="J12" s="26" t="s">
+      <c r="I12" s="25">
+        <v>64</v>
+      </c>
+      <c r="J12" s="25" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="25">
         <v>1</v>
       </c>
-      <c r="D13" s="26"/>
+      <c r="D13" s="25"/>
     </row>
     <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="25">
         <v>1</v>
       </c>
-      <c r="D14" s="26"/>
+      <c r="D14" s="25"/>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="25">
         <v>4</v>
       </c>
-      <c r="D15" s="26"/>
+      <c r="D15" s="25"/>
     </row>
     <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="28">
+      <c r="C16" s="27">
         <v>24</v>
       </c>
-      <c r="D16" s="28"/>
+      <c r="D16" s="27"/>
     </row>
     <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="25">
         <v>5</v>
       </c>
-      <c r="D17" s="26"/>
+      <c r="D17" s="25"/>
     </row>
     <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="25">
         <v>1</v>
       </c>
-      <c r="D18" s="26"/>
+      <c r="D18" s="25"/>
     </row>
     <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="25">
         <v>1</v>
       </c>
-      <c r="D19" s="26"/>
+      <c r="D19" s="25"/>
     </row>
     <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="25">
         <v>1</v>
       </c>
-      <c r="D20" s="26"/>
+      <c r="D20" s="25"/>
     </row>
     <row r="21" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="25">
         <v>1</v>
       </c>
-      <c r="D21" s="26"/>
+      <c r="D21" s="25"/>
     </row>
     <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="25">
         <v>5</v>
       </c>
-      <c r="D22" s="26"/>
+      <c r="D22" s="25"/>
     </row>
     <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="25">
         <v>5</v>
       </c>
-      <c r="D23" s="26"/>
+      <c r="D23" s="25"/>
     </row>
     <row r="24" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="26">
+      <c r="C24" s="25">
         <v>5</v>
       </c>
-      <c r="D24" s="26"/>
+      <c r="D24" s="25"/>
     </row>
     <row r="25" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="28">
+      <c r="C25" s="27">
         <v>18</v>
       </c>
-      <c r="D25" s="28"/>
+      <c r="D25" s="27"/>
     </row>
     <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="26">
+      <c r="C26" s="25">
         <v>5</v>
       </c>
-      <c r="D26" s="26"/>
+      <c r="D26" s="25"/>
     </row>
     <row r="27" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="25">
         <v>5</v>
       </c>
-      <c r="D27" s="26"/>
+      <c r="D27" s="25"/>
     </row>
     <row r="28" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="25">
         <v>5</v>
       </c>
-      <c r="D28" s="26"/>
+      <c r="D28" s="25"/>
     </row>
     <row r="29" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="25">
         <v>1</v>
       </c>
-      <c r="D29" s="26"/>
+      <c r="D29" s="25"/>
     </row>
     <row r="30" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C30" s="26">
+      <c r="C30" s="25">
         <v>2</v>
       </c>
-      <c r="D30" s="26"/>
+      <c r="D30" s="25"/>
     </row>
     <row r="31" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="28">
+      <c r="C31" s="27">
         <v>8</v>
       </c>
-      <c r="D31" s="28"/>
+      <c r="D31" s="27"/>
     </row>
     <row r="32" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="26">
+      <c r="C32" s="25">
         <v>5</v>
       </c>
-      <c r="D32" s="26"/>
+      <c r="D32" s="25"/>
     </row>
     <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="26">
+      <c r="C33" s="25">
         <v>3</v>
       </c>
-      <c r="D33" s="26"/>
+      <c r="D33" s="25"/>
     </row>
     <row r="34" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="28">
+      <c r="C34" s="27">
         <v>17</v>
       </c>
-      <c r="D34" s="28"/>
+      <c r="D34" s="27"/>
     </row>
     <row r="35" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="26">
+      <c r="C35" s="25">
         <v>4</v>
       </c>
-      <c r="D35" s="26"/>
+      <c r="D35" s="25"/>
     </row>
     <row r="36" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="25" t="s">
+      <c r="B36" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="26">
+      <c r="C36" s="25">
         <v>3</v>
       </c>
-      <c r="D36" s="26"/>
+      <c r="D36" s="25"/>
     </row>
     <row r="37" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="26">
+      <c r="C37" s="25">
         <v>5</v>
       </c>
-      <c r="D37" s="26"/>
+      <c r="D37" s="25"/>
     </row>
     <row r="38" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="26">
+      <c r="C38" s="25">
         <v>5</v>
       </c>
-      <c r="D38" s="26"/>
+      <c r="D38" s="25"/>
     </row>
     <row r="39" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="28">
+      <c r="C39" s="27">
         <v>105</v>
       </c>
-      <c r="D39" s="28"/>
+      <c r="D39" s="27"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
@@ -4621,7 +4873,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="18" customWidth="1"/>
     <col min="3" max="3" width="100.5703125" style="13" customWidth="1"/>
     <col min="4" max="4" width="4.28515625" customWidth="1"/>
     <col min="5" max="6" width="7.28515625" customWidth="1"/>
@@ -4644,125 +4896,125 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="C2" s="21" t="s">
+      <c r="B2" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="C3" s="19"/>
+        <v>135</v>
+      </c>
+      <c r="C3" s="18"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="13"/>
-      <c r="C4" s="19" t="s">
-        <v>112</v>
+      <c r="C4" s="18" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
-      <c r="C5" s="19" t="s">
-        <v>161</v>
+      <c r="C5" s="18" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="13"/>
       <c r="C6" s="13" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="19"/>
+      <c r="C7" s="18"/>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="13" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
       <c r="C9" s="13" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="C10" s="19"/>
+        <v>138</v>
+      </c>
+      <c r="C10" s="18"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="13" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
       <c r="C12" s="13" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="19"/>
+      <c r="C13" s="18"/>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="13"/>
       <c r="C14" s="13" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="13" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
       <c r="C16" s="13" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="13"/>
-      <c r="C17" s="19" t="s">
-        <v>167</v>
+      <c r="C17" s="18" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="13"/>
       <c r="C18" s="13" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="C19" s="19"/>
+      <c r="B19" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" s="18"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="19" t="s">
-        <v>171</v>
+      <c r="C20" s="18" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="C21" s="19"/>
+        <v>154</v>
+      </c>
+      <c r="C21" s="18"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25"/>
@@ -4773,26 +5025,26 @@
       <c r="C26"/>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C28" s="22"/>
+      <c r="C28" s="21"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B25:C1048576 B1:C21">
-    <cfRule type="expression" dxfId="96" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>$B1="Setup"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$B1="CSS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="3">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>$B1="HTML"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="4">
+    <cfRule type="expression" dxfId="9" priority="4">
       <formula>$B1="JS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>$B1="DB"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="6">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>$B1="PHP"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4810,14 +5062,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="B2:K25"/>
+  <dimension ref="B2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4825,244 +5077,275 @@
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="6" style="15" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="59.140625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="2.85546875" customWidth="1"/>
-    <col min="11" max="11" width="49.5703125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="6" style="15" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="59.140625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>175</v>
+        <v>204</v>
       </c>
       <c r="E2" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="15" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="C5" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F6" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F7" s="16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C9" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C10" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="C11" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="E11" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C12" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C13" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C14" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F14" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C15" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="16"/>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="16"/>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E23" s="16"/>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="16"/>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E25" s="16"/>
+        <v>3</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C19" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C20" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C21" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="16"/>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="16"/>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="16"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="containsText" dxfId="57" priority="2" operator="containsText" text="CSS">
+  <conditionalFormatting sqref="C1:E1048576">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="CSS">
       <formula>NOT(ISERROR(SEARCH("CSS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="3" operator="containsText" text="HTML">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="HTML">
       <formula>NOT(ISERROR(SEARCH("HTML",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="4" operator="containsText" text="JS">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="JS">
       <formula>NOT(ISERROR(SEARCH("JS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="5" operator="containsText" text="DB">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="DB">
       <formula>NOT(ISERROR(SEARCH("DB",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="6" operator="containsText" text="PHP">
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="PHP">
       <formula>NOT(ISERROR(SEARCH("PHP",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="52" priority="1" operator="containsText" text="Setup">
+  <conditionalFormatting sqref="C1:D1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Setup">
       <formula>NOT(ISERROR(SEARCH("Setup",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E1048576">
-    <cfRule type="expression" dxfId="51" priority="9">
+  <conditionalFormatting sqref="B2:F1048576">
+    <cfRule type="expression" dxfId="0" priority="9">
       <formula>$B2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="2">
-    <tablePart r:id="rId3"/>
+  <legacyDrawing r:id="rId3"/>
+  <tableParts count="1">
     <tablePart r:id="rId4"/>
   </tableParts>
   <extLst>
@@ -5080,19 +5363,19 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
     <col min="7" max="7" width="29.7109375" customWidth="1"/>
     <col min="8" max="8" width="25.7109375" customWidth="1"/>
@@ -5107,115 +5390,115 @@
         <v>54</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>100</v>
-      </c>
       <c r="K1" s="11" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="Q1" s="11" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>108</v>
+        <v>211</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>125</v>
+        <v>212</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>73</v>
+        <v>213</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>208</v>
+        <v>183</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
     </row>
-    <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>129</v>
+        <v>157</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>88</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>109</v>
+        <v>158</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>113</v>
+        <v>159</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -5230,34 +5513,16 @@
       <c r="Q3" s="12"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>91</v>
-      </c>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="12"/>
-      <c r="D4" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>56</v>
-      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
@@ -5266,21 +5531,23 @@
       <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
     </row>
-    <row r="5" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="F5" s="12"/>
+        <v>223</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>106</v>
+      </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -5293,35 +5560,35 @@
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
     </row>
-    <row r="6" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" s="12"/>
+        <v>89</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>209</v>
+      </c>
       <c r="D6" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>158</v>
+        <v>224</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>111</v>
+        <v>55</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>58</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
@@ -5332,21 +5599,19 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>111</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
@@ -5360,14 +5625,30 @@
       <c r="Q7" s="12"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
+      <c r="A8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
@@ -5380,18 +5661,20 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="B9" s="13"/>
+        <v>110</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>183</v>
+        <v>224</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>184</v>
+        <v>104</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
@@ -5407,7 +5690,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
@@ -5424,104 +5707,96 @@
       <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
     </row>
-    <row r="11" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>134</v>
-      </c>
       <c r="I11" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="M11" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="N11" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="O11" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="P11" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q11" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+    </row>
+    <row r="12" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>101</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
+        <v>130</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="P12" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q12" s="12" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>110</v>
-      </c>
+      <c r="A13" s="13"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
@@ -5536,20 +5811,20 @@
       <c r="Q13" s="12"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>121</v>
+      <c r="A14" s="12" t="s">
+        <v>112</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -5565,11 +5840,21 @@
       <c r="Q14" s="12"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
+      <c r="A15" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>114</v>
+      </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
@@ -5583,84 +5868,26 @@
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>152</v>
-      </c>
-      <c r="B22" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
+        <v>131</v>
+      </c>
+      <c r="B20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5696,50 +5923,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
+      <c r="A1" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
       <c r="F1" s="10"/>
-      <c r="G1" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
+      <c r="G1" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>47</v>
@@ -5748,177 +5975,177 @@
         <v>46</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>198</v>
+        <v>173</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="210" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:12" ht="210" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>196</v>
+        <v>171</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>10</v>
@@ -5926,136 +6153,136 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>195</v>
+        <v>170</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L12" s="7"/>
     </row>
@@ -6066,108 +6293,108 @@
       <c r="D13" s="9"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>199</v>
+        <v>174</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>199</v>
+        <v>174</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>202</v>
+        <v>177</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>202</v>
+        <v>177</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L16" s="7"/>
     </row>
@@ -6179,43 +6406,43 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7" t="s">
-        <v>203</v>
+        <v>178</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L18" s="7"/>
     </row>
@@ -7494,14 +7721,217 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6" style="38" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="36" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="33" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="33" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="33"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>236</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>244</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>245</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFE03237"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7515,238 +7945,272 @@
     <col min="10" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>217</v>
+      <c r="B1" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>222</v>
+      <c r="A2" s="34" t="s">
+        <v>197</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
+        <v>60</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31" t="s">
-        <v>220</v>
-      </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
+      <c r="A3" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" s="31"/>
+      <c r="A4" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="30"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
+      <c r="A5" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>213</v>
-      </c>
       <c r="B8" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
+        <v>60</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="34" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="B11" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
+      <c r="D12" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
+      <c r="A13" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
+      <c r="A14" s="34"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
+      <c r="A15" s="34"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-    </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-    </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-    </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-    </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-    </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
+      <c r="A16" s="34"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="34"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="34"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed tables, began work on registration.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="255">
   <si>
     <t>Design</t>
   </si>
@@ -1334,6 +1334,15 @@
   </si>
   <si>
     <t>register</t>
+  </si>
+  <si>
+    <t>Set new &lt;base href=""&gt; as needed</t>
+  </si>
+  <si>
+    <t>Check that app.min.js is actually smaller than app.js</t>
+  </si>
+  <si>
+    <t>$routeProvider to $stateProvider</t>
   </si>
 </sst>
 </file>
@@ -1604,12 +1613,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1628,6 +1631,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1751,6 +1760,46 @@
           <bgColor rgb="FF76B64A"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1771,59 +1820,16 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1956,6 +1962,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3020,11 +3029,11 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Category 1"/>
@@ -3041,7 +3050,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -3092,11 +3101,11 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>333375</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Done 1"/>
@@ -3113,7 +3122,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -3158,17 +3167,17 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="Look Into 1"/>
@@ -3185,7 +3194,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -3230,17 +3239,17 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>333374</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="5" name="Remember"/>
@@ -3257,7 +3266,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -4076,97 +4085,97 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F25" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
-  <autoFilter ref="B2:F25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F30" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+  <autoFilter ref="B2:F30">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
-  <sortState ref="B4:F25">
-    <sortCondition ref="C2:C25"/>
+  <sortState ref="B6:F30">
+    <sortCondition ref="C2:C30"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" name="Done" dataDxfId="65"/>
     <tableColumn id="3" name="Category" dataDxfId="64"/>
-    <tableColumn id="5" name="Remember" dataDxfId="22"/>
-    <tableColumn id="4" name="Look Into" dataDxfId="63"/>
-    <tableColumn id="2" name="Task" dataDxfId="62"/>
+    <tableColumn id="5" name="Remember" dataDxfId="63"/>
+    <tableColumn id="4" name="Look Into" dataDxfId="62"/>
+    <tableColumn id="2" name="Task" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="A1:Q15"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Name" dataDxfId="59"/>
-    <tableColumn id="2" name="Foreign Key1" dataDxfId="58"/>
-    <tableColumn id="3" name="Foreign Key2" dataDxfId="57"/>
-    <tableColumn id="4" name="Column1" dataDxfId="56"/>
-    <tableColumn id="5" name="Column2" dataDxfId="55"/>
-    <tableColumn id="6" name="Column3" dataDxfId="54"/>
-    <tableColumn id="7" name="Column4" dataDxfId="53"/>
-    <tableColumn id="8" name="Column5" dataDxfId="52"/>
-    <tableColumn id="9" name="Column6" dataDxfId="51"/>
-    <tableColumn id="13" name="Column7" dataDxfId="50"/>
-    <tableColumn id="12" name="Column8" dataDxfId="49"/>
-    <tableColumn id="11" name="Column9" dataDxfId="48"/>
-    <tableColumn id="17" name="Column10" dataDxfId="47"/>
-    <tableColumn id="16" name="Column11" dataDxfId="46"/>
-    <tableColumn id="15" name="Column12" dataDxfId="45"/>
-    <tableColumn id="14" name="Column13" dataDxfId="44"/>
-    <tableColumn id="10" name="Column14" dataDxfId="43"/>
+    <tableColumn id="1" name="Name" dataDxfId="58"/>
+    <tableColumn id="2" name="Foreign Key1" dataDxfId="57"/>
+    <tableColumn id="3" name="Foreign Key2" dataDxfId="56"/>
+    <tableColumn id="4" name="Column1" dataDxfId="55"/>
+    <tableColumn id="5" name="Column2" dataDxfId="54"/>
+    <tableColumn id="6" name="Column3" dataDxfId="53"/>
+    <tableColumn id="7" name="Column4" dataDxfId="52"/>
+    <tableColumn id="8" name="Column5" dataDxfId="51"/>
+    <tableColumn id="9" name="Column6" dataDxfId="50"/>
+    <tableColumn id="13" name="Column7" dataDxfId="49"/>
+    <tableColumn id="12" name="Column8" dataDxfId="48"/>
+    <tableColumn id="11" name="Column9" dataDxfId="47"/>
+    <tableColumn id="17" name="Column10" dataDxfId="46"/>
+    <tableColumn id="16" name="Column11" dataDxfId="45"/>
+    <tableColumn id="15" name="Column12" dataDxfId="44"/>
+    <tableColumn id="14" name="Column13" dataDxfId="43"/>
+    <tableColumn id="10" name="Column14" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A2:L108"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Notes: Client" dataDxfId="40"/>
-    <tableColumn id="2" name="A:C" dataDxfId="39"/>
-    <tableColumn id="3" name="U" dataDxfId="38"/>
-    <tableColumn id="4" name="S" dataDxfId="37"/>
-    <tableColumn id="5" name="Use Case: Client" dataDxfId="36"/>
-    <tableColumn id="6" name="Conversation" dataDxfId="35"/>
-    <tableColumn id="8" name="Use Case: Server" dataDxfId="34"/>
-    <tableColumn id="13" name="G" dataDxfId="33"/>
-    <tableColumn id="9" name="A:S" dataDxfId="32"/>
-    <tableColumn id="10" name="D" dataDxfId="31"/>
-    <tableColumn id="11" name="C" dataDxfId="30"/>
-    <tableColumn id="12" name="Notes: Server" dataDxfId="29"/>
+    <tableColumn id="1" name="Notes: Client" dataDxfId="39"/>
+    <tableColumn id="2" name="A:C" dataDxfId="38"/>
+    <tableColumn id="3" name="U" dataDxfId="37"/>
+    <tableColumn id="4" name="S" dataDxfId="36"/>
+    <tableColumn id="5" name="Use Case: Client" dataDxfId="35"/>
+    <tableColumn id="6" name="Conversation" dataDxfId="34"/>
+    <tableColumn id="8" name="Use Case: Server" dataDxfId="33"/>
+    <tableColumn id="13" name="G" dataDxfId="32"/>
+    <tableColumn id="9" name="A:S" dataDxfId="31"/>
+    <tableColumn id="10" name="D" dataDxfId="30"/>
+    <tableColumn id="11" name="C" dataDxfId="29"/>
+    <tableColumn id="12" name="Notes: Server" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="17" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A1:D21"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Type" dataDxfId="15"/>
-    <tableColumn id="6" name="Name" dataDxfId="13"/>
-    <tableColumn id="2" name="Messages" dataDxfId="14"/>
-    <tableColumn id="3" name="Collaborators" dataDxfId="21"/>
+    <tableColumn id="1" name="Type" dataDxfId="25"/>
+    <tableColumn id="6" name="Name" dataDxfId="24"/>
+    <tableColumn id="2" name="Messages" dataDxfId="23"/>
+    <tableColumn id="3" name="Collaborators" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="16" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:G25"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Name" dataDxfId="18"/>
-    <tableColumn id="7" name="Dependencies" dataDxfId="19"/>
-    <tableColumn id="6" name="Route" dataDxfId="27"/>
-    <tableColumn id="2" name="Controller" dataDxfId="26"/>
-    <tableColumn id="4" name="Directive" dataDxfId="25"/>
-    <tableColumn id="3" name="Factory" dataDxfId="24"/>
-    <tableColumn id="5" name="Service" dataDxfId="23"/>
+    <tableColumn id="1" name="Name" dataDxfId="19"/>
+    <tableColumn id="7" name="Dependencies" dataDxfId="18"/>
+    <tableColumn id="6" name="Route" dataDxfId="17"/>
+    <tableColumn id="2" name="Controller" dataDxfId="16"/>
+    <tableColumn id="4" name="Directive" dataDxfId="15"/>
+    <tableColumn id="3" name="Factory" dataDxfId="14"/>
+    <tableColumn id="5" name="Service" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project: Red" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5066,10 +5075,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="B2:F25"/>
+  <dimension ref="B2:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5115,7 +5124,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="C4" s="15" t="s">
         <v>135</v>
       </c>
@@ -5169,10 +5181,13 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C9" s="15" t="s">
-        <v>138</v>
+        <v>2</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>205</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>143</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -5180,7 +5195,7 @@
         <v>138</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5201,35 +5216,38 @@
       <c r="C12" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>64</v>
-      </c>
       <c r="F12" s="16" t="s">
-        <v>198</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C13" s="15" t="s">
-        <v>3</v>
+        <v>138</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>64</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>137</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C14" s="15" t="s">
-        <v>3</v>
+        <v>138</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>205</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>149</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C15" s="15" t="s">
-        <v>3</v>
+        <v>138</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>150</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5243,74 +5261,107 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C17" s="15" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C18" s="15" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="C19" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>205</v>
-      </c>
       <c r="F19" s="16" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" ht="60" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="C20" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="15" t="s">
-        <v>205</v>
-      </c>
       <c r="F20" s="16" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C21" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="F21" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F22" s="16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="F24" s="16" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="16" t="s">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="16" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="16"/>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="F24" s="16"/>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="F25" s="16"/>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="16"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="16"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="16"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="16"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="16"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -5907,7 +5958,7 @@
   <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5923,22 +5974,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
       <c r="F1" s="10"/>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -7727,104 +7778,104 @@
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" style="38" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="36" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="33" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="33" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="33"/>
+    <col min="1" max="1" width="6" style="36" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="34" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="31" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="31" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="36" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="33" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="31" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="31" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="31" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="31" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="34" t="s">
         <v>233</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="31" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="34" t="s">
         <v>234</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="31" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="34" t="s">
         <v>239</v>
       </c>
       <c r="D8" s="12" t="s">
@@ -7832,10 +7883,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="34" t="s">
         <v>238</v>
       </c>
       <c r="D9" s="12" t="s">
@@ -7843,35 +7894,35 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="34" t="s">
         <v>241</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="31" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="34" t="s">
         <v>242</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="31" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="31" t="s">
         <v>236</v>
       </c>
       <c r="D12" s="12" t="s">
@@ -7879,13 +7930,13 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="31" t="s">
         <v>240</v>
       </c>
       <c r="D13" s="12" t="s">
@@ -7893,24 +7944,24 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="34" t="s">
         <v>244</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="31" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="34" t="s">
         <v>245</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="31" t="s">
         <v>239</v>
       </c>
     </row>
@@ -7969,7 +8020,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="32" t="s">
         <v>197</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -7983,7 +8034,7 @@
       <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="32" t="s">
         <v>186</v>
       </c>
       <c r="D3" s="30"/>
@@ -7994,7 +8045,7 @@
       <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="32" t="s">
         <v>60</v>
       </c>
       <c r="D4" s="30"/>
@@ -8005,7 +8056,7 @@
       <c r="G4" s="30"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="32" t="s">
         <v>226</v>
       </c>
       <c r="D5" s="30"/>
@@ -8016,7 +8067,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="32" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="30"/>
@@ -8027,7 +8078,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="32" t="s">
         <v>187</v>
       </c>
       <c r="B7" s="12" t="s">
@@ -8043,7 +8094,7 @@
       <c r="G7" s="30"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="32" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -8059,7 +8110,7 @@
       <c r="G8" s="30"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="32" t="s">
         <v>196</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -8075,7 +8126,7 @@
       <c r="G9" s="30"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="32" t="s">
         <v>188</v>
       </c>
       <c r="B10" s="12" t="s">
@@ -8091,7 +8142,7 @@
       <c r="G10" s="30"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="32" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="12" t="s">
@@ -8107,7 +8158,7 @@
       <c r="G11" s="30"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="32" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="30" t="s">
@@ -8118,7 +8169,7 @@
       <c r="G12" s="30"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="32" t="s">
         <v>69</v>
       </c>
       <c r="D13" s="30" t="s">
@@ -8129,84 +8180,84 @@
       <c r="G13" s="30"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
+      <c r="A14" s="32"/>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
       <c r="G14" s="30"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
+      <c r="A15" s="32"/>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
       <c r="F15" s="30"/>
       <c r="G15" s="30"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="A16" s="32"/>
       <c r="D16" s="30"/>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
+      <c r="A17" s="32"/>
       <c r="D17" s="30"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
+      <c r="A18" s="32"/>
       <c r="D18" s="30"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
+      <c r="A19" s="32"/>
       <c r="D19" s="30"/>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
+      <c r="A20" s="32"/>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
       <c r="G20" s="30"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
+      <c r="A21" s="32"/>
       <c r="D21" s="30"/>
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
       <c r="G21" s="30"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+      <c r="A22" s="32"/>
       <c r="D22" s="30"/>
       <c r="E22" s="30"/>
       <c r="F22" s="30"/>
       <c r="G22" s="30"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
+      <c r="A23" s="32"/>
       <c r="D23" s="30"/>
       <c r="E23" s="30"/>
       <c r="F23" s="30"/>
       <c r="G23" s="30"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
+      <c r="A24" s="32"/>
       <c r="D24" s="30"/>
       <c r="E24" s="30"/>
       <c r="F24" s="30"/>
       <c r="G24" s="30"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
+      <c r="A25" s="32"/>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>

</xml_diff>

<commit_message>
Finish non-async validation on registration form and renamed some css classes.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -1643,125 +1643,6 @@
   </cellStyles>
   <dxfs count="119">
     <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1982,6 +1863,68 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2079,6 +2022,63 @@
     </dxf>
     <dxf>
       <alignment vertical="top" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3626,46 +3626,6 @@
     <i/>
   </colItems>
   <formats count="33">
-    <format dxfId="100">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="99">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="98">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="97">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="96">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="95">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
-    </format>
     <format dxfId="94">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
@@ -3681,6 +3641,46 @@
       </pivotArea>
     </format>
     <format dxfId="93">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="92">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="91">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="90">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="89">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="88">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="87">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3694,7 +3694,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3707,7 +3707,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="85">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3720,7 +3720,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3736,7 +3736,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="83">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3748,7 +3748,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3760,16 +3760,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="81">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="86">
+    <format dxfId="80">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="85">
+    <format dxfId="79">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="84">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -3783,7 +3783,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="77">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3797,7 +3797,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="76">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3810,7 +3810,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="75">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3823,7 +3823,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="74">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3839,7 +3839,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="73">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3851,7 +3851,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="72">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3863,10 +3863,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="71">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="76">
+    <format dxfId="70">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3875,7 +3875,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="69">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3884,7 +3884,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="68">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3893,7 +3893,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="67">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3902,7 +3902,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="66">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3911,7 +3911,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="65">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3923,7 +3923,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="64">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3936,7 +3936,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="63">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3949,7 +3949,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="62">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4085,7 +4085,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F30" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F30" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <autoFilter ref="B2:F30">
     <filterColumn colId="0">
       <filters blank="1"/>
@@ -4095,87 +4095,87 @@
     <sortCondition ref="C2:C30"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Done" dataDxfId="65"/>
-    <tableColumn id="3" name="Category" dataDxfId="64"/>
-    <tableColumn id="5" name="Remember" dataDxfId="63"/>
-    <tableColumn id="4" name="Look Into" dataDxfId="62"/>
-    <tableColumn id="2" name="Task" dataDxfId="61"/>
+    <tableColumn id="1" name="Done" dataDxfId="52"/>
+    <tableColumn id="3" name="Category" dataDxfId="51"/>
+    <tableColumn id="5" name="Remember" dataDxfId="50"/>
+    <tableColumn id="4" name="Look Into" dataDxfId="49"/>
+    <tableColumn id="2" name="Task" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A1:Q15"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Name" dataDxfId="58"/>
-    <tableColumn id="2" name="Foreign Key1" dataDxfId="57"/>
-    <tableColumn id="3" name="Foreign Key2" dataDxfId="56"/>
-    <tableColumn id="4" name="Column1" dataDxfId="55"/>
-    <tableColumn id="5" name="Column2" dataDxfId="54"/>
-    <tableColumn id="6" name="Column3" dataDxfId="53"/>
-    <tableColumn id="7" name="Column4" dataDxfId="52"/>
-    <tableColumn id="8" name="Column5" dataDxfId="51"/>
-    <tableColumn id="9" name="Column6" dataDxfId="50"/>
-    <tableColumn id="13" name="Column7" dataDxfId="49"/>
-    <tableColumn id="12" name="Column8" dataDxfId="48"/>
-    <tableColumn id="11" name="Column9" dataDxfId="47"/>
-    <tableColumn id="17" name="Column10" dataDxfId="46"/>
-    <tableColumn id="16" name="Column11" dataDxfId="45"/>
-    <tableColumn id="15" name="Column12" dataDxfId="44"/>
-    <tableColumn id="14" name="Column13" dataDxfId="43"/>
-    <tableColumn id="10" name="Column14" dataDxfId="42"/>
+    <tableColumn id="1" name="Name" dataDxfId="45"/>
+    <tableColumn id="2" name="Foreign Key1" dataDxfId="44"/>
+    <tableColumn id="3" name="Foreign Key2" dataDxfId="43"/>
+    <tableColumn id="4" name="Column1" dataDxfId="42"/>
+    <tableColumn id="5" name="Column2" dataDxfId="41"/>
+    <tableColumn id="6" name="Column3" dataDxfId="40"/>
+    <tableColumn id="7" name="Column4" dataDxfId="39"/>
+    <tableColumn id="8" name="Column5" dataDxfId="38"/>
+    <tableColumn id="9" name="Column6" dataDxfId="37"/>
+    <tableColumn id="13" name="Column7" dataDxfId="36"/>
+    <tableColumn id="12" name="Column8" dataDxfId="35"/>
+    <tableColumn id="11" name="Column9" dataDxfId="34"/>
+    <tableColumn id="17" name="Column10" dataDxfId="33"/>
+    <tableColumn id="16" name="Column11" dataDxfId="32"/>
+    <tableColumn id="15" name="Column12" dataDxfId="31"/>
+    <tableColumn id="14" name="Column13" dataDxfId="30"/>
+    <tableColumn id="10" name="Column14" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A2:L108"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Notes: Client" dataDxfId="39"/>
-    <tableColumn id="2" name="A:C" dataDxfId="38"/>
-    <tableColumn id="3" name="U" dataDxfId="37"/>
-    <tableColumn id="4" name="S" dataDxfId="36"/>
-    <tableColumn id="5" name="Use Case: Client" dataDxfId="35"/>
-    <tableColumn id="6" name="Conversation" dataDxfId="34"/>
-    <tableColumn id="8" name="Use Case: Server" dataDxfId="33"/>
-    <tableColumn id="13" name="G" dataDxfId="32"/>
-    <tableColumn id="9" name="A:S" dataDxfId="31"/>
-    <tableColumn id="10" name="D" dataDxfId="30"/>
-    <tableColumn id="11" name="C" dataDxfId="29"/>
-    <tableColumn id="12" name="Notes: Server" dataDxfId="28"/>
+    <tableColumn id="1" name="Notes: Client" dataDxfId="26"/>
+    <tableColumn id="2" name="A:C" dataDxfId="25"/>
+    <tableColumn id="3" name="U" dataDxfId="24"/>
+    <tableColumn id="4" name="S" dataDxfId="23"/>
+    <tableColumn id="5" name="Use Case: Client" dataDxfId="22"/>
+    <tableColumn id="6" name="Conversation" dataDxfId="21"/>
+    <tableColumn id="8" name="Use Case: Server" dataDxfId="20"/>
+    <tableColumn id="13" name="G" dataDxfId="19"/>
+    <tableColumn id="9" name="A:S" dataDxfId="18"/>
+    <tableColumn id="10" name="D" dataDxfId="17"/>
+    <tableColumn id="11" name="C" dataDxfId="16"/>
+    <tableColumn id="12" name="Notes: Server" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:D21"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Type" dataDxfId="25"/>
-    <tableColumn id="6" name="Name" dataDxfId="24"/>
-    <tableColumn id="2" name="Messages" dataDxfId="23"/>
-    <tableColumn id="3" name="Collaborators" dataDxfId="22"/>
+    <tableColumn id="1" name="Type" dataDxfId="12"/>
+    <tableColumn id="6" name="Name" dataDxfId="11"/>
+    <tableColumn id="2" name="Messages" dataDxfId="10"/>
+    <tableColumn id="3" name="Collaborators" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G25"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Name" dataDxfId="19"/>
-    <tableColumn id="7" name="Dependencies" dataDxfId="18"/>
-    <tableColumn id="6" name="Route" dataDxfId="17"/>
-    <tableColumn id="2" name="Controller" dataDxfId="16"/>
-    <tableColumn id="4" name="Directive" dataDxfId="15"/>
-    <tableColumn id="3" name="Factory" dataDxfId="14"/>
-    <tableColumn id="5" name="Service" dataDxfId="13"/>
+    <tableColumn id="1" name="Name" dataDxfId="6"/>
+    <tableColumn id="7" name="Dependencies" dataDxfId="5"/>
+    <tableColumn id="6" name="Route" dataDxfId="4"/>
+    <tableColumn id="2" name="Controller" dataDxfId="3"/>
+    <tableColumn id="4" name="Directive" dataDxfId="2"/>
+    <tableColumn id="3" name="Factory" dataDxfId="1"/>
+    <tableColumn id="5" name="Service" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project: Red" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4447,7 +4447,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -5038,22 +5038,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B25:C1048576 B1:C21">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="100" priority="1">
       <formula>$B1="Setup"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="99" priority="2">
       <formula>$B1="CSS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="98" priority="3">
       <formula>$B1="HTML"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="97" priority="4">
       <formula>$B1="JS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="96" priority="5">
       <formula>$B1="DB"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="95" priority="6">
       <formula>$B1="PHP"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5366,29 +5366,29 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="C1:E1048576">
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="CSS">
+    <cfRule type="containsText" dxfId="61" priority="2" operator="containsText" text="CSS">
       <formula>NOT(ISERROR(SEARCH("CSS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="HTML">
+    <cfRule type="containsText" dxfId="60" priority="3" operator="containsText" text="HTML">
       <formula>NOT(ISERROR(SEARCH("HTML",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="JS">
+    <cfRule type="containsText" dxfId="59" priority="4" operator="containsText" text="JS">
       <formula>NOT(ISERROR(SEARCH("JS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="DB">
+    <cfRule type="containsText" dxfId="58" priority="5" operator="containsText" text="DB">
       <formula>NOT(ISERROR(SEARCH("DB",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="PHP">
+    <cfRule type="containsText" dxfId="57" priority="6" operator="containsText" text="PHP">
       <formula>NOT(ISERROR(SEARCH("PHP",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Setup">
+    <cfRule type="containsText" dxfId="56" priority="1" operator="containsText" text="Setup">
       <formula>NOT(ISERROR(SEARCH("Setup",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F1048576">
-    <cfRule type="expression" dxfId="0" priority="9">
+    <cfRule type="expression" dxfId="55" priority="9">
       <formula>$B2="x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added excel temporary files to git ignore list.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -31,7 +31,7 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -3511,7 +3511,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Task_List_Pivot" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" mergeItem="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Task_List_Pivot" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" mergeItem="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="B2:C21" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -5078,7 +5078,7 @@
   <dimension ref="B2:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Notes on optional features.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
     <sheet name="Reminders Pivot" sheetId="5" state="hidden" r:id="rId2"/>
     <sheet name="Reminders" sheetId="4" r:id="rId3"/>
-    <sheet name="Databases" sheetId="2" r:id="rId4"/>
-    <sheet name="Use Cases" sheetId="3" r:id="rId5"/>
-    <sheet name="Classes" sheetId="7" r:id="rId6"/>
-    <sheet name="AngularJS" sheetId="6" r:id="rId7"/>
+    <sheet name="Optional Features" sheetId="8" r:id="rId4"/>
+    <sheet name="Databases" sheetId="2" r:id="rId5"/>
+    <sheet name="Use Cases" sheetId="3" r:id="rId6"/>
+    <sheet name="Classes" sheetId="7" r:id="rId7"/>
+    <sheet name="AngularJS" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="Slicer_Category">#N/A</definedName>
@@ -31,14 +32,14 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
-        <x14:slicerCache r:id="rId9"/>
         <x14:slicerCache r:id="rId10"/>
         <x14:slicerCache r:id="rId11"/>
+        <x14:slicerCache r:id="rId12"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -46,10 +47,10 @@
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
       <x15:slicerCaches xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicerCache r:id="rId12"/>
         <x14:slicerCache r:id="rId13"/>
         <x14:slicerCache r:id="rId14"/>
         <x14:slicerCache r:id="rId15"/>
+        <x14:slicerCache r:id="rId16"/>
       </x15:slicerCaches>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -513,7 +514,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="261">
   <si>
     <t>Design</t>
   </si>
@@ -1342,7 +1343,25 @@
     <t>Check that app.min.js is actually smaller than app.js</t>
   </si>
   <si>
-    <t>$routeProvider to $stateProvider</t>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>register.service.js</t>
+  </si>
+  <si>
+    <t>ASyncValidator unique username check</t>
+  </si>
+  <si>
+    <t>register.html</t>
+  </si>
+  <si>
+    <t>Spin icon when waiting for http requests (unique username and registeration submit)</t>
+  </si>
+  <si>
+    <t>$routeProvider to $stateProvider?</t>
   </si>
 </sst>
 </file>
@@ -1641,7 +1660,22 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="119">
+  <dxfs count="124">
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2314,32 +2348,32 @@
   </dxfs>
   <tableStyles count="5" defaultTableStyle="Senior Project" defaultPivotStyle="PivotTable Style 1">
     <tableStyle name="PivotTable Style 1" table="0" count="6">
-      <tableStyleElement type="wholeTable" dxfId="118"/>
-      <tableStyleElement type="headerRow" dxfId="117"/>
-      <tableStyleElement type="firstRowStripe" dxfId="116"/>
-      <tableStyleElement type="secondRowStripe" dxfId="115"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="114"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="113"/>
+      <tableStyleElement type="wholeTable" dxfId="123"/>
+      <tableStyleElement type="headerRow" dxfId="122"/>
+      <tableStyleElement type="firstRowStripe" dxfId="121"/>
+      <tableStyleElement type="secondRowStripe" dxfId="120"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="119"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="118"/>
     </tableStyle>
     <tableStyle name="Senior Project" pivot="0" count="4">
-      <tableStyleElement type="wholeTable" dxfId="112"/>
-      <tableStyleElement type="headerRow" dxfId="111"/>
-      <tableStyleElement type="firstRowStripe" dxfId="110"/>
-      <tableStyleElement type="secondRowStripe" dxfId="109"/>
+      <tableStyleElement type="wholeTable" dxfId="117"/>
+      <tableStyleElement type="headerRow" dxfId="116"/>
+      <tableStyleElement type="firstRowStripe" dxfId="115"/>
+      <tableStyleElement type="secondRowStripe" dxfId="114"/>
     </tableStyle>
     <tableStyle name="Senior Project: Red" pivot="0" count="4">
-      <tableStyleElement type="wholeTable" dxfId="108"/>
-      <tableStyleElement type="headerRow" dxfId="107"/>
-      <tableStyleElement type="firstRowStripe" dxfId="106"/>
-      <tableStyleElement type="secondRowStripe" dxfId="105"/>
+      <tableStyleElement type="wholeTable" dxfId="113"/>
+      <tableStyleElement type="headerRow" dxfId="112"/>
+      <tableStyleElement type="firstRowStripe" dxfId="111"/>
+      <tableStyleElement type="secondRowStripe" dxfId="110"/>
     </tableStyle>
     <tableStyle name="SlicerStyle1" pivot="0" table="0" count="10">
-      <tableStyleElement type="wholeTable" dxfId="104"/>
-      <tableStyleElement type="headerRow" dxfId="103"/>
+      <tableStyleElement type="wholeTable" dxfId="109"/>
+      <tableStyleElement type="headerRow" dxfId="108"/>
     </tableStyle>
     <tableStyle name="SlicerStyleDark1 2 2" pivot="0" table="0" count="10">
-      <tableStyleElement type="wholeTable" dxfId="102"/>
-      <tableStyleElement type="headerRow" dxfId="101"/>
+      <tableStyleElement type="wholeTable" dxfId="107"/>
+      <tableStyleElement type="headerRow" dxfId="106"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3626,7 +3660,7 @@
     <i/>
   </colItems>
   <formats count="33">
-    <format dxfId="94">
+    <format dxfId="99">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -3640,10 +3674,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="93">
+    <format dxfId="98">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="92">
+    <format dxfId="97">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -3657,16 +3691,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="96">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="90">
+    <format dxfId="95">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="89">
+    <format dxfId="94">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="88">
+    <format dxfId="93">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -3680,7 +3714,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="92">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3694,7 +3728,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="91">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3707,7 +3741,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3720,7 +3754,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="84">
+    <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3736,7 +3770,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3748,7 +3782,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="87">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3760,16 +3794,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="86">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="80">
+    <format dxfId="85">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="79">
+    <format dxfId="84">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="78">
+    <format dxfId="83">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -3783,7 +3817,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3797,7 +3831,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="81">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3810,7 +3844,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="80">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3823,7 +3857,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="79">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3839,7 +3873,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3851,7 +3885,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="77">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3863,10 +3897,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="76">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="70">
+    <format dxfId="75">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3875,7 +3909,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="74">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3884,7 +3918,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="73">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3893,7 +3927,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="72">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3902,7 +3936,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="66">
+    <format dxfId="71">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3911,7 +3945,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
+    <format dxfId="70">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3923,7 +3957,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="64">
+    <format dxfId="69">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3936,7 +3970,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="63">
+    <format dxfId="68">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3949,7 +3983,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
+    <format dxfId="67">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4085,7 +4119,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F30" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F30" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="B2:F30">
     <filterColumn colId="0">
       <filters blank="1"/>
@@ -4095,87 +4129,99 @@
     <sortCondition ref="C2:C30"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Done" dataDxfId="52"/>
-    <tableColumn id="3" name="Category" dataDxfId="51"/>
-    <tableColumn id="5" name="Remember" dataDxfId="50"/>
-    <tableColumn id="4" name="Look Into" dataDxfId="49"/>
-    <tableColumn id="2" name="Task" dataDxfId="48"/>
+    <tableColumn id="1" name="Done" dataDxfId="57"/>
+    <tableColumn id="3" name="Category" dataDxfId="56"/>
+    <tableColumn id="5" name="Remember" dataDxfId="55"/>
+    <tableColumn id="4" name="Look Into" dataDxfId="54"/>
+    <tableColumn id="2" name="Task" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
-  <autoFilter ref="A1:Q15"/>
-  <tableColumns count="17">
-    <tableColumn id="1" name="Name" dataDxfId="45"/>
-    <tableColumn id="2" name="Foreign Key1" dataDxfId="44"/>
-    <tableColumn id="3" name="Foreign Key2" dataDxfId="43"/>
-    <tableColumn id="4" name="Column1" dataDxfId="42"/>
-    <tableColumn id="5" name="Column2" dataDxfId="41"/>
-    <tableColumn id="6" name="Column3" dataDxfId="40"/>
-    <tableColumn id="7" name="Column4" dataDxfId="39"/>
-    <tableColumn id="8" name="Column5" dataDxfId="38"/>
-    <tableColumn id="9" name="Column6" dataDxfId="37"/>
-    <tableColumn id="13" name="Column7" dataDxfId="36"/>
-    <tableColumn id="12" name="Column8" dataDxfId="35"/>
-    <tableColumn id="11" name="Column9" dataDxfId="34"/>
-    <tableColumn id="17" name="Column10" dataDxfId="33"/>
-    <tableColumn id="16" name="Column11" dataDxfId="32"/>
-    <tableColumn id="15" name="Column12" dataDxfId="31"/>
-    <tableColumn id="14" name="Column13" dataDxfId="30"/>
-    <tableColumn id="10" name="Column14" dataDxfId="29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:C30" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Done" dataDxfId="2"/>
+    <tableColumn id="2" name="File" dataDxfId="0"/>
+    <tableColumn id="3" name="Feature" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
-  <autoFilter ref="A2:L108"/>
-  <tableColumns count="12">
-    <tableColumn id="1" name="Notes: Client" dataDxfId="26"/>
-    <tableColumn id="2" name="A:C" dataDxfId="25"/>
-    <tableColumn id="3" name="U" dataDxfId="24"/>
-    <tableColumn id="4" name="S" dataDxfId="23"/>
-    <tableColumn id="5" name="Use Case: Client" dataDxfId="22"/>
-    <tableColumn id="6" name="Conversation" dataDxfId="21"/>
-    <tableColumn id="8" name="Use Case: Server" dataDxfId="20"/>
-    <tableColumn id="13" name="G" dataDxfId="19"/>
-    <tableColumn id="9" name="A:S" dataDxfId="18"/>
-    <tableColumn id="10" name="D" dataDxfId="17"/>
-    <tableColumn id="11" name="C" dataDxfId="16"/>
-    <tableColumn id="12" name="Notes: Server" dataDxfId="15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+  <autoFilter ref="A1:Q15"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="Name" dataDxfId="50"/>
+    <tableColumn id="2" name="Foreign Key1" dataDxfId="49"/>
+    <tableColumn id="3" name="Foreign Key2" dataDxfId="48"/>
+    <tableColumn id="4" name="Column1" dataDxfId="47"/>
+    <tableColumn id="5" name="Column2" dataDxfId="46"/>
+    <tableColumn id="6" name="Column3" dataDxfId="45"/>
+    <tableColumn id="7" name="Column4" dataDxfId="44"/>
+    <tableColumn id="8" name="Column5" dataDxfId="43"/>
+    <tableColumn id="9" name="Column6" dataDxfId="42"/>
+    <tableColumn id="13" name="Column7" dataDxfId="41"/>
+    <tableColumn id="12" name="Column8" dataDxfId="40"/>
+    <tableColumn id="11" name="Column9" dataDxfId="39"/>
+    <tableColumn id="17" name="Column10" dataDxfId="38"/>
+    <tableColumn id="16" name="Column11" dataDxfId="37"/>
+    <tableColumn id="15" name="Column12" dataDxfId="36"/>
+    <tableColumn id="14" name="Column13" dataDxfId="35"/>
+    <tableColumn id="10" name="Column14" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:D21"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Type" dataDxfId="12"/>
-    <tableColumn id="6" name="Name" dataDxfId="11"/>
-    <tableColumn id="2" name="Messages" dataDxfId="10"/>
-    <tableColumn id="3" name="Collaborators" dataDxfId="9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="A2:L108"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="Notes: Client" dataDxfId="31"/>
+    <tableColumn id="2" name="A:C" dataDxfId="30"/>
+    <tableColumn id="3" name="U" dataDxfId="29"/>
+    <tableColumn id="4" name="S" dataDxfId="28"/>
+    <tableColumn id="5" name="Use Case: Client" dataDxfId="27"/>
+    <tableColumn id="6" name="Conversation" dataDxfId="26"/>
+    <tableColumn id="8" name="Use Case: Server" dataDxfId="25"/>
+    <tableColumn id="13" name="G" dataDxfId="24"/>
+    <tableColumn id="9" name="A:S" dataDxfId="23"/>
+    <tableColumn id="10" name="D" dataDxfId="22"/>
+    <tableColumn id="11" name="C" dataDxfId="21"/>
+    <tableColumn id="12" name="Notes: Server" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:D21"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Type" dataDxfId="17"/>
+    <tableColumn id="6" name="Name" dataDxfId="16"/>
+    <tableColumn id="2" name="Messages" dataDxfId="15"/>
+    <tableColumn id="3" name="Collaborators" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:G25"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Name" dataDxfId="6"/>
-    <tableColumn id="7" name="Dependencies" dataDxfId="5"/>
-    <tableColumn id="6" name="Route" dataDxfId="4"/>
-    <tableColumn id="2" name="Controller" dataDxfId="3"/>
-    <tableColumn id="4" name="Directive" dataDxfId="2"/>
-    <tableColumn id="3" name="Factory" dataDxfId="1"/>
-    <tableColumn id="5" name="Service" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="11"/>
+    <tableColumn id="7" name="Dependencies" dataDxfId="10"/>
+    <tableColumn id="6" name="Route" dataDxfId="9"/>
+    <tableColumn id="2" name="Controller" dataDxfId="8"/>
+    <tableColumn id="4" name="Directive" dataDxfId="7"/>
+    <tableColumn id="3" name="Factory" dataDxfId="6"/>
+    <tableColumn id="5" name="Service" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project: Red" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5038,22 +5084,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B25:C1048576 B1:C21">
-    <cfRule type="expression" dxfId="100" priority="1">
+    <cfRule type="expression" dxfId="105" priority="1">
       <formula>$B1="Setup"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="2">
+    <cfRule type="expression" dxfId="104" priority="2">
       <formula>$B1="CSS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="3">
+    <cfRule type="expression" dxfId="103" priority="3">
       <formula>$B1="HTML"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="4">
+    <cfRule type="expression" dxfId="102" priority="4">
       <formula>$B1="JS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="5">
+    <cfRule type="expression" dxfId="101" priority="5">
       <formula>$B1="DB"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="6">
+    <cfRule type="expression" dxfId="100" priority="6">
       <formula>$B1="PHP"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5077,8 +5123,8 @@
   </sheetPr>
   <dimension ref="B2:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5246,8 +5292,11 @@
       <c r="C15" s="15" t="s">
         <v>138</v>
       </c>
+      <c r="E15" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="F15" s="16" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5288,7 +5337,10 @@
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="C20" s="15" t="s">
         <v>3</v>
       </c>
@@ -5304,7 +5356,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C22" s="15" t="s">
         <v>3</v>
       </c>
@@ -5315,7 +5367,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="C23" s="15" t="s">
         <v>3</v>
       </c>
@@ -5326,7 +5378,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C24" s="15" t="s">
         <v>3</v>
       </c>
@@ -5366,29 +5418,29 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="C1:E1048576">
-    <cfRule type="containsText" dxfId="61" priority="2" operator="containsText" text="CSS">
+    <cfRule type="containsText" dxfId="66" priority="2" operator="containsText" text="CSS">
       <formula>NOT(ISERROR(SEARCH("CSS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="3" operator="containsText" text="HTML">
+    <cfRule type="containsText" dxfId="65" priority="3" operator="containsText" text="HTML">
       <formula>NOT(ISERROR(SEARCH("HTML",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="4" operator="containsText" text="JS">
+    <cfRule type="containsText" dxfId="64" priority="4" operator="containsText" text="JS">
       <formula>NOT(ISERROR(SEARCH("JS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="5" operator="containsText" text="DB">
+    <cfRule type="containsText" dxfId="63" priority="5" operator="containsText" text="DB">
       <formula>NOT(ISERROR(SEARCH("DB",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="6" operator="containsText" text="PHP">
+    <cfRule type="containsText" dxfId="62" priority="6" operator="containsText" text="PHP">
       <formula>NOT(ISERROR(SEARCH("PHP",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="containsText" dxfId="56" priority="1" operator="containsText" text="Setup">
+    <cfRule type="containsText" dxfId="61" priority="1" operator="containsText" text="Setup">
       <formula>NOT(ISERROR(SEARCH("Setup",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F1048576">
-    <cfRule type="expression" dxfId="55" priority="9">
+    <cfRule type="expression" dxfId="60" priority="9">
       <formula>$B2="x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5410,6 +5462,59 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="19.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" style="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>259</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FF7030A0"/>
@@ -5950,7 +6055,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4">
     <tabColor rgb="FFFFC000"/>
@@ -7771,15 +7876,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7974,7 +8079,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFE03237"/>

</xml_diff>

<commit_message>
PDO error fixed. Compatible with PHP 5.5.9 now.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\finap\git\cs480\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\pub\cs480\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId9"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -1662,21 +1662,6 @@
   </cellStyles>
   <dxfs count="124">
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1873,6 +1858,21 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3545,7 +3545,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Task_List_Pivot" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" mergeItem="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Task_List_Pivot" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" mergeItem="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="B2:C21" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -4140,88 +4140,88 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:C30" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:C30" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="A1:C30"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Done" dataDxfId="2"/>
-    <tableColumn id="2" name="File" dataDxfId="0"/>
-    <tableColumn id="3" name="Feature" dataDxfId="1"/>
+    <tableColumn id="1" name="Done" dataDxfId="50"/>
+    <tableColumn id="2" name="File" dataDxfId="49"/>
+    <tableColumn id="3" name="Feature" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A1:Q15"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Name" dataDxfId="50"/>
-    <tableColumn id="2" name="Foreign Key1" dataDxfId="49"/>
-    <tableColumn id="3" name="Foreign Key2" dataDxfId="48"/>
-    <tableColumn id="4" name="Column1" dataDxfId="47"/>
-    <tableColumn id="5" name="Column2" dataDxfId="46"/>
-    <tableColumn id="6" name="Column3" dataDxfId="45"/>
-    <tableColumn id="7" name="Column4" dataDxfId="44"/>
-    <tableColumn id="8" name="Column5" dataDxfId="43"/>
-    <tableColumn id="9" name="Column6" dataDxfId="42"/>
-    <tableColumn id="13" name="Column7" dataDxfId="41"/>
-    <tableColumn id="12" name="Column8" dataDxfId="40"/>
-    <tableColumn id="11" name="Column9" dataDxfId="39"/>
-    <tableColumn id="17" name="Column10" dataDxfId="38"/>
-    <tableColumn id="16" name="Column11" dataDxfId="37"/>
-    <tableColumn id="15" name="Column12" dataDxfId="36"/>
-    <tableColumn id="14" name="Column13" dataDxfId="35"/>
-    <tableColumn id="10" name="Column14" dataDxfId="34"/>
+    <tableColumn id="1" name="Name" dataDxfId="45"/>
+    <tableColumn id="2" name="Foreign Key1" dataDxfId="44"/>
+    <tableColumn id="3" name="Foreign Key2" dataDxfId="43"/>
+    <tableColumn id="4" name="Column1" dataDxfId="42"/>
+    <tableColumn id="5" name="Column2" dataDxfId="41"/>
+    <tableColumn id="6" name="Column3" dataDxfId="40"/>
+    <tableColumn id="7" name="Column4" dataDxfId="39"/>
+    <tableColumn id="8" name="Column5" dataDxfId="38"/>
+    <tableColumn id="9" name="Column6" dataDxfId="37"/>
+    <tableColumn id="13" name="Column7" dataDxfId="36"/>
+    <tableColumn id="12" name="Column8" dataDxfId="35"/>
+    <tableColumn id="11" name="Column9" dataDxfId="34"/>
+    <tableColumn id="17" name="Column10" dataDxfId="33"/>
+    <tableColumn id="16" name="Column11" dataDxfId="32"/>
+    <tableColumn id="15" name="Column12" dataDxfId="31"/>
+    <tableColumn id="14" name="Column13" dataDxfId="30"/>
+    <tableColumn id="10" name="Column14" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A2:L108"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Notes: Client" dataDxfId="31"/>
-    <tableColumn id="2" name="A:C" dataDxfId="30"/>
-    <tableColumn id="3" name="U" dataDxfId="29"/>
-    <tableColumn id="4" name="S" dataDxfId="28"/>
-    <tableColumn id="5" name="Use Case: Client" dataDxfId="27"/>
-    <tableColumn id="6" name="Conversation" dataDxfId="26"/>
-    <tableColumn id="8" name="Use Case: Server" dataDxfId="25"/>
-    <tableColumn id="13" name="G" dataDxfId="24"/>
-    <tableColumn id="9" name="A:S" dataDxfId="23"/>
-    <tableColumn id="10" name="D" dataDxfId="22"/>
-    <tableColumn id="11" name="C" dataDxfId="21"/>
-    <tableColumn id="12" name="Notes: Server" dataDxfId="20"/>
+    <tableColumn id="1" name="Notes: Client" dataDxfId="26"/>
+    <tableColumn id="2" name="A:C" dataDxfId="25"/>
+    <tableColumn id="3" name="U" dataDxfId="24"/>
+    <tableColumn id="4" name="S" dataDxfId="23"/>
+    <tableColumn id="5" name="Use Case: Client" dataDxfId="22"/>
+    <tableColumn id="6" name="Conversation" dataDxfId="21"/>
+    <tableColumn id="8" name="Use Case: Server" dataDxfId="20"/>
+    <tableColumn id="13" name="G" dataDxfId="19"/>
+    <tableColumn id="9" name="A:S" dataDxfId="18"/>
+    <tableColumn id="10" name="D" dataDxfId="17"/>
+    <tableColumn id="11" name="C" dataDxfId="16"/>
+    <tableColumn id="12" name="Notes: Server" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:D21"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Type" dataDxfId="17"/>
-    <tableColumn id="6" name="Name" dataDxfId="16"/>
-    <tableColumn id="2" name="Messages" dataDxfId="15"/>
-    <tableColumn id="3" name="Collaborators" dataDxfId="14"/>
+    <tableColumn id="1" name="Type" dataDxfId="12"/>
+    <tableColumn id="6" name="Name" dataDxfId="11"/>
+    <tableColumn id="2" name="Messages" dataDxfId="10"/>
+    <tableColumn id="3" name="Collaborators" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G25"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Name" dataDxfId="11"/>
-    <tableColumn id="7" name="Dependencies" dataDxfId="10"/>
-    <tableColumn id="6" name="Route" dataDxfId="9"/>
-    <tableColumn id="2" name="Controller" dataDxfId="8"/>
-    <tableColumn id="4" name="Directive" dataDxfId="7"/>
-    <tableColumn id="3" name="Factory" dataDxfId="6"/>
-    <tableColumn id="5" name="Service" dataDxfId="5"/>
+    <tableColumn id="1" name="Name" dataDxfId="6"/>
+    <tableColumn id="7" name="Dependencies" dataDxfId="5"/>
+    <tableColumn id="6" name="Route" dataDxfId="4"/>
+    <tableColumn id="2" name="Controller" dataDxfId="3"/>
+    <tableColumn id="4" name="Directive" dataDxfId="2"/>
+    <tableColumn id="3" name="Factory" dataDxfId="1"/>
+    <tableColumn id="5" name="Service" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project: Red" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5468,8 +5468,8 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7883,8 +7883,8 @@
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Start of CRUD type classes. Register converted to new CRUD structure.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\pub\cs480\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\finap\git\cs480\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -514,7 +514,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="263">
   <si>
     <t>Design</t>
   </si>
@@ -842,9 +842,6 @@
   </si>
   <si>
     <t>visible BOOL DEFAULT true</t>
-  </si>
-  <si>
-    <t>user</t>
   </si>
   <si>
     <t>calendar</t>
@@ -1362,6 +1359,15 @@
   </si>
   <si>
     <t>$routeProvider to $stateProvider?</t>
+  </si>
+  <si>
+    <t>Own classes for the various items -- Database class should not need to check for $bindings['password']</t>
+  </si>
+  <si>
+    <t>PHP in general</t>
+  </si>
+  <si>
+    <t>person</t>
   </si>
 </sst>
 </file>
@@ -1660,7 +1666,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="124">
+  <dxfs count="125">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2348,32 +2359,32 @@
   </dxfs>
   <tableStyles count="5" defaultTableStyle="Senior Project" defaultPivotStyle="PivotTable Style 1">
     <tableStyle name="PivotTable Style 1" table="0" count="6">
-      <tableStyleElement type="wholeTable" dxfId="123"/>
-      <tableStyleElement type="headerRow" dxfId="122"/>
-      <tableStyleElement type="firstRowStripe" dxfId="121"/>
-      <tableStyleElement type="secondRowStripe" dxfId="120"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="119"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="118"/>
+      <tableStyleElement type="wholeTable" dxfId="124"/>
+      <tableStyleElement type="headerRow" dxfId="123"/>
+      <tableStyleElement type="firstRowStripe" dxfId="122"/>
+      <tableStyleElement type="secondRowStripe" dxfId="121"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="120"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="119"/>
     </tableStyle>
     <tableStyle name="Senior Project" pivot="0" count="4">
-      <tableStyleElement type="wholeTable" dxfId="117"/>
-      <tableStyleElement type="headerRow" dxfId="116"/>
-      <tableStyleElement type="firstRowStripe" dxfId="115"/>
-      <tableStyleElement type="secondRowStripe" dxfId="114"/>
+      <tableStyleElement type="wholeTable" dxfId="118"/>
+      <tableStyleElement type="headerRow" dxfId="117"/>
+      <tableStyleElement type="firstRowStripe" dxfId="116"/>
+      <tableStyleElement type="secondRowStripe" dxfId="115"/>
     </tableStyle>
     <tableStyle name="Senior Project: Red" pivot="0" count="4">
-      <tableStyleElement type="wholeTable" dxfId="113"/>
-      <tableStyleElement type="headerRow" dxfId="112"/>
-      <tableStyleElement type="firstRowStripe" dxfId="111"/>
-      <tableStyleElement type="secondRowStripe" dxfId="110"/>
+      <tableStyleElement type="wholeTable" dxfId="114"/>
+      <tableStyleElement type="headerRow" dxfId="113"/>
+      <tableStyleElement type="firstRowStripe" dxfId="112"/>
+      <tableStyleElement type="secondRowStripe" dxfId="111"/>
     </tableStyle>
     <tableStyle name="SlicerStyle1" pivot="0" table="0" count="10">
-      <tableStyleElement type="wholeTable" dxfId="109"/>
-      <tableStyleElement type="headerRow" dxfId="108"/>
+      <tableStyleElement type="wholeTable" dxfId="110"/>
+      <tableStyleElement type="headerRow" dxfId="109"/>
     </tableStyle>
     <tableStyle name="SlicerStyleDark1 2 2" pivot="0" table="0" count="10">
-      <tableStyleElement type="wholeTable" dxfId="107"/>
-      <tableStyleElement type="headerRow" dxfId="106"/>
+      <tableStyleElement type="wholeTable" dxfId="108"/>
+      <tableStyleElement type="headerRow" dxfId="107"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3660,7 +3671,7 @@
     <i/>
   </colItems>
   <formats count="33">
-    <format dxfId="99">
+    <format dxfId="100">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -3674,10 +3685,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="98">
+    <format dxfId="99">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="97">
+    <format dxfId="98">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -3691,16 +3702,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="96">
+    <format dxfId="97">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="95">
+    <format dxfId="96">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="94">
+    <format dxfId="95">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="93">
+    <format dxfId="94">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -3714,7 +3725,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="93">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3728,7 +3739,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="92">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3741,7 +3752,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="91">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3754,7 +3765,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3770,7 +3781,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3782,7 +3793,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3794,16 +3805,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="87">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="85">
+    <format dxfId="86">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="84">
+    <format dxfId="85">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="83">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -3817,7 +3828,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="83">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3831,7 +3842,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3844,7 +3855,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="81">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3857,7 +3868,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="80">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3873,7 +3884,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="79">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3885,7 +3896,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3897,10 +3908,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="77">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="75">
+    <format dxfId="76">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3909,7 +3920,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="75">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3918,7 +3929,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="74">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3927,7 +3938,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="73">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3936,7 +3947,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="72">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3945,7 +3956,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="71">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3957,7 +3968,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="70">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3970,7 +3981,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="69">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3983,7 +3994,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="68">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4119,7 +4130,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F30" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F30" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="B2:F30">
     <filterColumn colId="0">
       <filters blank="1"/>
@@ -4129,99 +4140,99 @@
     <sortCondition ref="C2:C30"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Done" dataDxfId="57"/>
-    <tableColumn id="3" name="Category" dataDxfId="56"/>
-    <tableColumn id="5" name="Remember" dataDxfId="55"/>
-    <tableColumn id="4" name="Look Into" dataDxfId="54"/>
-    <tableColumn id="2" name="Task" dataDxfId="53"/>
+    <tableColumn id="1" name="Done" dataDxfId="58"/>
+    <tableColumn id="3" name="Category" dataDxfId="57"/>
+    <tableColumn id="5" name="Remember" dataDxfId="56"/>
+    <tableColumn id="4" name="Look Into" dataDxfId="55"/>
+    <tableColumn id="2" name="Task" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:C30" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:C30" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="A1:C30"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Done" dataDxfId="50"/>
-    <tableColumn id="2" name="File" dataDxfId="49"/>
-    <tableColumn id="3" name="Feature" dataDxfId="48"/>
+    <tableColumn id="1" name="Done" dataDxfId="51"/>
+    <tableColumn id="2" name="File" dataDxfId="50"/>
+    <tableColumn id="3" name="Feature" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <autoFilter ref="A1:Q15"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Name" dataDxfId="45"/>
-    <tableColumn id="2" name="Foreign Key1" dataDxfId="44"/>
-    <tableColumn id="3" name="Foreign Key2" dataDxfId="43"/>
-    <tableColumn id="4" name="Column1" dataDxfId="42"/>
-    <tableColumn id="5" name="Column2" dataDxfId="41"/>
-    <tableColumn id="6" name="Column3" dataDxfId="40"/>
-    <tableColumn id="7" name="Column4" dataDxfId="39"/>
-    <tableColumn id="8" name="Column5" dataDxfId="38"/>
-    <tableColumn id="9" name="Column6" dataDxfId="37"/>
-    <tableColumn id="13" name="Column7" dataDxfId="36"/>
-    <tableColumn id="12" name="Column8" dataDxfId="35"/>
-    <tableColumn id="11" name="Column9" dataDxfId="34"/>
-    <tableColumn id="17" name="Column10" dataDxfId="33"/>
-    <tableColumn id="16" name="Column11" dataDxfId="32"/>
-    <tableColumn id="15" name="Column12" dataDxfId="31"/>
-    <tableColumn id="14" name="Column13" dataDxfId="30"/>
-    <tableColumn id="10" name="Column14" dataDxfId="29"/>
+    <tableColumn id="1" name="Name" dataDxfId="46"/>
+    <tableColumn id="2" name="Foreign Key1" dataDxfId="45"/>
+    <tableColumn id="3" name="Foreign Key2" dataDxfId="44"/>
+    <tableColumn id="4" name="Column1" dataDxfId="43"/>
+    <tableColumn id="5" name="Column2" dataDxfId="42"/>
+    <tableColumn id="6" name="Column3" dataDxfId="41"/>
+    <tableColumn id="7" name="Column4" dataDxfId="40"/>
+    <tableColumn id="8" name="Column5" dataDxfId="39"/>
+    <tableColumn id="9" name="Column6" dataDxfId="38"/>
+    <tableColumn id="13" name="Column7" dataDxfId="37"/>
+    <tableColumn id="12" name="Column8" dataDxfId="36"/>
+    <tableColumn id="11" name="Column9" dataDxfId="35"/>
+    <tableColumn id="17" name="Column10" dataDxfId="34"/>
+    <tableColumn id="16" name="Column11" dataDxfId="33"/>
+    <tableColumn id="15" name="Column12" dataDxfId="32"/>
+    <tableColumn id="14" name="Column13" dataDxfId="31"/>
+    <tableColumn id="10" name="Column14" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A2:L108"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Notes: Client" dataDxfId="26"/>
-    <tableColumn id="2" name="A:C" dataDxfId="25"/>
-    <tableColumn id="3" name="U" dataDxfId="24"/>
-    <tableColumn id="4" name="S" dataDxfId="23"/>
-    <tableColumn id="5" name="Use Case: Client" dataDxfId="22"/>
-    <tableColumn id="6" name="Conversation" dataDxfId="21"/>
-    <tableColumn id="8" name="Use Case: Server" dataDxfId="20"/>
-    <tableColumn id="13" name="G" dataDxfId="19"/>
-    <tableColumn id="9" name="A:S" dataDxfId="18"/>
-    <tableColumn id="10" name="D" dataDxfId="17"/>
-    <tableColumn id="11" name="C" dataDxfId="16"/>
-    <tableColumn id="12" name="Notes: Server" dataDxfId="15"/>
+    <tableColumn id="1" name="Notes: Client" dataDxfId="27"/>
+    <tableColumn id="2" name="A:C" dataDxfId="26"/>
+    <tableColumn id="3" name="U" dataDxfId="25"/>
+    <tableColumn id="4" name="S" dataDxfId="24"/>
+    <tableColumn id="5" name="Use Case: Client" dataDxfId="23"/>
+    <tableColumn id="6" name="Conversation" dataDxfId="22"/>
+    <tableColumn id="8" name="Use Case: Server" dataDxfId="21"/>
+    <tableColumn id="13" name="G" dataDxfId="20"/>
+    <tableColumn id="9" name="A:S" dataDxfId="19"/>
+    <tableColumn id="10" name="D" dataDxfId="18"/>
+    <tableColumn id="11" name="C" dataDxfId="17"/>
+    <tableColumn id="12" name="Notes: Server" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:D21"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Type" dataDxfId="12"/>
-    <tableColumn id="6" name="Name" dataDxfId="11"/>
-    <tableColumn id="2" name="Messages" dataDxfId="10"/>
-    <tableColumn id="3" name="Collaborators" dataDxfId="9"/>
+    <tableColumn id="1" name="Type" dataDxfId="13"/>
+    <tableColumn id="6" name="Name" dataDxfId="12"/>
+    <tableColumn id="2" name="Messages" dataDxfId="11"/>
+    <tableColumn id="3" name="Collaborators" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:G25"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Name" dataDxfId="6"/>
-    <tableColumn id="7" name="Dependencies" dataDxfId="5"/>
-    <tableColumn id="6" name="Route" dataDxfId="4"/>
-    <tableColumn id="2" name="Controller" dataDxfId="3"/>
-    <tableColumn id="4" name="Directive" dataDxfId="2"/>
-    <tableColumn id="3" name="Factory" dataDxfId="1"/>
-    <tableColumn id="5" name="Service" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="7"/>
+    <tableColumn id="7" name="Dependencies" dataDxfId="6"/>
+    <tableColumn id="6" name="Route" dataDxfId="5"/>
+    <tableColumn id="2" name="Controller" dataDxfId="4"/>
+    <tableColumn id="4" name="Directive" dataDxfId="3"/>
+    <tableColumn id="3" name="Factory" dataDxfId="2"/>
+    <tableColumn id="5" name="Service" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project: Red" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4952,7 +4963,7 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>36</v>
@@ -4960,7 +4971,7 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C3" s="18"/>
     </row>
@@ -4973,13 +4984,13 @@
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
       <c r="C5" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="13"/>
       <c r="C6" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -4991,31 +5002,31 @@
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
       <c r="C9" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="18"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
       <c r="C12" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
@@ -5027,47 +5038,47 @@
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="13"/>
       <c r="C14" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
       <c r="C16" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="13"/>
       <c r="C17" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="13"/>
       <c r="C18" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C19" s="18"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C20" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C21" s="18"/>
     </row>
@@ -5084,22 +5095,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B25:C1048576 B1:C21">
-    <cfRule type="expression" dxfId="105" priority="1">
+    <cfRule type="expression" dxfId="106" priority="1">
       <formula>$B1="Setup"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="2">
+    <cfRule type="expression" dxfId="105" priority="2">
       <formula>$B1="CSS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="3">
+    <cfRule type="expression" dxfId="104" priority="3">
       <formula>$B1="HTML"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="4">
+    <cfRule type="expression" dxfId="103" priority="4">
       <formula>$B1="JS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="5">
+    <cfRule type="expression" dxfId="102" priority="5">
       <formula>$B1="DB"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="6">
+    <cfRule type="expression" dxfId="101" priority="6">
       <formula>$B1="PHP"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5124,7 +5135,7 @@
   <dimension ref="B2:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5144,16 +5155,16 @@
   <sheetData>
     <row r="2" spans="2:6" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>134</v>
-      </c>
       <c r="D2" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>36</v>
@@ -5164,10 +5175,10 @@
         <v>64</v>
       </c>
       <c r="C3" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>135</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5175,7 +5186,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>64</v>
@@ -5189,13 +5200,13 @@
         <v>64</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>64</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -5203,7 +5214,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -5211,7 +5222,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -5219,10 +5230,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -5230,18 +5241,18 @@
         <v>2</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C10" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5255,48 +5266,48 @@
         <v>64</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C12" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C13" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>64</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C14" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C15" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>64</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5304,10 +5315,10 @@
         <v>64</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -5315,7 +5326,7 @@
         <v>3</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -5323,7 +5334,7 @@
         <v>3</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5334,7 +5345,7 @@
         <v>3</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5345,7 +5356,7 @@
         <v>3</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -5353,7 +5364,7 @@
         <v>3</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -5361,10 +5372,10 @@
         <v>3</v>
       </c>
       <c r="D22" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>205</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="60" x14ac:dyDescent="0.25">
@@ -5372,10 +5383,10 @@
         <v>3</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -5383,10 +5394,10 @@
         <v>3</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -5397,7 +5408,7 @@
         <v>64</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -5418,29 +5429,29 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="C1:E1048576">
-    <cfRule type="containsText" dxfId="66" priority="2" operator="containsText" text="CSS">
+    <cfRule type="containsText" dxfId="67" priority="2" operator="containsText" text="CSS">
       <formula>NOT(ISERROR(SEARCH("CSS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="3" operator="containsText" text="HTML">
+    <cfRule type="containsText" dxfId="66" priority="3" operator="containsText" text="HTML">
       <formula>NOT(ISERROR(SEARCH("HTML",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="4" operator="containsText" text="JS">
+    <cfRule type="containsText" dxfId="65" priority="4" operator="containsText" text="JS">
       <formula>NOT(ISERROR(SEARCH("JS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="5" operator="containsText" text="DB">
+    <cfRule type="containsText" dxfId="64" priority="5" operator="containsText" text="DB">
       <formula>NOT(ISERROR(SEARCH("DB",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="6" operator="containsText" text="PHP">
+    <cfRule type="containsText" dxfId="63" priority="6" operator="containsText" text="PHP">
       <formula>NOT(ISERROR(SEARCH("PHP",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="containsText" dxfId="61" priority="1" operator="containsText" text="Setup">
+    <cfRule type="containsText" dxfId="62" priority="1" operator="containsText" text="Setup">
       <formula>NOT(ISERROR(SEARCH("Setup",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F1048576">
-    <cfRule type="expression" dxfId="60" priority="9">
+    <cfRule type="expression" dxfId="61" priority="9">
       <formula>$B2="x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5466,10 +5477,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5481,32 +5492,45 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>254</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>256</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>259</v>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$B4="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -5521,8 +5545,8 @@
   </sheetPr>
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5573,30 +5597,30 @@
         <v>98</v>
       </c>
       <c r="K1" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="O1" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="O1" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>128</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>107</v>
+        <v>262</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -5604,44 +5628,44 @@
         <v>87</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>212</v>
-      </c>
       <c r="G2" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>117</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>118</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>56</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M2" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="N2" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>183</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>184</v>
       </c>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>88</v>
@@ -5651,10 +5675,10 @@
         <v>87</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>158</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>159</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -5689,7 +5713,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>88</v>
@@ -5699,7 +5723,7 @@
         <v>87</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>106</v>
@@ -5724,25 +5748,25 @@
         <v>89</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>87</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>55</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
@@ -5755,7 +5779,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>88</v>
@@ -5765,7 +5789,7 @@
         <v>87</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -5788,16 +5812,16 @@
         <v>90</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>87</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>104</v>
@@ -5817,7 +5841,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>91</v>
@@ -5827,7 +5851,7 @@
         <v>87</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>104</v>
@@ -5865,20 +5889,20 @@
     </row>
     <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="12" t="s">
         <v>87</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>103</v>
@@ -5887,7 +5911,7 @@
         <v>101</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
@@ -5900,7 +5924,7 @@
     </row>
     <row r="12" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -5908,43 +5932,43 @@
         <v>87</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F12" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="H12" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="H12" s="12" t="s">
-        <v>122</v>
-      </c>
       <c r="I12" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="J12" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="K12" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="L12" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="M12" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="M12" s="12" t="s">
+      <c r="N12" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="N12" s="12" t="s">
+      <c r="O12" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="O12" s="12" t="s">
+      <c r="P12" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="P12" s="12" t="s">
+      <c r="Q12" s="12" t="s">
         <v>221</v>
-      </c>
-      <c r="Q12" s="12" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -5968,7 +5992,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>89</v>
@@ -5980,7 +6004,7 @@
         <v>87</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -5997,7 +6021,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>90</v>
@@ -6009,7 +6033,7 @@
         <v>87</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
@@ -6036,10 +6060,10 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" t="s">
         <v>131</v>
-      </c>
-      <c r="B20" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -6149,7 +6173,7 @@
         <v>69</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>69</v>
@@ -6179,7 +6203,7 @@
         <v>73</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>72</v>
@@ -6205,10 +6229,10 @@
         <v>80</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9" t="s">
@@ -6221,7 +6245,7 @@
         <v>64</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -6237,7 +6261,7 @@
         <v>81</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>81</v>
@@ -6253,7 +6277,7 @@
         <v>64</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="210" x14ac:dyDescent="0.25">
@@ -6301,7 +6325,7 @@
         <v>10</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>10</v>
@@ -6367,7 +6391,7 @@
         <v>71</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>71</v>
@@ -6394,13 +6418,13 @@
         <v>64</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F11" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>166</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>167</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -6427,7 +6451,7 @@
         <v>70</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>70</v>
@@ -6449,10 +6473,10 @@
       <c r="D13" s="9"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -6464,7 +6488,7 @@
     </row>
     <row r="14" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>64</v>
@@ -6476,13 +6500,13 @@
         <v>64</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -6506,13 +6530,13 @@
         <v>64</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
@@ -6536,13 +6560,13 @@
         <v>64</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -6562,7 +6586,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
@@ -6586,11 +6610,11 @@
         <v>64</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -7898,82 +7922,82 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>54</v>
       </c>
       <c r="C1" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" s="33" t="s">
         <v>228</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -7981,10 +8005,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -7992,10 +8016,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -8003,10 +8027,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -8014,10 +8038,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -8025,13 +8049,13 @@
         <v>3</v>
       </c>
       <c r="B12" s="34" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="31" t="s">
         <v>235</v>
       </c>
-      <c r="C12" s="31" t="s">
-        <v>236</v>
-      </c>
       <c r="D12" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -8039,13 +8063,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -8053,10 +8077,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -8064,10 +8088,10 @@
         <v>3</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -8106,27 +8130,27 @@
         <v>54</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>191</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>60</v>
@@ -8140,11 +8164,11 @@
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D3" s="30"/>
       <c r="E3" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
@@ -8162,7 +8186,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D5" s="30"/>
       <c r="E5" s="30"/>
@@ -8184,7 +8208,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>60</v>
@@ -8216,7 +8240,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>60</v>
@@ -8232,7 +8256,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
CaLogin and authentication started. Some project strcuture optimizations. Currently facing error with execute().
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <definedName name="Slicer_Category1">#N/A</definedName>
     <definedName name="Slicer_Done">#N/A</definedName>
     <definedName name="Slicer_Done1">#N/A</definedName>
+    <definedName name="Slicer_Done2">#N/A</definedName>
     <definedName name="Slicer_Look_Into">#N/A</definedName>
     <definedName name="Slicer_Look_Into1">#N/A</definedName>
     <definedName name="Slicer_Remember">#N/A</definedName>
@@ -51,6 +52,7 @@
         <x14:slicerCache r:id="rId14"/>
         <x14:slicerCache r:id="rId15"/>
         <x14:slicerCache r:id="rId16"/>
+        <x14:slicerCache r:id="rId17"/>
       </x15:slicerCaches>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -514,7 +516,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="265">
   <si>
     <t>Design</t>
   </si>
@@ -1361,13 +1363,19 @@
     <t>$routeProvider to $stateProvider?</t>
   </si>
   <si>
-    <t>Own classes for the various items -- Database class should not need to check for $bindings['password']</t>
-  </si>
-  <si>
-    <t>PHP in general</t>
-  </si>
-  <si>
     <t>person</t>
+  </si>
+  <si>
+    <t>Many</t>
+  </si>
+  <si>
+    <t>Message display ("flash service") system</t>
+  </si>
+  <si>
+    <t>register js</t>
+  </si>
+  <si>
+    <t>Move logic to service (how to access vm.loading from service without watch?)</t>
   </si>
 </sst>
 </file>
@@ -1673,6 +1681,125 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1908,68 +2035,6 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2067,63 +2132,6 @@
     </dxf>
     <dxf>
       <alignment vertical="top" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3355,6 +3363,83 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Done 2"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Done 2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5562600" y="190501"/>
+              <a:ext cx="1219200" cy="1104900"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a table slicer. Table slicers are supported in Excel or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2007 or earlier, the slicer can't be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Fina Jo" refreshedDate="42426.829079629628" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="23">
   <cacheSource type="worksheet">
@@ -3671,6 +3756,46 @@
     <i/>
   </colItems>
   <formats count="33">
+    <format dxfId="106">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="105">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="104">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="103">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="102">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="101">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
     <format dxfId="100">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
@@ -3686,46 +3811,6 @@
       </pivotArea>
     </format>
     <format dxfId="99">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="98">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="97">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="96">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="95">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
-    </format>
-    <format dxfId="94">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="93">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3739,7 +3824,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="98">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3752,7 +3837,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="97">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3765,7 +3850,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="96">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3781,7 +3866,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="95">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3793,7 +3878,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="94">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3805,16 +3890,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="93">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="86">
+    <format dxfId="92">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="85">
+    <format dxfId="91">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="84">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -3828,7 +3913,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3842,7 +3927,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3855,7 +3940,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="87">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3868,7 +3953,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3884,7 +3969,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="85">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3896,7 +3981,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3908,10 +3993,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="83">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="76">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3920,7 +4005,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="81">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3929,7 +4014,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="80">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3938,7 +4023,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="79">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3947,7 +4032,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -3956,7 +4041,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="77">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3968,7 +4053,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="76">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3981,7 +4066,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="75">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3994,7 +4079,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="74">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4112,6 +4197,16 @@
 </slicerCacheDefinition>
 </file>
 
+<file path=xl/slicerCaches/slicerCache8.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_Done2" sourceName="Done">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="6" column="1"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <slicer name="Category" cache="Slicer_Category" caption="Category" rowHeight="241300"/>
@@ -4129,8 +4224,14 @@
 </slicers>
 </file>
 
+<file path=xl/slicers/slicer3.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <slicer name="Done 2" cache="Slicer_Done2" caption="Done" rowHeight="241300"/>
+</slicers>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F30" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F30" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
   <autoFilter ref="B2:F30">
     <filterColumn colId="0">
       <filters blank="1"/>
@@ -4140,99 +4241,103 @@
     <sortCondition ref="C2:C30"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Done" dataDxfId="58"/>
-    <tableColumn id="3" name="Category" dataDxfId="57"/>
-    <tableColumn id="5" name="Remember" dataDxfId="56"/>
-    <tableColumn id="4" name="Look Into" dataDxfId="55"/>
-    <tableColumn id="2" name="Task" dataDxfId="54"/>
+    <tableColumn id="1" name="Done" dataDxfId="71"/>
+    <tableColumn id="3" name="Category" dataDxfId="70"/>
+    <tableColumn id="5" name="Remember" dataDxfId="69"/>
+    <tableColumn id="4" name="Look Into" dataDxfId="68"/>
+    <tableColumn id="2" name="Task" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:C30" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
-  <autoFilter ref="A1:C30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:D31" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
+  <autoFilter ref="B2:D31">
+    <filterColumn colId="0">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="Done" dataDxfId="51"/>
-    <tableColumn id="2" name="File" dataDxfId="50"/>
-    <tableColumn id="3" name="Feature" dataDxfId="49"/>
+    <tableColumn id="1" name="Done" dataDxfId="64"/>
+    <tableColumn id="2" name="File" dataDxfId="63"/>
+    <tableColumn id="3" name="Feature" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="A1:Q15"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Name" dataDxfId="46"/>
-    <tableColumn id="2" name="Foreign Key1" dataDxfId="45"/>
-    <tableColumn id="3" name="Foreign Key2" dataDxfId="44"/>
-    <tableColumn id="4" name="Column1" dataDxfId="43"/>
-    <tableColumn id="5" name="Column2" dataDxfId="42"/>
-    <tableColumn id="6" name="Column3" dataDxfId="41"/>
-    <tableColumn id="7" name="Column4" dataDxfId="40"/>
-    <tableColumn id="8" name="Column5" dataDxfId="39"/>
-    <tableColumn id="9" name="Column6" dataDxfId="38"/>
-    <tableColumn id="13" name="Column7" dataDxfId="37"/>
-    <tableColumn id="12" name="Column8" dataDxfId="36"/>
-    <tableColumn id="11" name="Column9" dataDxfId="35"/>
-    <tableColumn id="17" name="Column10" dataDxfId="34"/>
-    <tableColumn id="16" name="Column11" dataDxfId="33"/>
-    <tableColumn id="15" name="Column12" dataDxfId="32"/>
-    <tableColumn id="14" name="Column13" dataDxfId="31"/>
-    <tableColumn id="10" name="Column14" dataDxfId="30"/>
+    <tableColumn id="1" name="Name" dataDxfId="59"/>
+    <tableColumn id="2" name="Foreign Key1" dataDxfId="58"/>
+    <tableColumn id="3" name="Foreign Key2" dataDxfId="57"/>
+    <tableColumn id="4" name="Column1" dataDxfId="56"/>
+    <tableColumn id="5" name="Column2" dataDxfId="55"/>
+    <tableColumn id="6" name="Column3" dataDxfId="54"/>
+    <tableColumn id="7" name="Column4" dataDxfId="53"/>
+    <tableColumn id="8" name="Column5" dataDxfId="52"/>
+    <tableColumn id="9" name="Column6" dataDxfId="51"/>
+    <tableColumn id="13" name="Column7" dataDxfId="50"/>
+    <tableColumn id="12" name="Column8" dataDxfId="49"/>
+    <tableColumn id="11" name="Column9" dataDxfId="48"/>
+    <tableColumn id="17" name="Column10" dataDxfId="47"/>
+    <tableColumn id="16" name="Column11" dataDxfId="46"/>
+    <tableColumn id="15" name="Column12" dataDxfId="45"/>
+    <tableColumn id="14" name="Column13" dataDxfId="44"/>
+    <tableColumn id="10" name="Column14" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="A2:L108"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Notes: Client" dataDxfId="27"/>
-    <tableColumn id="2" name="A:C" dataDxfId="26"/>
-    <tableColumn id="3" name="U" dataDxfId="25"/>
-    <tableColumn id="4" name="S" dataDxfId="24"/>
-    <tableColumn id="5" name="Use Case: Client" dataDxfId="23"/>
-    <tableColumn id="6" name="Conversation" dataDxfId="22"/>
-    <tableColumn id="8" name="Use Case: Server" dataDxfId="21"/>
-    <tableColumn id="13" name="G" dataDxfId="20"/>
-    <tableColumn id="9" name="A:S" dataDxfId="19"/>
-    <tableColumn id="10" name="D" dataDxfId="18"/>
-    <tableColumn id="11" name="C" dataDxfId="17"/>
-    <tableColumn id="12" name="Notes: Server" dataDxfId="16"/>
+    <tableColumn id="1" name="Notes: Client" dataDxfId="40"/>
+    <tableColumn id="2" name="A:C" dataDxfId="39"/>
+    <tableColumn id="3" name="U" dataDxfId="38"/>
+    <tableColumn id="4" name="S" dataDxfId="37"/>
+    <tableColumn id="5" name="Use Case: Client" dataDxfId="36"/>
+    <tableColumn id="6" name="Conversation" dataDxfId="35"/>
+    <tableColumn id="8" name="Use Case: Server" dataDxfId="34"/>
+    <tableColumn id="13" name="G" dataDxfId="33"/>
+    <tableColumn id="9" name="A:S" dataDxfId="32"/>
+    <tableColumn id="10" name="D" dataDxfId="31"/>
+    <tableColumn id="11" name="C" dataDxfId="30"/>
+    <tableColumn id="12" name="Notes: Server" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:D21"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Type" dataDxfId="13"/>
-    <tableColumn id="6" name="Name" dataDxfId="12"/>
-    <tableColumn id="2" name="Messages" dataDxfId="11"/>
-    <tableColumn id="3" name="Collaborators" dataDxfId="10"/>
+    <tableColumn id="1" name="Type" dataDxfId="26"/>
+    <tableColumn id="6" name="Name" dataDxfId="25"/>
+    <tableColumn id="2" name="Messages" dataDxfId="24"/>
+    <tableColumn id="3" name="Collaborators" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:G25"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Name" dataDxfId="7"/>
-    <tableColumn id="7" name="Dependencies" dataDxfId="6"/>
-    <tableColumn id="6" name="Route" dataDxfId="5"/>
-    <tableColumn id="2" name="Controller" dataDxfId="4"/>
-    <tableColumn id="4" name="Directive" dataDxfId="3"/>
-    <tableColumn id="3" name="Factory" dataDxfId="2"/>
-    <tableColumn id="5" name="Service" dataDxfId="1"/>
+    <tableColumn id="1" name="Name" dataDxfId="20"/>
+    <tableColumn id="7" name="Dependencies" dataDxfId="19"/>
+    <tableColumn id="6" name="Route" dataDxfId="18"/>
+    <tableColumn id="2" name="Controller" dataDxfId="17"/>
+    <tableColumn id="4" name="Directive" dataDxfId="16"/>
+    <tableColumn id="3" name="Factory" dataDxfId="15"/>
+    <tableColumn id="5" name="Service" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project: Red" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5095,22 +5200,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B25:C1048576 B1:C21">
-    <cfRule type="expression" dxfId="106" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>$B1="Setup"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>$B1="CSS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>$B1="HTML"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>$B1="JS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>$B1="DB"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>$B1="PHP"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5429,29 +5534,29 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="C1:E1048576">
-    <cfRule type="containsText" dxfId="67" priority="2" operator="containsText" text="CSS">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="CSS">
       <formula>NOT(ISERROR(SEARCH("CSS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="3" operator="containsText" text="HTML">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="HTML">
       <formula>NOT(ISERROR(SEARCH("HTML",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="4" operator="containsText" text="JS">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="JS">
       <formula>NOT(ISERROR(SEARCH("JS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="5" operator="containsText" text="DB">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="DB">
       <formula>NOT(ISERROR(SEARCH("DB",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="6" operator="containsText" text="PHP">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="PHP">
       <formula>NOT(ISERROR(SEARCH("PHP",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="containsText" dxfId="62" priority="1" operator="containsText" text="Setup">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Setup">
       <formula>NOT(ISERROR(SEARCH("Setup",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F1048576">
-    <cfRule type="expression" dxfId="61" priority="9">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>$B2="x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5477,64 +5582,85 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="19.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="4"/>
+    <col min="3" max="3" width="19.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="2" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D3" s="12" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+    <row r="4" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D4" s="12" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>260</v>
+      <c r="D5" s="16" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C4">
+  <conditionalFormatting sqref="D5">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$B4="x"</formula>
+      <formula>$C5="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{3A4CF648-6AED-40f4-86FF-DC5316D8AED3}">
+      <x14:slicerList xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5545,7 +5671,7 @@
   </sheetPr>
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -5620,7 +5746,7 @@
     </row>
     <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>

</xml_diff>

<commit_message>
Generalized userService to crudService. Cleaned up registration and login.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -517,7 +517,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="271">
   <si>
     <t>Design</t>
   </si>
@@ -1380,6 +1380,21 @@
   </si>
   <si>
     <t>.htaccess from XAMPP to appropriate location</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Add cookie support</t>
+  </si>
+  <si>
+    <t>register, login</t>
+  </si>
+  <si>
+    <t>Usernames should not be case sensitive</t>
+  </si>
+  <si>
+    <t>Controllers are nearly identical; fix if time</t>
   </si>
 </sst>
 </file>
@@ -3086,7 +3101,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -3158,7 +3173,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -3225,12 +3240,12 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -3296,13 +3311,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -4613,8 +4628,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4709,7 +4724,9 @@
       <c r="C8" s="25">
         <v>5</v>
       </c>
-      <c r="D8" s="25"/>
+      <c r="D8" s="25" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="24" t="s">
@@ -4718,7 +4735,9 @@
       <c r="C9" s="25">
         <v>2</v>
       </c>
-      <c r="D9" s="25"/>
+      <c r="D9" s="25" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="24" t="s">
@@ -5244,7 +5263,7 @@
   <dimension ref="B2:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5318,7 +5337,10 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="C6" s="15" t="s">
         <v>2</v>
       </c>
@@ -5386,7 +5408,10 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="C13" s="15" t="s">
         <v>137</v>
       </c>
@@ -5438,7 +5463,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="C18" s="15" t="s">
         <v>3</v>
       </c>
@@ -5594,10 +5622,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B2:D6"/>
+  <dimension ref="B2:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5658,6 +5686,30 @@
         <v>264</v>
       </c>
     </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>270</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D5">
     <cfRule type="expression" dxfId="53" priority="1">
@@ -5665,14 +5717,15 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{3A4CF648-6AED-40f4-86FF-DC5316D8AED3}">
       <x14:slicerList xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicer r:id="rId3"/>
+        <x14:slicer r:id="rId4"/>
       </x14:slicerList>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Fixed error with update. Will need to overhaul api returns if have time. See notes.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -517,7 +517,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="272">
   <si>
     <t>Design</t>
   </si>
@@ -1382,9 +1382,6 @@
     <t>.htaccess from XAMPP to appropriate location</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Add cookie support</t>
   </si>
   <si>
@@ -1394,7 +1391,13 @@
     <t>Usernames should not be case sensitive</t>
   </si>
   <si>
-    <t>Controllers are nearly identical; fix if time</t>
+    <t>Controllers and services are nearly identical</t>
+  </si>
+  <si>
+    <t>SessionHander.php, db files</t>
+  </si>
+  <si>
+    <t>rowCount will return 0 if data is the same, but no error occurred; change api to return errors as something other than 0</t>
   </si>
 </sst>
 </file>
@@ -3101,7 +3104,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -3174,7 +3177,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>333375</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
       <mc:Choice Requires="sle15">
@@ -3239,13 +3242,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -3311,14 +3314,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:rowOff>333374</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
       <mc:Choice Requires="sle15">
@@ -4256,7 +4259,7 @@
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
-  <sortState ref="B6:F30">
+  <sortState ref="B8:F30">
     <sortCondition ref="C2:C30"/>
   </sortState>
   <tableColumns count="5">
@@ -4628,8 +4631,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4725,7 +4728,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>266</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4736,7 +4739,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>266</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5263,7 +5266,7 @@
   <dimension ref="B2:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5348,7 +5351,10 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="C7" s="15" t="s">
         <v>2</v>
       </c>
@@ -5380,10 +5386,13 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C10" s="15" t="s">
-        <v>137</v>
+        <v>2</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>204</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>142</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5405,7 +5414,7 @@
         <v>137</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5426,22 +5435,19 @@
       <c r="C14" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>204</v>
-      </c>
       <c r="F14" s="16" t="s">
-        <v>252</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C15" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>64</v>
+      <c r="D15" s="15" t="s">
+        <v>204</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5457,10 +5463,13 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C17" s="15" t="s">
-        <v>3</v>
+        <v>137</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>64</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>136</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5501,18 +5510,15 @@
         <v>3</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C22" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="15" t="s">
-        <v>204</v>
-      </c>
       <c r="F22" s="16" t="s">
-        <v>205</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="60" x14ac:dyDescent="0.25">
@@ -5523,7 +5529,7 @@
         <v>204</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -5534,29 +5540,29 @@
         <v>204</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C25" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="15" t="s">
-        <v>64</v>
+      <c r="D25" s="15" t="s">
+        <v>204</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>147</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C26" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>204</v>
+        <v>3</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>64</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>265</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -5622,10 +5628,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B2:D9"/>
+  <dimension ref="B2:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5691,23 +5697,39 @@
         <v>3</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>268</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D9" s="12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C11" s="4" t="s">
         <v>270</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -5739,7 +5761,7 @@
   </sheetPr>
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Reworked redirection on not logged in. Fixed a few errors missed on the promise revamp.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,8 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId9"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
   </pivotCaches>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
@@ -517,7 +516,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="282">
   <si>
     <t>Design</t>
   </si>
@@ -1201,9 +1200,6 @@
     <t>recurrence(id)</t>
   </si>
   <si>
-    <t>activity_prefs</t>
-  </si>
-  <si>
     <t>activity_prefs(id)</t>
   </si>
   <si>
@@ -1340,9 +1336,6 @@
     <t>Set new &lt;base href=""&gt; as needed</t>
   </si>
   <si>
-    <t>Check that app.min.js is actually smaller than app.js</t>
-  </si>
-  <si>
     <t>File</t>
   </si>
   <si>
@@ -1398,6 +1391,42 @@
   </si>
   <si>
     <t>rowCount will return 0 if data is the same, but no error occurred; change api to return errors as something other than 0</t>
+  </si>
+  <si>
+    <t>header.controller.js</t>
+  </si>
+  <si>
+    <t>Update of name and url to directive? (Issue with view updating)</t>
+  </si>
+  <si>
+    <t>sessionVarManager.php</t>
+  </si>
+  <si>
+    <t>Move api calls to another file. Managers are acting as controller and should not contain logic</t>
+  </si>
+  <si>
+    <t>Autoload</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>Normalize</t>
+  </si>
+  <si>
+    <t>activity_info</t>
+  </si>
+  <si>
+    <t>Move map of app.min.js to another file</t>
+  </si>
+  <si>
+    <t>header.*.js</t>
+  </si>
+  <si>
+    <t>Username under a resolve</t>
+  </si>
+  <si>
+    <t>Convert angularjs back to .min.js</t>
   </si>
 </sst>
 </file>
@@ -3104,7 +3133,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -3320,11 +3349,11 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>333374</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>514350</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-      <mc:Choice Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="5" name="Remember"/>
@@ -3341,7 +3370,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -3352,7 +3381,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="7972425" y="2095499"/>
-              <a:ext cx="1314450" cy="904875"/>
+              <a:ext cx="1314450" cy="895351"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3400,8 +3429,8 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-      <mc:Choice Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Done 2"/>
@@ -3418,7 +3447,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -3428,7 +3457,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5562600" y="190501"/>
+              <a:off x="5791200" y="190501"/>
               <a:ext cx="1219200" cy="1104900"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3663,7 +3692,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Task_List_Pivot" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" mergeItem="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Task_List_Pivot" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" mergeItem="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="B2:C21" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -4631,7 +4660,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -5265,8 +5294,8 @@
   </sheetPr>
   <dimension ref="B2:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5381,7 +5410,7 @@
         <v>204</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -5392,7 +5421,7 @@
         <v>204</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5447,7 +5476,7 @@
         <v>204</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5469,7 +5498,7 @@
         <v>64</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5513,7 +5542,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="C22" s="15" t="s">
         <v>3</v>
       </c>
@@ -5566,7 +5598,15 @@
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F27" s="16"/>
+      <c r="C27" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F28" s="16"/>
@@ -5628,17 +5668,17 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B2:D11"/>
+  <dimension ref="B2:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="4"/>
-    <col min="3" max="3" width="19.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="48.7109375" style="12" customWidth="1"/>
     <col min="5" max="5" width="2.85546875" customWidth="1"/>
   </cols>
@@ -5648,18 +5688,18 @@
         <v>132</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5667,18 +5707,18 @@
         <v>64</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5686,10 +5726,10 @@
         <v>64</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -5697,39 +5737,82 @@
         <v>3</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>267</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="C11" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C12" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D12" s="12" t="s">
         <v>271</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C13" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -5761,8 +5844,8 @@
   </sheetPr>
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5836,7 +5919,7 @@
     </row>
     <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -5844,10 +5927,10 @@
         <v>87</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>210</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>211</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>114</v>
@@ -5865,7 +5948,7 @@
         <v>56</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M2" s="12" t="s">
         <v>181</v>
@@ -5939,7 +6022,7 @@
         <v>87</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>106</v>
@@ -5964,13 +6047,13 @@
         <v>89</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>87</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>199</v>
@@ -5982,7 +6065,7 @@
         <v>55</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
@@ -6005,7 +6088,7 @@
         <v>87</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -6028,13 +6111,13 @@
         <v>90</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>87</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>155</v>
@@ -6067,7 +6150,7 @@
         <v>87</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>104</v>
@@ -6105,7 +6188,7 @@
     </row>
     <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>207</v>
+        <v>277</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>206</v>
@@ -6118,7 +6201,7 @@
         <v>154</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>103</v>
@@ -6160,31 +6243,31 @@
         <v>121</v>
       </c>
       <c r="I12" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="J12" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="K12" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="L12" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="M12" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="M12" s="12" t="s">
+      <c r="N12" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="N12" s="12" t="s">
+      <c r="O12" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="O12" s="12" t="s">
+      <c r="P12" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="P12" s="12" t="s">
+      <c r="Q12" s="12" t="s">
         <v>220</v>
-      </c>
-      <c r="Q12" s="12" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -8138,16 +8221,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>54</v>
       </c>
       <c r="C1" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1" s="33" t="s">
         <v>227</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -8155,10 +8238,10 @@
         <v>137</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8166,10 +8249,10 @@
         <v>137</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -8177,10 +8260,10 @@
         <v>137</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -8188,10 +8271,10 @@
         <v>137</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -8199,10 +8282,10 @@
         <v>137</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -8210,10 +8293,10 @@
         <v>137</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -8221,10 +8304,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -8232,10 +8315,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -8243,10 +8326,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -8254,10 +8337,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -8265,13 +8348,13 @@
         <v>3</v>
       </c>
       <c r="B12" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C12" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="C12" s="31" t="s">
-        <v>235</v>
-      </c>
       <c r="D12" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -8279,13 +8362,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -8293,10 +8376,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -8304,10 +8387,10 @@
         <v>3</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -8402,7 +8485,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D5" s="30"/>
       <c r="E5" s="30"/>

</xml_diff>

<commit_message>
Added events and tasks. And some tests. Got sick of not having them.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -175,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0" shapeId="0">
+    <comment ref="G8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -516,7 +516,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="283">
   <si>
     <t>Design</t>
   </si>
@@ -1427,6 +1427,9 @@
   </si>
   <si>
     <t>Convert angularjs back to .min.js</t>
+  </si>
+  <si>
+    <t>Promise maker vs manually making array</t>
   </si>
 </sst>
 </file>
@@ -1727,6 +1730,130 @@
   </cellStyles>
   <dxfs count="125">
     <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1941,11 +2068,6 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1967,68 +2089,6 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2126,63 +2186,6 @@
     </dxf>
     <dxf>
       <alignment vertical="top" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3807,6 +3810,46 @@
     <i/>
   </colItems>
   <formats count="33">
+    <format dxfId="106">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="105">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="104">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="103">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="102">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="101">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
     <format dxfId="100">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
@@ -3822,46 +3865,6 @@
       </pivotArea>
     </format>
     <format dxfId="99">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="98">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="97">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="96">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="95">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
-    </format>
-    <format dxfId="94">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="93">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3875,7 +3878,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="98">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3888,7 +3891,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="97">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3901,7 +3904,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="96">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3917,7 +3920,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="95">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3929,7 +3932,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="94">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3941,16 +3944,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="93">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="86">
+    <format dxfId="92">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="85">
+    <format dxfId="91">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="84">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -3964,7 +3967,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3978,7 +3981,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3991,7 +3994,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="87">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4004,7 +4007,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4020,7 +4023,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="85">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4032,7 +4035,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4044,10 +4047,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="83">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="76">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4056,7 +4059,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="81">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4065,7 +4068,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="80">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4074,7 +4077,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="79">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4083,7 +4086,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4092,7 +4095,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="77">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4104,7 +4107,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="76">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4117,7 +4120,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="75">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4130,7 +4133,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="74">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4282,7 +4285,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F30" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F30" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
   <autoFilter ref="B2:F30">
     <filterColumn colId="0">
       <filters blank="1"/>
@@ -4292,103 +4295,103 @@
     <sortCondition ref="C2:C30"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Done" dataDxfId="58"/>
-    <tableColumn id="3" name="Category" dataDxfId="57"/>
-    <tableColumn id="5" name="Remember" dataDxfId="56"/>
-    <tableColumn id="4" name="Look Into" dataDxfId="55"/>
-    <tableColumn id="2" name="Task" dataDxfId="54"/>
+    <tableColumn id="1" name="Done" dataDxfId="71"/>
+    <tableColumn id="3" name="Category" dataDxfId="70"/>
+    <tableColumn id="5" name="Remember" dataDxfId="69"/>
+    <tableColumn id="4" name="Look Into" dataDxfId="68"/>
+    <tableColumn id="2" name="Task" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:D31" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:D31" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="B2:D31">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="Done" dataDxfId="50"/>
-    <tableColumn id="2" name="File" dataDxfId="49"/>
-    <tableColumn id="3" name="Feature" dataDxfId="48"/>
+    <tableColumn id="1" name="Done" dataDxfId="64"/>
+    <tableColumn id="2" name="File" dataDxfId="63"/>
+    <tableColumn id="3" name="Feature" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="A1:Q15"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Name" dataDxfId="45"/>
-    <tableColumn id="2" name="Foreign Key1" dataDxfId="44"/>
-    <tableColumn id="3" name="Foreign Key2" dataDxfId="43"/>
-    <tableColumn id="4" name="Column1" dataDxfId="42"/>
-    <tableColumn id="5" name="Column2" dataDxfId="41"/>
-    <tableColumn id="6" name="Column3" dataDxfId="40"/>
-    <tableColumn id="7" name="Column4" dataDxfId="39"/>
-    <tableColumn id="8" name="Column5" dataDxfId="38"/>
-    <tableColumn id="9" name="Column6" dataDxfId="37"/>
-    <tableColumn id="13" name="Column7" dataDxfId="36"/>
-    <tableColumn id="12" name="Column8" dataDxfId="35"/>
-    <tableColumn id="11" name="Column9" dataDxfId="34"/>
-    <tableColumn id="17" name="Column10" dataDxfId="33"/>
-    <tableColumn id="16" name="Column11" dataDxfId="32"/>
-    <tableColumn id="15" name="Column12" dataDxfId="31"/>
-    <tableColumn id="14" name="Column13" dataDxfId="30"/>
-    <tableColumn id="10" name="Column14" dataDxfId="29"/>
+    <tableColumn id="1" name="Name" dataDxfId="59"/>
+    <tableColumn id="2" name="Foreign Key1" dataDxfId="58"/>
+    <tableColumn id="3" name="Foreign Key2" dataDxfId="57"/>
+    <tableColumn id="4" name="Column1" dataDxfId="56"/>
+    <tableColumn id="5" name="Column2" dataDxfId="55"/>
+    <tableColumn id="6" name="Column3" dataDxfId="54"/>
+    <tableColumn id="7" name="Column4" dataDxfId="53"/>
+    <tableColumn id="8" name="Column5" dataDxfId="52"/>
+    <tableColumn id="9" name="Column6" dataDxfId="51"/>
+    <tableColumn id="13" name="Column7" dataDxfId="50"/>
+    <tableColumn id="12" name="Column8" dataDxfId="49"/>
+    <tableColumn id="11" name="Column9" dataDxfId="48"/>
+    <tableColumn id="17" name="Column10" dataDxfId="47"/>
+    <tableColumn id="16" name="Column11" dataDxfId="46"/>
+    <tableColumn id="15" name="Column12" dataDxfId="45"/>
+    <tableColumn id="14" name="Column13" dataDxfId="44"/>
+    <tableColumn id="10" name="Column14" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="A2:L108"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Notes: Client" dataDxfId="26"/>
-    <tableColumn id="2" name="A:C" dataDxfId="25"/>
-    <tableColumn id="3" name="U" dataDxfId="24"/>
-    <tableColumn id="4" name="S" dataDxfId="23"/>
-    <tableColumn id="5" name="Use Case: Client" dataDxfId="22"/>
-    <tableColumn id="6" name="Conversation" dataDxfId="21"/>
-    <tableColumn id="8" name="Use Case: Server" dataDxfId="20"/>
-    <tableColumn id="13" name="G" dataDxfId="19"/>
-    <tableColumn id="9" name="A:S" dataDxfId="18"/>
-    <tableColumn id="10" name="D" dataDxfId="17"/>
-    <tableColumn id="11" name="C" dataDxfId="16"/>
-    <tableColumn id="12" name="Notes: Server" dataDxfId="15"/>
+    <tableColumn id="1" name="Notes: Client" dataDxfId="40"/>
+    <tableColumn id="2" name="A:C" dataDxfId="39"/>
+    <tableColumn id="3" name="U" dataDxfId="38"/>
+    <tableColumn id="4" name="S" dataDxfId="37"/>
+    <tableColumn id="5" name="Use Case: Client" dataDxfId="36"/>
+    <tableColumn id="6" name="Conversation" dataDxfId="35"/>
+    <tableColumn id="8" name="Use Case: Server" dataDxfId="34"/>
+    <tableColumn id="13" name="G" dataDxfId="33"/>
+    <tableColumn id="9" name="A:S" dataDxfId="32"/>
+    <tableColumn id="10" name="D" dataDxfId="31"/>
+    <tableColumn id="11" name="C" dataDxfId="30"/>
+    <tableColumn id="12" name="Notes: Server" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:D21"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Type" dataDxfId="12"/>
-    <tableColumn id="6" name="Name" dataDxfId="11"/>
-    <tableColumn id="2" name="Messages" dataDxfId="10"/>
-    <tableColumn id="3" name="Collaborators" dataDxfId="9"/>
+    <tableColumn id="1" name="Type" dataDxfId="26"/>
+    <tableColumn id="6" name="Name" dataDxfId="25"/>
+    <tableColumn id="2" name="Messages" dataDxfId="24"/>
+    <tableColumn id="3" name="Collaborators" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:G25"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Name" dataDxfId="6"/>
-    <tableColumn id="7" name="Dependencies" dataDxfId="5"/>
-    <tableColumn id="6" name="Route" dataDxfId="4"/>
-    <tableColumn id="2" name="Controller" dataDxfId="3"/>
-    <tableColumn id="4" name="Directive" dataDxfId="2"/>
-    <tableColumn id="3" name="Factory" dataDxfId="1"/>
-    <tableColumn id="5" name="Service" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="20"/>
+    <tableColumn id="7" name="Dependencies" dataDxfId="19"/>
+    <tableColumn id="6" name="Route" dataDxfId="18"/>
+    <tableColumn id="2" name="Controller" dataDxfId="17"/>
+    <tableColumn id="4" name="Directive" dataDxfId="16"/>
+    <tableColumn id="3" name="Factory" dataDxfId="15"/>
+    <tableColumn id="5" name="Service" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project: Red" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4660,8 +4663,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5255,22 +5258,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B25:C1048576 B1:C21">
-    <cfRule type="expression" dxfId="106" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>$B1="Setup"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>$B1="CSS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>$B1="HTML"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>$B1="JS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>$B1="DB"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>$B1="PHP"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5294,7 +5297,7 @@
   </sheetPr>
   <dimension ref="B2:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -5620,29 +5623,29 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="C1:E1048576">
-    <cfRule type="containsText" dxfId="67" priority="2" operator="containsText" text="CSS">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="CSS">
       <formula>NOT(ISERROR(SEARCH("CSS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="3" operator="containsText" text="HTML">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="HTML">
       <formula>NOT(ISERROR(SEARCH("HTML",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="4" operator="containsText" text="JS">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="JS">
       <formula>NOT(ISERROR(SEARCH("JS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="5" operator="containsText" text="DB">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="DB">
       <formula>NOT(ISERROR(SEARCH("DB",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="6" operator="containsText" text="PHP">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="PHP">
       <formula>NOT(ISERROR(SEARCH("PHP",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="containsText" dxfId="62" priority="1" operator="containsText" text="Setup">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Setup">
       <formula>NOT(ISERROR(SEARCH("Setup",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F1048576">
-    <cfRule type="expression" dxfId="61" priority="9">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>$B2="x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5668,10 +5671,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B2:D16"/>
+  <dimension ref="B2:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5815,9 +5818,17 @@
         <v>280</v>
       </c>
     </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>282</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="53" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$C5="x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5844,8 +5855,8 @@
   </sheetPr>
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6053,20 +6064,18 @@
         <v>87</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>198</v>
+        <v>55</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="I6" s="12" t="s">
         <v>223</v>
       </c>
+      <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
@@ -6117,17 +6126,15 @@
         <v>87</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>222</v>
+        <v>155</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>155</v>
+        <v>104</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="H8" s="12" t="s">
         <v>57</v>
       </c>
+      <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
@@ -6198,21 +6205,23 @@
         <v>87</v>
       </c>
       <c r="E11" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="G11" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="H11" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="I11" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="J11" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>

</xml_diff>

<commit_message>
Added tasks directive to view tasks.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -5297,8 +5297,8 @@
   </sheetPr>
   <dimension ref="B2:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5855,8 +5855,8 @@
   </sheetPr>
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added bootstrap to save time on areas not being graded for. Will rework without bootstrap if have time. Tasks can now be listed, updated, and deleted.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -516,7 +516,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="285">
   <si>
     <t>Design</t>
   </si>
@@ -1430,6 +1430,12 @@
   </si>
   <si>
     <t>Promise maker vs manually making array</t>
+  </si>
+  <si>
+    <t>Trim + lowercase email and username</t>
+  </si>
+  <si>
+    <t>Option to create labels and calendars when choosing category in edit task/event</t>
   </si>
 </sst>
 </file>
@@ -4663,8 +4669,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5297,8 +5303,8 @@
   </sheetPr>
   <dimension ref="B2:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5612,7 +5618,12 @@
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F28" s="16"/>
+      <c r="C28" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F29" s="16"/>
@@ -5671,10 +5682,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B2:D17"/>
+  <dimension ref="B2:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5824,6 +5835,14 @@
       </c>
       <c r="D17" s="12" t="s">
         <v>282</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Slight rework of ActivityCRUD's create. Full CRUD on tasks now working.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -31,7 +31,7 @@
     <definedName name="Slicer_Look_Into1">#N/A</definedName>
     <definedName name="Slicer_Remember">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId9"/>
   </pivotCaches>
@@ -516,7 +516,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="285">
   <si>
     <t>Design</t>
   </si>
@@ -1736,130 +1736,6 @@
   </cellStyles>
   <dxfs count="125">
     <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2074,6 +1950,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2095,6 +1976,68 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2192,6 +2135,63 @@
     </dxf>
     <dxf>
       <alignment vertical="top" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3361,8 +3361,8 @@
       <xdr:row>22</xdr:row>
       <xdr:rowOff>514350</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="5" name="Remember"/>
@@ -3379,7 +3379,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -3438,8 +3438,8 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Done 2"/>
@@ -3456,7 +3456,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -3816,46 +3816,6 @@
     <i/>
   </colItems>
   <formats count="33">
-    <format dxfId="106">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="105">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="104">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="103">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="102">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="101">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
-    </format>
     <format dxfId="100">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
@@ -3871,6 +3831,46 @@
       </pivotArea>
     </format>
     <format dxfId="99">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="98">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="97">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="96">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="95">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="94">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="93">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3884,7 +3884,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="98">
+    <format dxfId="92">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3897,7 +3897,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="97">
+    <format dxfId="91">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3910,7 +3910,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="96">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3926,7 +3926,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="95">
+    <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3938,7 +3938,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="94">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3950,16 +3950,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="93">
+    <format dxfId="87">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="92">
+    <format dxfId="86">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="91">
+    <format dxfId="85">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="90">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -3973,7 +3973,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="83">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3987,7 +3987,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4000,7 +4000,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="81">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4013,7 +4013,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="80">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4029,7 +4029,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="79">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4041,7 +4041,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="84">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4053,10 +4053,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="77">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="82">
+    <format dxfId="76">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4065,7 +4065,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="75">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4074,7 +4074,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="74">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4083,7 +4083,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="73">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4092,7 +4092,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="72">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4101,7 +4101,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="71">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4113,7 +4113,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="70">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4126,7 +4126,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="69">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4139,7 +4139,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="68">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4291,7 +4291,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F30" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F30" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="B2:F30">
     <filterColumn colId="0">
       <filters blank="1"/>
@@ -4301,103 +4301,103 @@
     <sortCondition ref="C2:C30"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Done" dataDxfId="71"/>
-    <tableColumn id="3" name="Category" dataDxfId="70"/>
-    <tableColumn id="5" name="Remember" dataDxfId="69"/>
-    <tableColumn id="4" name="Look Into" dataDxfId="68"/>
-    <tableColumn id="2" name="Task" dataDxfId="67"/>
+    <tableColumn id="1" name="Done" dataDxfId="58"/>
+    <tableColumn id="3" name="Category" dataDxfId="57"/>
+    <tableColumn id="5" name="Remember" dataDxfId="56"/>
+    <tableColumn id="4" name="Look Into" dataDxfId="55"/>
+    <tableColumn id="2" name="Task" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:D31" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:D31" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="B2:D31">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="Done" dataDxfId="64"/>
-    <tableColumn id="2" name="File" dataDxfId="63"/>
-    <tableColumn id="3" name="Feature" dataDxfId="62"/>
+    <tableColumn id="1" name="Done" dataDxfId="50"/>
+    <tableColumn id="2" name="File" dataDxfId="49"/>
+    <tableColumn id="3" name="Feature" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A1:Q15"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Name" dataDxfId="59"/>
-    <tableColumn id="2" name="Foreign Key1" dataDxfId="58"/>
-    <tableColumn id="3" name="Foreign Key2" dataDxfId="57"/>
-    <tableColumn id="4" name="Column1" dataDxfId="56"/>
-    <tableColumn id="5" name="Column2" dataDxfId="55"/>
-    <tableColumn id="6" name="Column3" dataDxfId="54"/>
-    <tableColumn id="7" name="Column4" dataDxfId="53"/>
-    <tableColumn id="8" name="Column5" dataDxfId="52"/>
-    <tableColumn id="9" name="Column6" dataDxfId="51"/>
-    <tableColumn id="13" name="Column7" dataDxfId="50"/>
-    <tableColumn id="12" name="Column8" dataDxfId="49"/>
-    <tableColumn id="11" name="Column9" dataDxfId="48"/>
-    <tableColumn id="17" name="Column10" dataDxfId="47"/>
-    <tableColumn id="16" name="Column11" dataDxfId="46"/>
-    <tableColumn id="15" name="Column12" dataDxfId="45"/>
-    <tableColumn id="14" name="Column13" dataDxfId="44"/>
-    <tableColumn id="10" name="Column14" dataDxfId="43"/>
+    <tableColumn id="1" name="Name" dataDxfId="45"/>
+    <tableColumn id="2" name="Foreign Key1" dataDxfId="44"/>
+    <tableColumn id="3" name="Foreign Key2" dataDxfId="43"/>
+    <tableColumn id="4" name="Column1" dataDxfId="42"/>
+    <tableColumn id="5" name="Column2" dataDxfId="41"/>
+    <tableColumn id="6" name="Column3" dataDxfId="40"/>
+    <tableColumn id="7" name="Column4" dataDxfId="39"/>
+    <tableColumn id="8" name="Column5" dataDxfId="38"/>
+    <tableColumn id="9" name="Column6" dataDxfId="37"/>
+    <tableColumn id="13" name="Column7" dataDxfId="36"/>
+    <tableColumn id="12" name="Column8" dataDxfId="35"/>
+    <tableColumn id="11" name="Column9" dataDxfId="34"/>
+    <tableColumn id="17" name="Column10" dataDxfId="33"/>
+    <tableColumn id="16" name="Column11" dataDxfId="32"/>
+    <tableColumn id="15" name="Column12" dataDxfId="31"/>
+    <tableColumn id="14" name="Column13" dataDxfId="30"/>
+    <tableColumn id="10" name="Column14" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A2:L108"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Notes: Client" dataDxfId="40"/>
-    <tableColumn id="2" name="A:C" dataDxfId="39"/>
-    <tableColumn id="3" name="U" dataDxfId="38"/>
-    <tableColumn id="4" name="S" dataDxfId="37"/>
-    <tableColumn id="5" name="Use Case: Client" dataDxfId="36"/>
-    <tableColumn id="6" name="Conversation" dataDxfId="35"/>
-    <tableColumn id="8" name="Use Case: Server" dataDxfId="34"/>
-    <tableColumn id="13" name="G" dataDxfId="33"/>
-    <tableColumn id="9" name="A:S" dataDxfId="32"/>
-    <tableColumn id="10" name="D" dataDxfId="31"/>
-    <tableColumn id="11" name="C" dataDxfId="30"/>
-    <tableColumn id="12" name="Notes: Server" dataDxfId="29"/>
+    <tableColumn id="1" name="Notes: Client" dataDxfId="26"/>
+    <tableColumn id="2" name="A:C" dataDxfId="25"/>
+    <tableColumn id="3" name="U" dataDxfId="24"/>
+    <tableColumn id="4" name="S" dataDxfId="23"/>
+    <tableColumn id="5" name="Use Case: Client" dataDxfId="22"/>
+    <tableColumn id="6" name="Conversation" dataDxfId="21"/>
+    <tableColumn id="8" name="Use Case: Server" dataDxfId="20"/>
+    <tableColumn id="13" name="G" dataDxfId="19"/>
+    <tableColumn id="9" name="A:S" dataDxfId="18"/>
+    <tableColumn id="10" name="D" dataDxfId="17"/>
+    <tableColumn id="11" name="C" dataDxfId="16"/>
+    <tableColumn id="12" name="Notes: Server" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:D21"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Type" dataDxfId="26"/>
-    <tableColumn id="6" name="Name" dataDxfId="25"/>
-    <tableColumn id="2" name="Messages" dataDxfId="24"/>
-    <tableColumn id="3" name="Collaborators" dataDxfId="23"/>
+    <tableColumn id="1" name="Type" dataDxfId="12"/>
+    <tableColumn id="6" name="Name" dataDxfId="11"/>
+    <tableColumn id="2" name="Messages" dataDxfId="10"/>
+    <tableColumn id="3" name="Collaborators" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G25"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Name" dataDxfId="20"/>
-    <tableColumn id="7" name="Dependencies" dataDxfId="19"/>
-    <tableColumn id="6" name="Route" dataDxfId="18"/>
-    <tableColumn id="2" name="Controller" dataDxfId="17"/>
-    <tableColumn id="4" name="Directive" dataDxfId="16"/>
-    <tableColumn id="3" name="Factory" dataDxfId="15"/>
-    <tableColumn id="5" name="Service" dataDxfId="14"/>
+    <tableColumn id="1" name="Name" dataDxfId="6"/>
+    <tableColumn id="7" name="Dependencies" dataDxfId="5"/>
+    <tableColumn id="6" name="Route" dataDxfId="4"/>
+    <tableColumn id="2" name="Controller" dataDxfId="3"/>
+    <tableColumn id="4" name="Directive" dataDxfId="2"/>
+    <tableColumn id="3" name="Factory" dataDxfId="1"/>
+    <tableColumn id="5" name="Service" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project: Red" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4669,8 +4669,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4880,7 +4880,9 @@
       <c r="C17" s="25">
         <v>5</v>
       </c>
-      <c r="D17" s="25"/>
+      <c r="D17" s="25" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="24" t="s">
@@ -4907,7 +4909,9 @@
       <c r="C20" s="25">
         <v>1</v>
       </c>
-      <c r="D20" s="25"/>
+      <c r="D20" s="25" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="21" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="24" t="s">
@@ -4916,7 +4920,9 @@
       <c r="C21" s="25">
         <v>1</v>
       </c>
-      <c r="D21" s="25"/>
+      <c r="D21" s="25" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="24" t="s">
@@ -4925,7 +4931,9 @@
       <c r="C22" s="25">
         <v>5</v>
       </c>
-      <c r="D22" s="25"/>
+      <c r="D22" s="25" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24" t="s">
@@ -5078,7 +5086,10 @@
       <c r="C39" s="27">
         <v>105</v>
       </c>
-      <c r="D39" s="27"/>
+      <c r="D39" s="27">
+        <f>SUMIF(D2:D38,"&lt;&gt;",C2:C38)</f>
+        <v>24</v>
+      </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
@@ -5264,22 +5275,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B25:C1048576 B1:C21">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="106" priority="1">
       <formula>$B1="Setup"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="105" priority="2">
       <formula>$B1="CSS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="104" priority="3">
       <formula>$B1="HTML"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="103" priority="4">
       <formula>$B1="JS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="102" priority="5">
       <formula>$B1="DB"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="101" priority="6">
       <formula>$B1="PHP"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5634,29 +5645,29 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="C1:E1048576">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="CSS">
+    <cfRule type="containsText" dxfId="67" priority="2" operator="containsText" text="CSS">
       <formula>NOT(ISERROR(SEARCH("CSS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="HTML">
+    <cfRule type="containsText" dxfId="66" priority="3" operator="containsText" text="HTML">
       <formula>NOT(ISERROR(SEARCH("HTML",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="JS">
+    <cfRule type="containsText" dxfId="65" priority="4" operator="containsText" text="JS">
       <formula>NOT(ISERROR(SEARCH("JS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="DB">
+    <cfRule type="containsText" dxfId="64" priority="5" operator="containsText" text="DB">
       <formula>NOT(ISERROR(SEARCH("DB",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="PHP">
+    <cfRule type="containsText" dxfId="63" priority="6" operator="containsText" text="PHP">
       <formula>NOT(ISERROR(SEARCH("PHP",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Setup">
+    <cfRule type="containsText" dxfId="62" priority="1" operator="containsText" text="Setup">
       <formula>NOT(ISERROR(SEARCH("Setup",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F1048576">
-    <cfRule type="expression" dxfId="1" priority="9">
+    <cfRule type="expression" dxfId="61" priority="9">
       <formula>$B2="x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5847,7 +5858,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="53" priority="1">
       <formula>$C5="x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5875,7 +5886,7 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Events and tasks now resolved before dashboard is loaded. Fixed error when getting events.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -516,7 +516,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="285">
   <si>
     <t>Design</t>
   </si>
@@ -868,9 +868,6 @@
   </si>
   <si>
     <t>admin BOOL DEFAULT false</t>
-  </si>
-  <si>
-    <t>priority ENUM('low', 'normal', 'high') DEFAULT 'normal'</t>
   </si>
   <si>
     <t>theme ENUM('light', 'dark') DEFAULT 'light'</t>
@@ -1436,6 +1433,9 @@
   </si>
   <si>
     <t>Option to create labels and calendars when choosing category in edit task/event</t>
+  </si>
+  <si>
+    <t>priority BOOL</t>
   </si>
 </sst>
 </file>
@@ -4669,8 +4669,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4891,7 +4891,9 @@
       <c r="C18" s="25">
         <v>1</v>
       </c>
-      <c r="D18" s="25"/>
+      <c r="D18" s="25" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="24" t="s">
@@ -5088,7 +5090,7 @@
       </c>
       <c r="D39" s="27">
         <f>SUMIF(D2:D38,"&lt;&gt;",C2:C38)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
@@ -5143,7 +5145,7 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>36</v>
@@ -5151,7 +5153,7 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C3" s="18"/>
     </row>
@@ -5164,13 +5166,13 @@
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
       <c r="C5" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="13"/>
       <c r="C6" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -5182,31 +5184,31 @@
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
       <c r="C9" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C10" s="18"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
       <c r="C12" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
@@ -5218,47 +5220,47 @@
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="13"/>
       <c r="C14" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
       <c r="C16" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="13"/>
       <c r="C17" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="13"/>
       <c r="C18" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C19" s="18"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C20" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C21" s="18"/>
     </row>
@@ -5335,16 +5337,16 @@
   <sheetData>
     <row r="2" spans="2:6" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>133</v>
-      </c>
       <c r="D2" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>36</v>
@@ -5355,10 +5357,10 @@
         <v>64</v>
       </c>
       <c r="C3" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>134</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5366,7 +5368,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>64</v>
@@ -5380,13 +5382,13 @@
         <v>64</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>64</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5397,7 +5399,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5408,7 +5410,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -5416,10 +5418,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -5427,10 +5429,10 @@
         <v>2</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -5438,10 +5440,10 @@
         <v>2</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5455,15 +5457,15 @@
         <v>64</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C12" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5471,32 +5473,32 @@
         <v>64</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>64</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C14" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C15" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5504,21 +5506,21 @@
         <v>64</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C17" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>64</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5529,7 +5531,7 @@
         <v>3</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5540,7 +5542,7 @@
         <v>3</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5551,7 +5553,7 @@
         <v>3</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -5559,7 +5561,7 @@
         <v>3</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5570,7 +5572,7 @@
         <v>3</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="60" x14ac:dyDescent="0.25">
@@ -5578,10 +5580,10 @@
         <v>3</v>
       </c>
       <c r="D23" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="F23" s="16" t="s">
         <v>204</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -5589,10 +5591,10 @@
         <v>3</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -5600,10 +5602,10 @@
         <v>3</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -5614,26 +5616,26 @@
         <v>64</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C27" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C28" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -5710,21 +5712,21 @@
   <sheetData>
     <row r="2" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>251</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>253</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5732,18 +5734,18 @@
         <v>64</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>255</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>259</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5751,10 +5753,10 @@
         <v>64</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>261</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -5762,31 +5764,31 @@
         <v>3</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>265</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -5794,26 +5796,26 @@
         <v>64</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>268</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C12" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>270</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C13" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>272</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
@@ -5821,23 +5823,23 @@
         <v>3</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C15" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>275</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>279</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
@@ -5845,15 +5847,15 @@
         <v>3</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -5885,8 +5887,8 @@
   </sheetPr>
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5937,30 +5939,30 @@
         <v>98</v>
       </c>
       <c r="K1" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="O1" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="O1" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>127</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -5968,44 +5970,44 @@
         <v>87</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>209</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>210</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>114</v>
       </c>
       <c r="H2" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>116</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>117</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>56</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="M2" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="N2" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>182</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>183</v>
       </c>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>88</v>
@@ -6015,10 +6017,10 @@
         <v>87</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>157</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>158</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -6063,7 +6065,7 @@
         <v>87</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>106</v>
@@ -6088,22 +6090,22 @@
         <v>89</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>87</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>55</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -6127,7 +6129,7 @@
         <v>87</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -6150,13 +6152,13 @@
         <v>90</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>87</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>104</v>
@@ -6187,7 +6189,7 @@
         <v>87</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>104</v>
@@ -6223,25 +6225,25 @@
       <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
     </row>
-    <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="12" t="s">
         <v>87</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>103</v>
@@ -6250,7 +6252,7 @@
         <v>101</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>115</v>
+        <v>284</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
@@ -6270,43 +6272,43 @@
         <v>87</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F12" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="H12" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="H12" s="12" t="s">
-        <v>121</v>
-      </c>
       <c r="I12" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="J12" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="K12" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="L12" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="M12" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="M12" s="12" t="s">
+      <c r="N12" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="N12" s="12" t="s">
+      <c r="O12" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="O12" s="12" t="s">
+      <c r="P12" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="P12" s="12" t="s">
+      <c r="Q12" s="12" t="s">
         <v>219</v>
-      </c>
-      <c r="Q12" s="12" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -6398,10 +6400,10 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" t="s">
         <v>130</v>
-      </c>
-      <c r="B20" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -6511,7 +6513,7 @@
         <v>69</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>69</v>
@@ -6541,7 +6543,7 @@
         <v>73</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>72</v>
@@ -6567,10 +6569,10 @@
         <v>80</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9" t="s">
@@ -6583,7 +6585,7 @@
         <v>64</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -6599,7 +6601,7 @@
         <v>81</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>81</v>
@@ -6615,7 +6617,7 @@
         <v>64</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="210" x14ac:dyDescent="0.25">
@@ -6663,7 +6665,7 @@
         <v>10</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>10</v>
@@ -6729,7 +6731,7 @@
         <v>71</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>71</v>
@@ -6756,13 +6758,13 @@
         <v>64</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F11" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>165</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>166</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -6789,7 +6791,7 @@
         <v>70</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>70</v>
@@ -6811,10 +6813,10 @@
       <c r="D13" s="9"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -6826,7 +6828,7 @@
     </row>
     <row r="14" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>64</v>
@@ -6838,13 +6840,13 @@
         <v>64</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -6868,13 +6870,13 @@
         <v>64</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
@@ -6898,13 +6900,13 @@
         <v>64</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -6924,7 +6926,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
@@ -6948,11 +6950,11 @@
         <v>64</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -8260,82 +8262,82 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>54</v>
       </c>
       <c r="C1" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="33" t="s">
         <v>226</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -8343,10 +8345,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -8354,10 +8356,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -8365,10 +8367,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -8376,10 +8378,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -8387,13 +8389,13 @@
         <v>3</v>
       </c>
       <c r="B12" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="C12" s="31" t="s">
         <v>233</v>
       </c>
-      <c r="C12" s="31" t="s">
-        <v>234</v>
-      </c>
       <c r="D12" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -8401,13 +8403,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -8415,10 +8417,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -8426,10 +8428,10 @@
         <v>3</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -8468,27 +8470,27 @@
         <v>54</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>60</v>
@@ -8502,11 +8504,11 @@
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D3" s="30"/>
       <c r="E3" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
@@ -8524,7 +8526,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D5" s="30"/>
       <c r="E5" s="30"/>
@@ -8546,7 +8548,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>60</v>
@@ -8578,7 +8580,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>60</v>
@@ -8594,7 +8596,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Fixed error when saving session caused by the last error fix. A perfect example of why tests are good. In middle of modal work for events.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -516,7 +516,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="284">
   <si>
     <t>Design</t>
   </si>
@@ -681,9 +681,6 @@
   </si>
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>description TEXT</t>
   </si>
   <si>
     <t>avatar TEXT</t>
@@ -868,6 +865,9 @@
   </si>
   <si>
     <t>admin BOOL DEFAULT false</t>
+  </si>
+  <si>
+    <t>priority ENUM('low', 'normal', 'high') DEFAULT 'normal'</t>
   </si>
   <si>
     <t>theme ENUM('light', 'dark') DEFAULT 'light'</t>
@@ -1433,9 +1433,6 @@
   </si>
   <si>
     <t>Option to create labels and calendars when choosing category in edit task/event</t>
-  </si>
-  <si>
-    <t>priority BOOL</t>
   </si>
 </sst>
 </file>
@@ -1736,6 +1733,130 @@
   </cellStyles>
   <dxfs count="125">
     <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1950,11 +2071,6 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1976,68 +2092,6 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2135,63 +2189,6 @@
     </dxf>
     <dxf>
       <alignment vertical="top" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3816,6 +3813,46 @@
     <i/>
   </colItems>
   <formats count="33">
+    <format dxfId="106">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="105">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="104">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="103">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="102">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="101">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
     <format dxfId="100">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
@@ -3831,46 +3868,6 @@
       </pivotArea>
     </format>
     <format dxfId="99">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="98">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="97">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="96">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="95">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
-    </format>
-    <format dxfId="94">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="93">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3884,7 +3881,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="98">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3897,7 +3894,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="97">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3910,7 +3907,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="96">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3926,7 +3923,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="95">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3938,7 +3935,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="94">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3950,16 +3947,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="93">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="86">
+    <format dxfId="92">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="85">
+    <format dxfId="91">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="84">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -3973,7 +3970,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3987,7 +3984,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4000,7 +3997,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="87">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4013,7 +4010,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4029,7 +4026,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="85">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4041,7 +4038,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4053,10 +4050,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="83">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="76">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4065,7 +4062,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="81">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4074,7 +4071,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="80">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4083,7 +4080,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="79">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4092,7 +4089,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4101,7 +4098,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="77">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4113,7 +4110,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="76">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4126,7 +4123,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="75">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4139,7 +4136,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="74">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4291,7 +4288,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F30" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F30" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
   <autoFilter ref="B2:F30">
     <filterColumn colId="0">
       <filters blank="1"/>
@@ -4301,103 +4298,103 @@
     <sortCondition ref="C2:C30"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Done" dataDxfId="58"/>
-    <tableColumn id="3" name="Category" dataDxfId="57"/>
-    <tableColumn id="5" name="Remember" dataDxfId="56"/>
-    <tableColumn id="4" name="Look Into" dataDxfId="55"/>
-    <tableColumn id="2" name="Task" dataDxfId="54"/>
+    <tableColumn id="1" name="Done" dataDxfId="71"/>
+    <tableColumn id="3" name="Category" dataDxfId="70"/>
+    <tableColumn id="5" name="Remember" dataDxfId="69"/>
+    <tableColumn id="4" name="Look Into" dataDxfId="68"/>
+    <tableColumn id="2" name="Task" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:D31" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:D31" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="B2:D31">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="Done" dataDxfId="50"/>
-    <tableColumn id="2" name="File" dataDxfId="49"/>
-    <tableColumn id="3" name="Feature" dataDxfId="48"/>
+    <tableColumn id="1" name="Done" dataDxfId="64"/>
+    <tableColumn id="2" name="File" dataDxfId="63"/>
+    <tableColumn id="3" name="Feature" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="A1:Q15"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Name" dataDxfId="45"/>
-    <tableColumn id="2" name="Foreign Key1" dataDxfId="44"/>
-    <tableColumn id="3" name="Foreign Key2" dataDxfId="43"/>
-    <tableColumn id="4" name="Column1" dataDxfId="42"/>
-    <tableColumn id="5" name="Column2" dataDxfId="41"/>
-    <tableColumn id="6" name="Column3" dataDxfId="40"/>
-    <tableColumn id="7" name="Column4" dataDxfId="39"/>
-    <tableColumn id="8" name="Column5" dataDxfId="38"/>
-    <tableColumn id="9" name="Column6" dataDxfId="37"/>
-    <tableColumn id="13" name="Column7" dataDxfId="36"/>
-    <tableColumn id="12" name="Column8" dataDxfId="35"/>
-    <tableColumn id="11" name="Column9" dataDxfId="34"/>
-    <tableColumn id="17" name="Column10" dataDxfId="33"/>
-    <tableColumn id="16" name="Column11" dataDxfId="32"/>
-    <tableColumn id="15" name="Column12" dataDxfId="31"/>
-    <tableColumn id="14" name="Column13" dataDxfId="30"/>
-    <tableColumn id="10" name="Column14" dataDxfId="29"/>
+    <tableColumn id="1" name="Name" dataDxfId="59"/>
+    <tableColumn id="2" name="Foreign Key1" dataDxfId="58"/>
+    <tableColumn id="3" name="Foreign Key2" dataDxfId="57"/>
+    <tableColumn id="4" name="Column1" dataDxfId="56"/>
+    <tableColumn id="5" name="Column2" dataDxfId="55"/>
+    <tableColumn id="6" name="Column3" dataDxfId="54"/>
+    <tableColumn id="7" name="Column4" dataDxfId="53"/>
+    <tableColumn id="8" name="Column5" dataDxfId="52"/>
+    <tableColumn id="9" name="Column6" dataDxfId="51"/>
+    <tableColumn id="13" name="Column7" dataDxfId="50"/>
+    <tableColumn id="12" name="Column8" dataDxfId="49"/>
+    <tableColumn id="11" name="Column9" dataDxfId="48"/>
+    <tableColumn id="17" name="Column10" dataDxfId="47"/>
+    <tableColumn id="16" name="Column11" dataDxfId="46"/>
+    <tableColumn id="15" name="Column12" dataDxfId="45"/>
+    <tableColumn id="14" name="Column13" dataDxfId="44"/>
+    <tableColumn id="10" name="Column14" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="A2:L108"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Notes: Client" dataDxfId="26"/>
-    <tableColumn id="2" name="A:C" dataDxfId="25"/>
-    <tableColumn id="3" name="U" dataDxfId="24"/>
-    <tableColumn id="4" name="S" dataDxfId="23"/>
-    <tableColumn id="5" name="Use Case: Client" dataDxfId="22"/>
-    <tableColumn id="6" name="Conversation" dataDxfId="21"/>
-    <tableColumn id="8" name="Use Case: Server" dataDxfId="20"/>
-    <tableColumn id="13" name="G" dataDxfId="19"/>
-    <tableColumn id="9" name="A:S" dataDxfId="18"/>
-    <tableColumn id="10" name="D" dataDxfId="17"/>
-    <tableColumn id="11" name="C" dataDxfId="16"/>
-    <tableColumn id="12" name="Notes: Server" dataDxfId="15"/>
+    <tableColumn id="1" name="Notes: Client" dataDxfId="40"/>
+    <tableColumn id="2" name="A:C" dataDxfId="39"/>
+    <tableColumn id="3" name="U" dataDxfId="38"/>
+    <tableColumn id="4" name="S" dataDxfId="37"/>
+    <tableColumn id="5" name="Use Case: Client" dataDxfId="36"/>
+    <tableColumn id="6" name="Conversation" dataDxfId="35"/>
+    <tableColumn id="8" name="Use Case: Server" dataDxfId="34"/>
+    <tableColumn id="13" name="G" dataDxfId="33"/>
+    <tableColumn id="9" name="A:S" dataDxfId="32"/>
+    <tableColumn id="10" name="D" dataDxfId="31"/>
+    <tableColumn id="11" name="C" dataDxfId="30"/>
+    <tableColumn id="12" name="Notes: Server" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:D21"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Type" dataDxfId="12"/>
-    <tableColumn id="6" name="Name" dataDxfId="11"/>
-    <tableColumn id="2" name="Messages" dataDxfId="10"/>
-    <tableColumn id="3" name="Collaborators" dataDxfId="9"/>
+    <tableColumn id="1" name="Type" dataDxfId="26"/>
+    <tableColumn id="6" name="Name" dataDxfId="25"/>
+    <tableColumn id="2" name="Messages" dataDxfId="24"/>
+    <tableColumn id="3" name="Collaborators" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:G25"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Name" dataDxfId="6"/>
-    <tableColumn id="7" name="Dependencies" dataDxfId="5"/>
-    <tableColumn id="6" name="Route" dataDxfId="4"/>
-    <tableColumn id="2" name="Controller" dataDxfId="3"/>
-    <tableColumn id="4" name="Directive" dataDxfId="2"/>
-    <tableColumn id="3" name="Factory" dataDxfId="1"/>
-    <tableColumn id="5" name="Service" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="20"/>
+    <tableColumn id="7" name="Dependencies" dataDxfId="19"/>
+    <tableColumn id="6" name="Route" dataDxfId="18"/>
+    <tableColumn id="2" name="Controller" dataDxfId="17"/>
+    <tableColumn id="4" name="Directive" dataDxfId="16"/>
+    <tableColumn id="3" name="Factory" dataDxfId="15"/>
+    <tableColumn id="5" name="Service" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project: Red" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4670,7 +4667,7 @@
   <dimension ref="B1:J46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4704,7 +4701,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
@@ -4766,7 +4763,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4777,7 +4774,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4881,7 +4878,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4892,7 +4889,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4902,7 +4899,9 @@
       <c r="C19" s="25">
         <v>1</v>
       </c>
-      <c r="D19" s="25"/>
+      <c r="D19" s="25" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="24" t="s">
@@ -4912,7 +4911,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4923,7 +4922,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4934,7 +4933,7 @@
         <v>5</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5090,7 +5089,7 @@
       </c>
       <c r="D39" s="27">
         <f>SUMIF(D2:D38,"&lt;&gt;",C2:C38)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
@@ -5160,7 +5159,7 @@
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="13"/>
       <c r="C4" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -5277,22 +5276,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B25:C1048576 B1:C21">
-    <cfRule type="expression" dxfId="106" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>$B1="Setup"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>$B1="CSS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>$B1="HTML"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>$B1="JS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>$B1="DB"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>$B1="PHP"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5354,7 +5353,7 @@
     </row>
     <row r="3" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>133</v>
@@ -5365,27 +5364,27 @@
     </row>
     <row r="4" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>133</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>133</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>137</v>
@@ -5393,7 +5392,7 @@
     </row>
     <row r="6" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>2</v>
@@ -5404,7 +5403,7 @@
     </row>
     <row r="7" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>2</v>
@@ -5448,13 +5447,13 @@
     </row>
     <row r="11" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>143</v>
@@ -5470,13 +5469,13 @@
     </row>
     <row r="13" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>136</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>196</v>
@@ -5503,7 +5502,7 @@
     </row>
     <row r="16" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>138</v>
@@ -5517,7 +5516,7 @@
         <v>136</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>256</v>
@@ -5525,7 +5524,7 @@
     </row>
     <row r="18" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>3</v>
@@ -5536,7 +5535,7 @@
     </row>
     <row r="19" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>3</v>
@@ -5547,7 +5546,7 @@
     </row>
     <row r="20" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>3</v>
@@ -5566,7 +5565,7 @@
     </row>
     <row r="22" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>3</v>
@@ -5613,7 +5612,7 @@
         <v>3</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>146</v>
@@ -5647,29 +5646,29 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="C1:E1048576">
-    <cfRule type="containsText" dxfId="67" priority="2" operator="containsText" text="CSS">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="CSS">
       <formula>NOT(ISERROR(SEARCH("CSS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="3" operator="containsText" text="HTML">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="HTML">
       <formula>NOT(ISERROR(SEARCH("HTML",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="4" operator="containsText" text="JS">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="JS">
       <formula>NOT(ISERROR(SEARCH("JS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="5" operator="containsText" text="DB">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="DB">
       <formula>NOT(ISERROR(SEARCH("DB",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="6" operator="containsText" text="PHP">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="PHP">
       <formula>NOT(ISERROR(SEARCH("PHP",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="containsText" dxfId="62" priority="1" operator="containsText" text="Setup">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Setup">
       <formula>NOT(ISERROR(SEARCH("Setup",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F1048576">
-    <cfRule type="expression" dxfId="61" priority="9">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>$B2="x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5731,7 +5730,7 @@
     </row>
     <row r="4" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>254</v>
@@ -5750,7 +5749,7 @@
     </row>
     <row r="6" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>260</v>
@@ -5793,7 +5792,7 @@
     </row>
     <row r="11" spans="2:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>267</v>
@@ -5860,7 +5859,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="53" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$C5="x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5888,7 +5887,7 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5912,31 +5911,31 @@
         <v>54</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>100</v>
-      </c>
       <c r="D1" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>97</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>98</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>121</v>
@@ -5967,7 +5966,7 @@
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>208</v>
@@ -5976,7 +5975,7 @@
         <v>209</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>115</v>
@@ -5988,7 +5987,7 @@
         <v>116</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>210</v>
@@ -6010,11 +6009,11 @@
         <v>155</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>156</v>
@@ -6055,20 +6054,20 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>220</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -6087,13 +6086,13 @@
         <v>40</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>206</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>198</v>
@@ -6102,11 +6101,9 @@
         <v>197</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="12" t="s">
         <v>222</v>
       </c>
+      <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
@@ -6119,14 +6116,14 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>220</v>
@@ -6149,22 +6146,22 @@
         <v>39</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>206</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>154</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
@@ -6179,20 +6176,20 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>221</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
@@ -6225,7 +6222,7 @@
       <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>276</v>
       </c>
@@ -6234,7 +6231,7 @@
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>221</v>
@@ -6246,13 +6243,13 @@
         <v>207</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>284</v>
+        <v>114</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
@@ -6264,12 +6261,12 @@
     </row>
     <row r="12" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>128</v>
@@ -6332,19 +6329,19 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -6361,19 +6358,19 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="12" t="s">
         <v>112</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>113</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
@@ -6390,12 +6387,12 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -6444,7 +6441,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -6452,7 +6449,7 @@
       <c r="E1" s="38"/>
       <c r="F1" s="10"/>
       <c r="G1" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H1" s="37"/>
       <c r="I1" s="37"/>
@@ -6462,31 +6459,31 @@
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>85</v>
-      </c>
       <c r="G2" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>47</v>
@@ -6495,78 +6492,78 @@
         <v>46</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>170</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>160</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>161</v>
@@ -6576,13 +6573,13 @@
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L5" s="7" t="s">
         <v>163</v>
@@ -6591,30 +6588,30 @@
     <row r="6" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>162</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L6" s="7" t="s">
         <v>163</v>
@@ -6623,43 +6620,43 @@
     <row r="7" spans="1:12" ht="210" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:12" ht="210" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>10</v>
@@ -6673,89 +6670,89 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>167</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>166</v>
@@ -6769,40 +6766,40 @@
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>168</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L12" s="7"/>
     </row>
@@ -6822,7 +6819,7 @@
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L13" s="7"/>
     </row>
@@ -6831,13 +6828,13 @@
         <v>173</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>172</v>
@@ -6851,23 +6848,23 @@
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>174</v>
@@ -6881,23 +6878,23 @@
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>175</v>
@@ -6911,10 +6908,10 @@
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L16" s="7"/>
     </row>
@@ -6931,23 +6928,23 @@
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>183</v>
@@ -6959,10 +6956,10 @@
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L18" s="7"/>
     </row>
@@ -8493,10 +8490,10 @@
         <v>195</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="30"/>
       <c r="F2" s="30"/>
@@ -8515,12 +8512,12 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="30"/>
       <c r="E4" s="30"/>
       <c r="F4" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G4" s="30"/>
     </row>
@@ -8532,7 +8529,7 @@
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
       <c r="G5" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -8543,7 +8540,7 @@
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -8551,13 +8548,13 @@
         <v>185</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
@@ -8567,13 +8564,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
@@ -8583,13 +8580,13 @@
         <v>194</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F9" s="30"/>
       <c r="G9" s="30"/>
@@ -8599,13 +8596,13 @@
         <v>186</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F10" s="30"/>
       <c r="G10" s="30"/>
@@ -8615,13 +8612,13 @@
         <v>36</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F11" s="30"/>
       <c r="G11" s="30"/>
@@ -8631,7 +8628,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
@@ -8639,10 +8636,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E13" s="30"/>
       <c r="F13" s="30"/>

</xml_diff>

<commit_message>
Labels and calendars now cached rather than called every time a modal is opened.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -516,7 +516,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="285">
   <si>
     <t>Design</t>
   </si>
@@ -1433,6 +1433,9 @@
   </si>
   <si>
     <t>Option to create labels and calendars when choosing category in edit task/event</t>
+  </si>
+  <si>
+    <t>Color belongs to calendar and label, NOT activities</t>
   </si>
 </sst>
 </file>
@@ -3432,7 +3435,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -4666,8 +4669,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4970,7 +4973,9 @@
       <c r="C26" s="25">
         <v>5</v>
       </c>
-      <c r="D26" s="25"/>
+      <c r="D26" s="25" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="27" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="24" t="s">
@@ -5089,7 +5094,7 @@
       </c>
       <c r="D39" s="27">
         <f>SUMIF(D2:D38,"&lt;&gt;",C2:C38)</f>
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
@@ -5694,10 +5699,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B2:D18"/>
+  <dimension ref="B2:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5758,7 +5763,10 @@
         <v>261</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
@@ -5774,7 +5782,10 @@
         <v>265</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="C9" s="4" t="s">
         <v>264</v>
       </c>
@@ -5801,7 +5812,10 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="C12" s="4" t="s">
         <v>269</v>
       </c>
@@ -5855,6 +5869,14 @@
       </c>
       <c r="D18" s="12" t="s">
         <v>283</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -5886,7 +5908,7 @@
   </sheetPr>
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Can now upload files to tasks.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -516,7 +516,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="291">
   <si>
     <t>Design</t>
   </si>
@@ -1436,6 +1436,24 @@
   </si>
   <si>
     <t>Color belongs to calendar and label, NOT activities</t>
+  </si>
+  <si>
+    <t>Events JS</t>
+  </si>
+  <si>
+    <t>Better display and handling of dates (like timezone compliant)</t>
+  </si>
+  <si>
+    <t>File Upload</t>
+  </si>
+  <si>
+    <t>Add support for non-images</t>
+  </si>
+  <si>
+    <t>attachment TEXT</t>
+  </si>
+  <si>
+    <t>Delete pre-existing file (given by target variable) before uploading</t>
   </si>
 </sst>
 </file>
@@ -4669,8 +4687,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5699,10 +5717,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B2:D19"/>
+  <dimension ref="B2:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5877,6 +5895,30 @@
       </c>
       <c r="D19" s="12" t="s">
         <v>284</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C20" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C22" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -5908,8 +5950,8 @@
   </sheetPr>
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6273,7 +6315,9 @@
       <c r="J11" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="K11" s="12"/>
+      <c r="K11" s="12" t="s">
+        <v>289</v>
+      </c>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
       <c r="N11" s="12"/>

</xml_diff>

<commit_message>
Subtasks converted to text in task table. Can now use subtasks.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -175,31 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Administrator:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Relative path; NOT absolute</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A12" authorId="1" shapeId="0">
+    <comment ref="A11" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -516,7 +492,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="292">
   <si>
     <t>Design</t>
   </si>
@@ -684,9 +660,6 @@
   </si>
   <si>
     <t>avatar TEXT</t>
-  </si>
-  <si>
-    <t>picture TEXT</t>
   </si>
   <si>
     <t>Optimistic Concurrency for multiple users editting data at same time</t>
@@ -795,9 +768,6 @@
     <t>label(id)</t>
   </si>
   <si>
-    <t>task(id)</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -847,9 +817,6 @@
   </si>
   <si>
     <t>label</t>
-  </si>
-  <si>
-    <t>subtask</t>
   </si>
   <si>
     <t>recurrence</t>
@@ -1455,12 +1422,24 @@
   <si>
     <t>Delete pre-existing file (given by target variable) before uploading</t>
   </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Subtasks</t>
+  </si>
+  <si>
+    <t>Make look nice in task modal</t>
+  </si>
+  <si>
+    <t>subtasks TEXT</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1529,6 +1508,19 @@
     <font>
       <sz val="11"/>
       <color rgb="FF404040"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1636,7 +1628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1748,6 +1740,14 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4346,8 +4346,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
-  <autoFilter ref="A1:Q15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q14" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+  <autoFilter ref="A1:Q14"/>
   <tableColumns count="17">
     <tableColumn id="1" name="Name" dataDxfId="59"/>
     <tableColumn id="2" name="Foreign Key1" dataDxfId="58"/>
@@ -4685,10 +4685,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:J46"/>
+  <dimension ref="B1:K46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4696,13 +4696,14 @@
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
     <col min="2" max="2" width="56.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="39"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
@@ -4710,11 +4711,12 @@
         <v>17</v>
       </c>
       <c r="D2" s="23"/>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="40"/>
+      <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="24" t="s">
         <v>49</v>
       </c>
@@ -4722,13 +4724,14 @@
         <v>5</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="41"/>
+      <c r="G3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="24" t="s">
         <v>20</v>
       </c>
@@ -4736,11 +4739,12 @@
         <v>2</v>
       </c>
       <c r="D4" s="25"/>
-      <c r="F4" t="s">
+      <c r="E4" s="41"/>
+      <c r="G4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="24" t="s">
         <v>32</v>
       </c>
@@ -4748,11 +4752,12 @@
         <v>5</v>
       </c>
       <c r="D5" s="25"/>
-      <c r="F5" t="s">
+      <c r="E5" s="41"/>
+      <c r="G5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24" t="s">
         <v>31</v>
       </c>
@@ -4760,11 +4765,12 @@
         <v>5</v>
       </c>
       <c r="D6" s="25"/>
-      <c r="F6" t="s">
+      <c r="E6" s="41"/>
+      <c r="G6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="26" t="s">
         <v>8</v>
       </c>
@@ -4772,11 +4778,12 @@
         <v>15</v>
       </c>
       <c r="D7" s="27"/>
-      <c r="F7" t="s">
+      <c r="E7" s="40"/>
+      <c r="G7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="24" t="s">
         <v>9</v>
       </c>
@@ -4784,10 +4791,11 @@
         <v>5</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="E8" s="41"/>
+    </row>
+    <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="24" t="s">
         <v>10</v>
       </c>
@@ -4795,10 +4803,11 @@
         <v>2</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="E9" s="41"/>
+    </row>
+    <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="24" t="s">
         <v>11</v>
       </c>
@@ -4806,8 +4815,9 @@
         <v>5</v>
       </c>
       <c r="D10" s="25"/>
-    </row>
-    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="41"/>
+    </row>
+    <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="24" t="s">
         <v>38</v>
       </c>
@@ -4815,23 +4825,26 @@
         <v>3</v>
       </c>
       <c r="D11" s="25"/>
-      <c r="F11" s="28" t="s">
+      <c r="E11" s="41" t="s">
+        <v>288</v>
+      </c>
+      <c r="G11" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="H11" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="I11" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="J11" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="K11" s="23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="26" t="s">
         <v>13</v>
       </c>
@@ -4839,23 +4852,24 @@
         <v>6</v>
       </c>
       <c r="D12" s="27"/>
-      <c r="F12" s="29" t="s">
+      <c r="E12" s="40"/>
+      <c r="G12" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="25">
+      <c r="H12" s="25">
         <v>84</v>
       </c>
-      <c r="H12" s="25">
+      <c r="I12" s="25">
         <v>74</v>
       </c>
-      <c r="I12" s="25">
+      <c r="J12" s="25">
         <v>64</v>
       </c>
-      <c r="J12" s="25" t="s">
+      <c r="K12" s="25" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="24" t="s">
         <v>14</v>
       </c>
@@ -4863,8 +4877,9 @@
         <v>1</v>
       </c>
       <c r="D13" s="25"/>
-    </row>
-    <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="41"/>
+    </row>
+    <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="24" t="s">
         <v>15</v>
       </c>
@@ -4872,8 +4887,9 @@
         <v>1</v>
       </c>
       <c r="D14" s="25"/>
-    </row>
-    <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="41"/>
+    </row>
+    <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="24" t="s">
         <v>16</v>
       </c>
@@ -4881,8 +4897,9 @@
         <v>4</v>
       </c>
       <c r="D15" s="25"/>
-    </row>
-    <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="41"/>
+    </row>
+    <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>25</v>
       </c>
@@ -4890,8 +4907,9 @@
         <v>24</v>
       </c>
       <c r="D16" s="27"/>
-    </row>
-    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="40"/>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="24" t="s">
         <v>42</v>
       </c>
@@ -4899,10 +4917,11 @@
         <v>5</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="E17" s="41"/>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="24" t="s">
         <v>24</v>
       </c>
@@ -4910,10 +4929,11 @@
         <v>1</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="E18" s="41"/>
+    </row>
+    <row r="19" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="24" t="s">
         <v>17</v>
       </c>
@@ -4921,10 +4941,11 @@
         <v>1</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="E19" s="41"/>
+    </row>
+    <row r="20" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="24" t="s">
         <v>21</v>
       </c>
@@ -4932,10 +4953,11 @@
         <v>1</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="E20" s="41"/>
+    </row>
+    <row r="21" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="24" t="s">
         <v>30</v>
       </c>
@@ -4943,10 +4965,11 @@
         <v>1</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="E21" s="41"/>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="24" t="s">
         <v>18</v>
       </c>
@@ -4954,19 +4977,23 @@
         <v>5</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="E22" s="41"/>
+    </row>
+    <row r="23" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="25">
         <v>5</v>
       </c>
-      <c r="D23" s="25"/>
-    </row>
-    <row r="24" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="41"/>
+    </row>
+    <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="24" t="s">
         <v>29</v>
       </c>
@@ -4974,8 +5001,9 @@
         <v>5</v>
       </c>
       <c r="D24" s="25"/>
-    </row>
-    <row r="25" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="41"/>
+    </row>
+    <row r="25" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="26" t="s">
         <v>5</v>
       </c>
@@ -4983,8 +5011,9 @@
         <v>18</v>
       </c>
       <c r="D25" s="27"/>
-    </row>
-    <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="40"/>
+    </row>
+    <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="24" t="s">
         <v>43</v>
       </c>
@@ -4992,10 +5021,11 @@
         <v>5</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="E26" s="41"/>
+    </row>
+    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="24" t="s">
         <v>33</v>
       </c>
@@ -5003,8 +5033,9 @@
         <v>5</v>
       </c>
       <c r="D27" s="25"/>
-    </row>
-    <row r="28" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="41"/>
+    </row>
+    <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="24" t="s">
         <v>12</v>
       </c>
@@ -5012,8 +5043,9 @@
         <v>5</v>
       </c>
       <c r="D28" s="25"/>
-    </row>
-    <row r="29" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="41"/>
+    </row>
+    <row r="29" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="24" t="s">
         <v>23</v>
       </c>
@@ -5021,8 +5053,9 @@
         <v>1</v>
       </c>
       <c r="D29" s="25"/>
-    </row>
-    <row r="30" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="41"/>
+    </row>
+    <row r="30" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="24" t="s">
         <v>22</v>
       </c>
@@ -5030,8 +5063,9 @@
         <v>2</v>
       </c>
       <c r="D30" s="25"/>
-    </row>
-    <row r="31" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E30" s="41"/>
+    </row>
+    <row r="31" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="26" t="s">
         <v>26</v>
       </c>
@@ -5039,8 +5073,9 @@
         <v>8</v>
       </c>
       <c r="D31" s="27"/>
-    </row>
-    <row r="32" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E31" s="40"/>
+    </row>
+    <row r="32" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="24" t="s">
         <v>27</v>
       </c>
@@ -5048,8 +5083,9 @@
         <v>5</v>
       </c>
       <c r="D32" s="25"/>
-    </row>
-    <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E32" s="41"/>
+    </row>
+    <row r="33" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="24" t="s">
         <v>28</v>
       </c>
@@ -5057,8 +5093,9 @@
         <v>3</v>
       </c>
       <c r="D33" s="25"/>
-    </row>
-    <row r="34" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="41"/>
+    </row>
+    <row r="34" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="26" t="s">
         <v>34</v>
       </c>
@@ -5066,8 +5103,9 @@
         <v>17</v>
       </c>
       <c r="D34" s="27"/>
-    </row>
-    <row r="35" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E34" s="40"/>
+    </row>
+    <row r="35" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="24" t="s">
         <v>7</v>
       </c>
@@ -5075,8 +5113,9 @@
         <v>4</v>
       </c>
       <c r="D35" s="25"/>
-    </row>
-    <row r="36" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E35" s="41"/>
+    </row>
+    <row r="36" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="24" t="s">
         <v>6</v>
       </c>
@@ -5084,8 +5123,9 @@
         <v>3</v>
       </c>
       <c r="D36" s="25"/>
-    </row>
-    <row r="37" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E36" s="41"/>
+    </row>
+    <row r="37" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="24" t="s">
         <v>41</v>
       </c>
@@ -5093,8 +5133,9 @@
         <v>5</v>
       </c>
       <c r="D37" s="25"/>
-    </row>
-    <row r="38" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E37" s="41"/>
+    </row>
+    <row r="38" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="24" t="s">
         <v>35</v>
       </c>
@@ -5102,8 +5143,9 @@
         <v>5</v>
       </c>
       <c r="D38" s="25"/>
-    </row>
-    <row r="39" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E38" s="41"/>
+    </row>
+    <row r="39" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="26" t="s">
         <v>37</v>
       </c>
@@ -5112,18 +5154,21 @@
       </c>
       <c r="D39" s="27">
         <f>SUMIF(D2:D38,"&lt;&gt;",C2:C38)</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E39" s="40"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="42"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
+      <c r="E46" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5167,7 +5212,7 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>36</v>
@@ -5175,26 +5220,26 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C3" s="18"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="13"/>
       <c r="C4" s="18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
       <c r="C5" s="18" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="13"/>
       <c r="C6" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -5206,31 +5251,31 @@
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
       <c r="C9" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C10" s="18"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
       <c r="C12" s="13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
@@ -5242,47 +5287,47 @@
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="13"/>
       <c r="C14" s="13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
       <c r="C16" s="13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="13"/>
       <c r="C17" s="18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="13"/>
       <c r="C18" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C19" s="18"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C20" s="18" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C21" s="18"/>
     </row>
@@ -5359,16 +5404,16 @@
   <sheetData>
     <row r="2" spans="2:6" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>36</v>
@@ -5376,63 +5421,63 @@
     </row>
     <row r="3" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>2</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -5440,10 +5485,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -5451,10 +5496,10 @@
         <v>2</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -5462,120 +5507,120 @@
         <v>2</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C12" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C14" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C15" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C17" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>3</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -5583,18 +5628,18 @@
         <v>3</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>3</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="60" x14ac:dyDescent="0.25">
@@ -5602,10 +5647,10 @@
         <v>3</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -5613,10 +5658,10 @@
         <v>3</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -5624,10 +5669,10 @@
         <v>3</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -5635,29 +5680,29 @@
         <v>3</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C27" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C28" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -5717,10 +5762,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B2:D22"/>
+  <dimension ref="B2:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5734,119 +5779,119 @@
   <sheetData>
     <row r="2" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C13" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
@@ -5854,23 +5899,23 @@
         <v>3</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C15" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
@@ -5878,46 +5923,54 @@
         <v>3</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="22" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="D22" s="12" t="s">
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>290</v>
       </c>
     </row>
@@ -5948,10 +6001,10 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5975,115 +6028,115 @@
         <v>54</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>97</v>
-      </c>
       <c r="K1" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="O1" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="L1" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="M1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="N1" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="O1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G2" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>113</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>116</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>55</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -6118,20 +6171,20 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -6150,22 +6203,22 @@
         <v>40</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -6180,17 +6233,17 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -6210,22 +6263,22 @@
         <v>39</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>56</v>
+        <v>291</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
@@ -6239,22 +6292,12 @@
       <c r="Q8" s="12"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>90</v>
-      </c>
+      <c r="A9" s="13"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="12"/>
-      <c r="D9" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>103</v>
-      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -6267,18 +6310,38 @@
       <c r="P9" s="12"/>
       <c r="Q9" s="12"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="12"/>
+    <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>202</v>
+      </c>
       <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
+      <c r="D10" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>286</v>
+      </c>
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
@@ -6288,98 +6351,88 @@
     </row>
     <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>205</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>221</v>
+        <v>125</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>153</v>
+        <v>115</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>207</v>
+        <v>116</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>100</v>
+        <v>208</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>114</v>
+        <v>209</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>289</v>
-      </c>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-    </row>
-    <row r="12" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>109</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="O11" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="P11" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q11" s="12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="N12" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="P12" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="Q12" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
+      <c r="D13" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>109</v>
+      </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
@@ -6395,19 +6448,19 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>88</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -6422,55 +6475,26 @@
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>129</v>
-      </c>
-      <c r="B20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6507,7 +6531,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -6515,7 +6539,7 @@
       <c r="E1" s="38"/>
       <c r="F1" s="10"/>
       <c r="G1" s="37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H1" s="37"/>
       <c r="I1" s="37"/>
@@ -6525,31 +6549,31 @@
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>84</v>
-      </c>
       <c r="G2" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>47</v>
@@ -6558,177 +6582,177 @@
         <v>46</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="210" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:12" ht="210" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>10</v>
@@ -6736,136 +6760,136 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L12" s="7"/>
     </row>
@@ -6876,108 +6900,108 @@
       <c r="D13" s="9"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E16" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>178</v>
-      </c>
       <c r="G16" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L16" s="7"/>
     </row>
@@ -6989,43 +7013,43 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L18" s="7"/>
     </row>
@@ -8325,82 +8349,82 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>54</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -8408,10 +8432,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -8419,10 +8443,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -8430,10 +8454,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -8441,10 +8465,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -8452,13 +8476,13 @@
         <v>3</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -8466,13 +8490,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>240</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -8480,10 +8504,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -8491,10 +8515,10 @@
         <v>3</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -8533,33 +8557,33 @@
         <v>54</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="30"/>
       <c r="F2" s="30"/>
@@ -8567,35 +8591,35 @@
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D3" s="30"/>
       <c r="E3" s="30" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="30"/>
       <c r="E4" s="30"/>
       <c r="F4" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="30"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D5" s="30"/>
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
       <c r="G5" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -8606,21 +8630,21 @@
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
@@ -8630,45 +8654,45 @@
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F9" s="30"/>
       <c r="G9" s="30"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" s="30"/>
       <c r="G10" s="30"/>
@@ -8678,13 +8702,13 @@
         <v>36</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F11" s="30"/>
       <c r="G11" s="30"/>
@@ -8694,7 +8718,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
@@ -8702,10 +8726,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" s="30"/>
       <c r="F13" s="30"/>

</xml_diff>

<commit_message>
DifDifferent task pages (inbox, today, week) added.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -492,7 +492,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="297">
   <si>
     <t>Design</t>
   </si>
@@ -844,9 +844,6 @@
   </si>
   <si>
     <t>week_start ENUM('su', 'mo') DEFAULT 'so'</t>
-  </si>
-  <si>
-    <t>until DATETIME</t>
   </si>
   <si>
     <t>count INT</t>
@@ -1433,6 +1430,24 @@
   </si>
   <si>
     <t>subtasks TEXT</t>
+  </si>
+  <si>
+    <t>recurrence BOOL</t>
+  </si>
+  <si>
+    <t>Recurrence</t>
+  </si>
+  <si>
+    <t>Support by_set_pos</t>
+  </si>
+  <si>
+    <t>until DATE</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Recurrence changes are saved regardless of if submit is clicked or not</t>
   </si>
 </sst>
 </file>
@@ -4687,8 +4702,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:K46"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4738,7 +4753,9 @@
       <c r="C4" s="25">
         <v>2</v>
       </c>
-      <c r="D4" s="25"/>
+      <c r="D4" s="25" t="s">
+        <v>295</v>
+      </c>
       <c r="E4" s="41"/>
       <c r="G4" t="s">
         <v>51</v>
@@ -4751,7 +4768,9 @@
       <c r="C5" s="25">
         <v>5</v>
       </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="25" t="s">
+        <v>62</v>
+      </c>
       <c r="E5" s="41"/>
       <c r="G5" t="s">
         <v>52</v>
@@ -4764,7 +4783,9 @@
       <c r="C6" s="25">
         <v>5</v>
       </c>
-      <c r="D6" s="25"/>
+      <c r="D6" s="25" t="s">
+        <v>287</v>
+      </c>
       <c r="E6" s="41"/>
       <c r="G6" t="s">
         <v>3</v>
@@ -4814,7 +4835,9 @@
       <c r="C10" s="25">
         <v>5</v>
       </c>
-      <c r="D10" s="25"/>
+      <c r="D10" s="25" t="s">
+        <v>295</v>
+      </c>
       <c r="E10" s="41"/>
     </row>
     <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4824,10 +4847,10 @@
       <c r="C11" s="25">
         <v>3</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="41" t="s">
-        <v>288</v>
-      </c>
+      <c r="D11" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="41"/>
       <c r="G11" s="28" t="s">
         <v>44</v>
       </c>
@@ -4876,7 +4899,9 @@
       <c r="C13" s="25">
         <v>1</v>
       </c>
-      <c r="D13" s="25"/>
+      <c r="D13" s="25" t="s">
+        <v>295</v>
+      </c>
       <c r="E13" s="41"/>
     </row>
     <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4886,7 +4911,9 @@
       <c r="C14" s="25">
         <v>1</v>
       </c>
-      <c r="D14" s="25"/>
+      <c r="D14" s="25" t="s">
+        <v>295</v>
+      </c>
       <c r="E14" s="41"/>
     </row>
     <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4896,7 +4923,9 @@
       <c r="C15" s="25">
         <v>4</v>
       </c>
-      <c r="D15" s="25"/>
+      <c r="D15" s="25" t="s">
+        <v>295</v>
+      </c>
       <c r="E15" s="41"/>
     </row>
     <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5000,7 +5029,9 @@
       <c r="C24" s="25">
         <v>5</v>
       </c>
-      <c r="D24" s="25"/>
+      <c r="D24" s="25" t="s">
+        <v>62</v>
+      </c>
       <c r="E24" s="41"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5042,7 +5073,9 @@
       <c r="C28" s="25">
         <v>5</v>
       </c>
-      <c r="D28" s="25"/>
+      <c r="D28" s="25" t="s">
+        <v>295</v>
+      </c>
       <c r="E28" s="41"/>
     </row>
     <row r="29" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5052,7 +5085,9 @@
       <c r="C29" s="25">
         <v>1</v>
       </c>
-      <c r="D29" s="25"/>
+      <c r="D29" s="25" t="s">
+        <v>295</v>
+      </c>
       <c r="E29" s="41"/>
     </row>
     <row r="30" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5062,7 +5097,9 @@
       <c r="C30" s="25">
         <v>2</v>
       </c>
-      <c r="D30" s="25"/>
+      <c r="D30" s="25" t="s">
+        <v>295</v>
+      </c>
       <c r="E30" s="41"/>
     </row>
     <row r="31" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5082,7 +5119,9 @@
       <c r="C32" s="25">
         <v>5</v>
       </c>
-      <c r="D32" s="25"/>
+      <c r="D32" s="25" t="s">
+        <v>295</v>
+      </c>
       <c r="E32" s="41"/>
     </row>
     <row r="33" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5092,7 +5131,9 @@
       <c r="C33" s="25">
         <v>3</v>
       </c>
-      <c r="D33" s="25"/>
+      <c r="D33" s="25" t="s">
+        <v>295</v>
+      </c>
       <c r="E33" s="41"/>
     </row>
     <row r="34" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5112,7 +5153,9 @@
       <c r="C35" s="25">
         <v>4</v>
       </c>
-      <c r="D35" s="25"/>
+      <c r="D35" s="25" t="s">
+        <v>295</v>
+      </c>
       <c r="E35" s="41"/>
     </row>
     <row r="36" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5122,7 +5165,9 @@
       <c r="C36" s="25">
         <v>3</v>
       </c>
-      <c r="D36" s="25"/>
+      <c r="D36" s="25" t="s">
+        <v>295</v>
+      </c>
       <c r="E36" s="41"/>
     </row>
     <row r="37" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5132,7 +5177,9 @@
       <c r="C37" s="25">
         <v>5</v>
       </c>
-      <c r="D37" s="25"/>
+      <c r="D37" s="25" t="s">
+        <v>295</v>
+      </c>
       <c r="E37" s="41"/>
     </row>
     <row r="38" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5142,7 +5189,9 @@
       <c r="C38" s="25">
         <v>5</v>
       </c>
-      <c r="D38" s="25"/>
+      <c r="D38" s="25" t="s">
+        <v>287</v>
+      </c>
       <c r="E38" s="41"/>
     </row>
     <row r="39" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5153,8 +5202,8 @@
         <v>105</v>
       </c>
       <c r="D39" s="27">
-        <f>SUMIF(D2:D38,"&lt;&gt;",C2:C38)</f>
-        <v>36</v>
+        <f>SUMIF(D2:D38,"x",C2:C38)</f>
+        <v>49</v>
       </c>
       <c r="E39" s="40"/>
     </row>
@@ -5212,7 +5261,7 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>36</v>
@@ -5220,7 +5269,7 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C3" s="18"/>
     </row>
@@ -5233,13 +5282,13 @@
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
       <c r="C5" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="13"/>
       <c r="C6" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -5251,31 +5300,31 @@
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
       <c r="C9" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C10" s="18"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
       <c r="C12" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
@@ -5287,47 +5336,47 @@
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="13"/>
       <c r="C14" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
       <c r="C16" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="13"/>
       <c r="C17" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="13"/>
       <c r="C18" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C19" s="18"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C20" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C21" s="18"/>
     </row>
@@ -5404,16 +5453,16 @@
   <sheetData>
     <row r="2" spans="2:6" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>129</v>
-      </c>
       <c r="D2" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>36</v>
@@ -5424,10 +5473,10 @@
         <v>62</v>
       </c>
       <c r="C3" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>130</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5435,7 +5484,7 @@
         <v>62</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>62</v>
@@ -5449,13 +5498,13 @@
         <v>62</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>62</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5466,7 +5515,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5477,7 +5526,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -5485,10 +5534,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -5496,10 +5545,10 @@
         <v>2</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -5507,10 +5556,10 @@
         <v>2</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5524,15 +5573,15 @@
         <v>62</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C12" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5540,32 +5589,32 @@
         <v>62</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>62</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C14" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C15" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5573,21 +5622,21 @@
         <v>62</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C17" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>62</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5598,7 +5647,7 @@
         <v>3</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5609,7 +5658,7 @@
         <v>3</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5620,7 +5669,7 @@
         <v>3</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -5628,7 +5677,7 @@
         <v>3</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5639,7 +5688,7 @@
         <v>3</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="60" x14ac:dyDescent="0.25">
@@ -5647,10 +5696,10 @@
         <v>3</v>
       </c>
       <c r="D23" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="F23" s="16" t="s">
         <v>200</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -5658,10 +5707,10 @@
         <v>3</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -5669,10 +5718,10 @@
         <v>3</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -5683,26 +5732,26 @@
         <v>62</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C27" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C28" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -5762,10 +5811,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B2:D23"/>
+  <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5779,21 +5828,21 @@
   <sheetData>
     <row r="2" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>247</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>249</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5801,18 +5850,18 @@
         <v>62</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>251</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>255</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5820,10 +5869,10 @@
         <v>62</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>257</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="7" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
@@ -5834,15 +5883,15 @@
         <v>3</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>261</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="9" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
@@ -5850,18 +5899,18 @@
         <v>62</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -5869,10 +5918,10 @@
         <v>62</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>264</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5880,18 +5929,18 @@
         <v>62</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>266</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C13" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>268</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
@@ -5899,23 +5948,23 @@
         <v>3</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C15" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>271</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>275</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
@@ -5923,55 +5972,71 @@
         <v>3</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>282</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>284</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="22" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>289</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>290</v>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C25" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -6003,8 +6068,8 @@
   </sheetPr>
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6055,30 +6120,30 @@
         <v>95</v>
       </c>
       <c r="K1" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="O1" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="O1" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>123</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -6086,10 +6151,10 @@
         <v>85</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>205</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>206</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>110</v>
@@ -6107,23 +6172,23 @@
         <v>55</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M2" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="N2" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>178</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>179</v>
       </c>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>86</v>
@@ -6133,10 +6198,10 @@
         <v>85</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>153</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>154</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -6181,7 +6246,7 @@
         <v>85</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>103</v>
@@ -6206,19 +6271,19 @@
         <v>87</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>85</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -6243,7 +6308,7 @@
         <v>85</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -6266,19 +6331,19 @@
         <v>88</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>85</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>101</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
@@ -6312,23 +6377,23 @@
     </row>
     <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12" t="s">
         <v>85</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>100</v>
@@ -6340,9 +6405,11 @@
         <v>111</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="L10" s="12"/>
+        <v>285</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>291</v>
+      </c>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
@@ -6359,43 +6426,43 @@
         <v>85</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F11" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="H11" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>117</v>
-      </c>
       <c r="I11" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="J11" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="K11" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="L11" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="M11" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="M11" s="12" t="s">
+      <c r="N11" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="N11" s="12" t="s">
+      <c r="O11" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="O11" s="12" t="s">
+      <c r="P11" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="P11" s="12" t="s">
+      <c r="Q11" s="12" t="s">
         <v>215</v>
-      </c>
-      <c r="Q11" s="12" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -6487,10 +6554,10 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" t="s">
         <v>126</v>
-      </c>
-      <c r="B19" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -6600,7 +6667,7 @@
         <v>67</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>67</v>
@@ -6630,7 +6697,7 @@
         <v>71</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>70</v>
@@ -6656,10 +6723,10 @@
         <v>78</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9" t="s">
@@ -6672,7 +6739,7 @@
         <v>62</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -6688,7 +6755,7 @@
         <v>79</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>79</v>
@@ -6704,7 +6771,7 @@
         <v>62</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="210" x14ac:dyDescent="0.25">
@@ -6752,7 +6819,7 @@
         <v>10</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>10</v>
@@ -6818,7 +6885,7 @@
         <v>69</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>69</v>
@@ -6845,13 +6912,13 @@
         <v>62</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F11" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>162</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -6878,7 +6945,7 @@
         <v>68</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>68</v>
@@ -6900,10 +6967,10 @@
       <c r="D13" s="9"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -6915,7 +6982,7 @@
     </row>
     <row r="14" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>62</v>
@@ -6927,13 +6994,13 @@
         <v>62</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -6957,13 +7024,13 @@
         <v>62</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
@@ -6987,13 +7054,13 @@
         <v>62</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -7013,7 +7080,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
@@ -7037,11 +7104,11 @@
         <v>62</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -8349,82 +8416,82 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>54</v>
       </c>
       <c r="C1" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1" s="33" t="s">
         <v>222</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -8432,10 +8499,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -8443,10 +8510,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -8454,10 +8521,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -8465,10 +8532,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -8476,13 +8543,13 @@
         <v>3</v>
       </c>
       <c r="B12" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="C12" s="31" t="s">
         <v>229</v>
       </c>
-      <c r="C12" s="31" t="s">
-        <v>230</v>
-      </c>
       <c r="D12" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -8490,13 +8557,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -8504,10 +8571,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -8515,10 +8582,10 @@
         <v>3</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -8557,27 +8624,27 @@
         <v>54</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>186</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>58</v>
@@ -8591,11 +8658,11 @@
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D3" s="30"/>
       <c r="E3" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
@@ -8613,7 +8680,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D5" s="30"/>
       <c r="E5" s="30"/>
@@ -8635,7 +8702,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>58</v>
@@ -8667,7 +8734,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>58</v>
@@ -8683,7 +8750,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
Paper finished and some code clean up.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -492,23 +492,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="297">
   <si>
     <t>Design</t>
   </si>
   <si>
-    <t>Languages</t>
-  </si>
-  <si>
     <t>HTML</t>
   </si>
   <si>
     <t>PHP</t>
   </si>
   <si>
-    <t>MySQL</t>
-  </si>
-  <si>
     <t>Calendar</t>
   </si>
   <si>
@@ -645,12 +639,6 @@
   </si>
   <si>
     <t>&lt; 64</t>
-  </si>
-  <si>
-    <t>CSS (SASS)</t>
-  </si>
-  <si>
-    <t>JavaScript + jQuery</t>
   </si>
   <si>
     <t xml:space="preserve"> &gt;= 94</t>
@@ -1448,6 +1436,18 @@
   </si>
   <si>
     <t>Recurrence changes are saved regardless of if submit is clicked or not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other </t>
+  </si>
+  <si>
+    <t>Sanitize input</t>
+  </si>
+  <si>
+    <t>cacheService to share the activities between main controller and directives</t>
+  </si>
+  <si>
+    <t>"all" query</t>
   </si>
 </sst>
 </file>
@@ -1749,12 +1749,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1763,6 +1757,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3175,7 +3175,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -3319,7 +3319,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -3385,14 +3385,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>514350</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
       <mc:Choice Requires="sle15">
@@ -4324,8 +4324,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F30" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
-  <autoFilter ref="B2:F30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F32" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
+  <autoFilter ref="B2:F32">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
@@ -4700,10 +4700,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:K46"/>
+  <dimension ref="B1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4711,14 +4711,15 @@
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
     <col min="2" max="2" width="56.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="39"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="37"/>
+    <col min="6" max="6" width="43" style="37" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
@@ -4726,477 +4727,499 @@
         <v>17</v>
       </c>
       <c r="D2" s="23"/>
-      <c r="E2" s="40"/>
-      <c r="G2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="38"/>
+      <c r="F2" s="22" t="s">
+        <v>293</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C3" s="25">
         <v>5</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="41"/>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E3" s="39"/>
+      <c r="F3" s="24" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="25">
         <v>2</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="E4" s="41"/>
-      <c r="G4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+      <c r="E4" s="39"/>
+      <c r="F4" s="24"/>
+    </row>
+    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" s="25">
         <v>5</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="41"/>
-      <c r="G5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E5" s="39"/>
+      <c r="F5" s="24"/>
+    </row>
+    <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="25">
         <v>5</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>287</v>
-      </c>
-      <c r="E6" s="41"/>
-      <c r="G6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>283</v>
+      </c>
+      <c r="E6" s="39"/>
+      <c r="F6" s="24"/>
+    </row>
+    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="26" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" s="27">
         <v>15</v>
       </c>
       <c r="D7" s="27"/>
-      <c r="E7" s="40"/>
-      <c r="G7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+    </row>
+    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" s="25">
         <v>5</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="41"/>
-    </row>
-    <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+    </row>
+    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="25">
         <v>2</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="41"/>
-    </row>
-    <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+    </row>
+    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" s="25">
         <v>5</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="E10" s="41"/>
-    </row>
-    <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+    </row>
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" s="25">
         <v>3</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="41"/>
-      <c r="G11" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="H11" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="K11" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="L11" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="K11" s="23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12" s="27">
         <v>6</v>
       </c>
       <c r="D12" s="27"/>
-      <c r="E12" s="40"/>
-      <c r="G12" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="25">
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="H12" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="25">
         <v>84</v>
       </c>
-      <c r="I12" s="25">
+      <c r="J12" s="25">
         <v>74</v>
       </c>
-      <c r="J12" s="25">
+      <c r="K12" s="25">
         <v>64</v>
       </c>
-      <c r="K12" s="25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L12" s="25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13" s="25">
         <v>1</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="E13" s="41"/>
-    </row>
-    <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+    </row>
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="25">
         <v>1</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="E14" s="41"/>
-    </row>
-    <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+    </row>
+    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="24" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" s="25">
         <v>4</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="E15" s="41"/>
-    </row>
-    <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+    </row>
+    <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" s="27">
         <v>24</v>
       </c>
       <c r="D16" s="27"/>
-      <c r="E16" s="40"/>
-    </row>
-    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+    </row>
+    <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17" s="25">
         <v>5</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="41"/>
-    </row>
-    <row r="18" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+    </row>
+    <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" s="25">
         <v>1</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="41"/>
-    </row>
-    <row r="19" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+    </row>
+    <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C19" s="25">
         <v>1</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="41"/>
-    </row>
-    <row r="20" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+    </row>
+    <row r="20" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" s="25">
         <v>1</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="41"/>
-    </row>
-    <row r="21" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+    </row>
+    <row r="21" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C21" s="25">
         <v>1</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="41"/>
-    </row>
-    <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+    </row>
+    <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="24" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C22" s="25">
         <v>5</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" s="41"/>
-    </row>
-    <row r="23" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+    </row>
+    <row r="23" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C23" s="25">
         <v>5</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="41"/>
-    </row>
-    <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C24" s="25">
         <v>5</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" s="41"/>
-    </row>
-    <row r="25" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+    </row>
+    <row r="25" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="26" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C25" s="27">
         <v>18</v>
       </c>
       <c r="D25" s="27"/>
-      <c r="E25" s="40"/>
-    </row>
-    <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+    </row>
+    <row r="26" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C26" s="25">
         <v>5</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E26" s="41"/>
-    </row>
-    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+    </row>
+    <row r="27" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C27" s="25">
         <v>5</v>
       </c>
       <c r="D27" s="25"/>
-      <c r="E27" s="41"/>
-    </row>
-    <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+    </row>
+    <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C28" s="25">
         <v>5</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="E28" s="41"/>
-    </row>
-    <row r="29" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+    </row>
+    <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C29" s="25">
         <v>1</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="E29" s="41"/>
-    </row>
-    <row r="30" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+    </row>
+    <row r="30" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C30" s="25">
         <v>2</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="E30" s="41"/>
-    </row>
-    <row r="31" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+    </row>
+    <row r="31" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C31" s="27">
         <v>8</v>
       </c>
       <c r="D31" s="27"/>
-      <c r="E31" s="40"/>
-    </row>
-    <row r="32" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+    </row>
+    <row r="32" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C32" s="25">
         <v>5</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="E32" s="41"/>
-    </row>
-    <row r="33" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+    </row>
+    <row r="33" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C33" s="25">
         <v>3</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="E33" s="41"/>
-    </row>
-    <row r="34" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+    </row>
+    <row r="34" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C34" s="27">
         <v>17</v>
       </c>
       <c r="D34" s="27"/>
-      <c r="E34" s="40"/>
-    </row>
-    <row r="35" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+    </row>
+    <row r="35" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C35" s="25">
         <v>4</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="E35" s="41"/>
-    </row>
-    <row r="36" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+    </row>
+    <row r="36" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="24" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C36" s="25">
         <v>3</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="E36" s="41"/>
-    </row>
-    <row r="37" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+    </row>
+    <row r="37" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C37" s="25">
         <v>5</v>
       </c>
-      <c r="D37" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="E37" s="41"/>
-    </row>
-    <row r="38" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="25"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+    </row>
+    <row r="38" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C38" s="25">
         <v>5</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>287</v>
-      </c>
-      <c r="E38" s="41"/>
-    </row>
-    <row r="39" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>283</v>
+      </c>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+    </row>
+    <row r="39" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C39" s="27">
         <v>105</v>
@@ -5205,19 +5228,22 @@
         <f>SUMIF(D2:D38,"x",C2:C38)</f>
         <v>49</v>
       </c>
-      <c r="E39" s="40"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="42"/>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="42"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5261,122 +5287,122 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C3" s="18"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="13"/>
       <c r="C4" s="18" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
       <c r="C5" s="18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="13"/>
       <c r="C6" s="13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="18"/>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
       <c r="C9" s="13" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C10" s="18"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
       <c r="C12" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="13"/>
       <c r="C14" s="13" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="13" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
       <c r="C16" s="13" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="13"/>
       <c r="C17" s="18" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="13"/>
       <c r="C18" s="13" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C19" s="18"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C20" s="18" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C21" s="18"/>
     </row>
@@ -5430,10 +5456,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="B2:F30"/>
+  <dimension ref="B2:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5453,312 +5479,355 @@
   <sheetData>
     <row r="2" spans="2:6" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C5" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>129</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="6" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C9" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C10" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C12" s="15" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C14" s="15" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C15" s="15" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C17" s="15" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C21" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C23" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C24" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C25" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C26" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C27" s="15" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C28" s="15" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F29" s="16"/>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C29" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F30" s="16"/>
+      <c r="C30" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="16"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="16"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -5828,215 +5897,215 @@
   <sheetData>
     <row r="2" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C13" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C14" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C15" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="25" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C25" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>292</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -6069,7 +6138,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6090,118 +6159,118 @@
   <sheetData>
     <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>95</v>
-      </c>
       <c r="K1" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="N1" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="O1" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="P1" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="G2" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>114</v>
-      </c>
       <c r="J2" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -6236,20 +6305,20 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -6265,25 +6334,25 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -6298,17 +6367,17 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -6325,25 +6394,25 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
@@ -6377,38 +6446,38 @@
     </row>
     <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
@@ -6418,51 +6487,51 @@
     </row>
     <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I11" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="M11" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="N11" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="O11" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="P11" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="M11" s="12" t="s">
+      <c r="Q11" s="12" t="s">
         <v>211</v>
-      </c>
-      <c r="N11" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="O11" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="P11" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="Q11" s="12" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -6486,19 +6555,19 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
@@ -6515,19 +6584,19 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -6544,20 +6613,20 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -6597,366 +6666,366 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="A1" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
       <c r="F1" s="10"/>
-      <c r="G1" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
+      <c r="G1" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="210" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:12" ht="210" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L12" s="7"/>
     </row>
@@ -6967,108 +7036,108 @@
       <c r="D13" s="9"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>173</v>
-      </c>
       <c r="G14" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L16" s="7"/>
     </row>
@@ -7080,43 +7149,43 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L18" s="7"/>
     </row>
@@ -8416,176 +8485,176 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -8621,36 +8690,36 @@
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E2" s="30"/>
       <c r="F2" s="30"/>
@@ -8658,134 +8727,134 @@
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D3" s="30"/>
       <c r="E3" s="30" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D4" s="30"/>
       <c r="E4" s="30"/>
       <c r="F4" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G4" s="30"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D5" s="30"/>
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
       <c r="G5" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F9" s="30"/>
       <c r="G9" s="30"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F10" s="30"/>
       <c r="G10" s="30"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F11" s="30"/>
       <c r="G11" s="30"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
@@ -8793,10 +8862,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E13" s="30"/>
       <c r="F13" s="30"/>

</xml_diff>

<commit_message>
Paper and notes updated. Don't remember what with.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -492,7 +492,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="300">
   <si>
     <t>Design</t>
   </si>
@@ -1441,13 +1441,22 @@
     <t xml:space="preserve">Other </t>
   </si>
   <si>
-    <t>Sanitize input</t>
-  </si>
-  <si>
     <t>cacheService to share the activities between main controller and directives</t>
   </si>
   <si>
-    <t>"all" query</t>
+    <t>"all" query: separated into subgroups</t>
+  </si>
+  <si>
+    <t>Sanitize input/files</t>
+  </si>
+  <si>
+    <t>Labels and calendars</t>
+  </si>
+  <si>
+    <t>If error on query, create object in vm.x under x.summary that displays error message</t>
+  </si>
+  <si>
+    <t>start and get session user id on query in php to reduce api calls</t>
   </si>
 </sst>
 </file>
@@ -3391,8 +3400,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
       <mc:Choice Requires="sle15">
@@ -4324,8 +4333,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F32" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
-  <autoFilter ref="B2:F32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F36" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
+  <autoFilter ref="B2:F36">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
@@ -4702,8 +4711,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:L46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4745,7 +4754,7 @@
       </c>
       <c r="E3" s="39"/>
       <c r="F3" s="24" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4759,7 +4768,9 @@
         <v>291</v>
       </c>
       <c r="E4" s="39"/>
-      <c r="F4" s="24"/>
+      <c r="F4" s="24" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="24" t="s">
@@ -5456,10 +5467,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="B2:F32"/>
+  <dimension ref="B2:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5812,7 +5823,7 @@
         <v>128</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -5820,14 +5831,36 @@
         <v>2</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F31" s="16"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F32" s="16"/>
+      <c r="C31" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C32" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="16"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="16"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="16"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="16"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>

<commit_message>
Admin page added that can CRUD users. Bug fixes.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -492,7 +492,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="299">
   <si>
     <t>Design</t>
   </si>
@@ -1430,9 +1430,6 @@
   </si>
   <si>
     <t>until DATE</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Recurrence changes are saved regardless of if submit is clicked or not</t>
@@ -1778,130 +1775,6 @@
   </cellStyles>
   <dxfs count="125">
     <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2116,6 +1989,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2137,6 +2015,68 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2234,6 +2174,63 @@
     </dxf>
     <dxf>
       <alignment vertical="top" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3184,7 +3181,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -3256,8 +3253,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>333375</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
       <mc:Choice Requires="sle15">
@@ -3322,13 +3319,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -3394,14 +3391,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>323850</xdr:rowOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
       <mc:Choice Requires="sle15">
@@ -3478,7 +3475,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:rowOff>342901</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
       <mc:Choice Requires="sle15">
@@ -3858,46 +3855,6 @@
     <i/>
   </colItems>
   <formats count="33">
-    <format dxfId="106">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="105">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="104">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="103">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="102">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="101">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
-    </format>
     <format dxfId="100">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
@@ -3913,6 +3870,46 @@
       </pivotArea>
     </format>
     <format dxfId="99">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="98">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="97">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="96">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="95">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="94">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="93">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3926,7 +3923,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="98">
+    <format dxfId="92">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3939,7 +3936,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="97">
+    <format dxfId="91">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3952,7 +3949,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="96">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3968,7 +3965,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="95">
+    <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3980,7 +3977,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="94">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3992,16 +3989,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="93">
+    <format dxfId="87">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="92">
+    <format dxfId="86">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="91">
+    <format dxfId="85">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="90">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -4015,7 +4012,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="83">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4029,7 +4026,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4042,7 +4039,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="81">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4055,7 +4052,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="80">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4071,7 +4068,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="79">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4083,7 +4080,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="84">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4095,10 +4092,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="77">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="82">
+    <format dxfId="76">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4107,7 +4104,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="75">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4116,7 +4113,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="74">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4125,7 +4122,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="73">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4134,7 +4131,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="72">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4143,7 +4140,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="71">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4155,7 +4152,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="70">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4168,7 +4165,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="69">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4181,7 +4178,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="68">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4333,7 +4330,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F36" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F36" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="B2:F36">
     <filterColumn colId="0">
       <filters blank="1"/>
@@ -4343,103 +4340,103 @@
     <sortCondition ref="C2:C30"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Done" dataDxfId="71"/>
-    <tableColumn id="3" name="Category" dataDxfId="70"/>
-    <tableColumn id="5" name="Remember" dataDxfId="69"/>
-    <tableColumn id="4" name="Look Into" dataDxfId="68"/>
-    <tableColumn id="2" name="Task" dataDxfId="67"/>
+    <tableColumn id="1" name="Done" dataDxfId="58"/>
+    <tableColumn id="3" name="Category" dataDxfId="57"/>
+    <tableColumn id="5" name="Remember" dataDxfId="56"/>
+    <tableColumn id="4" name="Look Into" dataDxfId="55"/>
+    <tableColumn id="2" name="Task" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:D31" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:D31" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="B2:D31">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="Done" dataDxfId="64"/>
-    <tableColumn id="2" name="File" dataDxfId="63"/>
-    <tableColumn id="3" name="Feature" dataDxfId="62"/>
+    <tableColumn id="1" name="Done" dataDxfId="50"/>
+    <tableColumn id="2" name="File" dataDxfId="49"/>
+    <tableColumn id="3" name="Feature" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q14" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q14" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A1:Q14"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Name" dataDxfId="59"/>
-    <tableColumn id="2" name="Foreign Key1" dataDxfId="58"/>
-    <tableColumn id="3" name="Foreign Key2" dataDxfId="57"/>
-    <tableColumn id="4" name="Column1" dataDxfId="56"/>
-    <tableColumn id="5" name="Column2" dataDxfId="55"/>
-    <tableColumn id="6" name="Column3" dataDxfId="54"/>
-    <tableColumn id="7" name="Column4" dataDxfId="53"/>
-    <tableColumn id="8" name="Column5" dataDxfId="52"/>
-    <tableColumn id="9" name="Column6" dataDxfId="51"/>
-    <tableColumn id="13" name="Column7" dataDxfId="50"/>
-    <tableColumn id="12" name="Column8" dataDxfId="49"/>
-    <tableColumn id="11" name="Column9" dataDxfId="48"/>
-    <tableColumn id="17" name="Column10" dataDxfId="47"/>
-    <tableColumn id="16" name="Column11" dataDxfId="46"/>
-    <tableColumn id="15" name="Column12" dataDxfId="45"/>
-    <tableColumn id="14" name="Column13" dataDxfId="44"/>
-    <tableColumn id="10" name="Column14" dataDxfId="43"/>
+    <tableColumn id="1" name="Name" dataDxfId="45"/>
+    <tableColumn id="2" name="Foreign Key1" dataDxfId="44"/>
+    <tableColumn id="3" name="Foreign Key2" dataDxfId="43"/>
+    <tableColumn id="4" name="Column1" dataDxfId="42"/>
+    <tableColumn id="5" name="Column2" dataDxfId="41"/>
+    <tableColumn id="6" name="Column3" dataDxfId="40"/>
+    <tableColumn id="7" name="Column4" dataDxfId="39"/>
+    <tableColumn id="8" name="Column5" dataDxfId="38"/>
+    <tableColumn id="9" name="Column6" dataDxfId="37"/>
+    <tableColumn id="13" name="Column7" dataDxfId="36"/>
+    <tableColumn id="12" name="Column8" dataDxfId="35"/>
+    <tableColumn id="11" name="Column9" dataDxfId="34"/>
+    <tableColumn id="17" name="Column10" dataDxfId="33"/>
+    <tableColumn id="16" name="Column11" dataDxfId="32"/>
+    <tableColumn id="15" name="Column12" dataDxfId="31"/>
+    <tableColumn id="14" name="Column13" dataDxfId="30"/>
+    <tableColumn id="10" name="Column14" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A2:L108"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Notes: Client" dataDxfId="40"/>
-    <tableColumn id="2" name="A:C" dataDxfId="39"/>
-    <tableColumn id="3" name="U" dataDxfId="38"/>
-    <tableColumn id="4" name="S" dataDxfId="37"/>
-    <tableColumn id="5" name="Use Case: Client" dataDxfId="36"/>
-    <tableColumn id="6" name="Conversation" dataDxfId="35"/>
-    <tableColumn id="8" name="Use Case: Server" dataDxfId="34"/>
-    <tableColumn id="13" name="G" dataDxfId="33"/>
-    <tableColumn id="9" name="A:S" dataDxfId="32"/>
-    <tableColumn id="10" name="D" dataDxfId="31"/>
-    <tableColumn id="11" name="C" dataDxfId="30"/>
-    <tableColumn id="12" name="Notes: Server" dataDxfId="29"/>
+    <tableColumn id="1" name="Notes: Client" dataDxfId="26"/>
+    <tableColumn id="2" name="A:C" dataDxfId="25"/>
+    <tableColumn id="3" name="U" dataDxfId="24"/>
+    <tableColumn id="4" name="S" dataDxfId="23"/>
+    <tableColumn id="5" name="Use Case: Client" dataDxfId="22"/>
+    <tableColumn id="6" name="Conversation" dataDxfId="21"/>
+    <tableColumn id="8" name="Use Case: Server" dataDxfId="20"/>
+    <tableColumn id="13" name="G" dataDxfId="19"/>
+    <tableColumn id="9" name="A:S" dataDxfId="18"/>
+    <tableColumn id="10" name="D" dataDxfId="17"/>
+    <tableColumn id="11" name="C" dataDxfId="16"/>
+    <tableColumn id="12" name="Notes: Server" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:D21"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Type" dataDxfId="26"/>
-    <tableColumn id="6" name="Name" dataDxfId="25"/>
-    <tableColumn id="2" name="Messages" dataDxfId="24"/>
-    <tableColumn id="3" name="Collaborators" dataDxfId="23"/>
+    <tableColumn id="1" name="Type" dataDxfId="12"/>
+    <tableColumn id="6" name="Name" dataDxfId="11"/>
+    <tableColumn id="2" name="Messages" dataDxfId="10"/>
+    <tableColumn id="3" name="Collaborators" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G25"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Name" dataDxfId="20"/>
-    <tableColumn id="7" name="Dependencies" dataDxfId="19"/>
-    <tableColumn id="6" name="Route" dataDxfId="18"/>
-    <tableColumn id="2" name="Controller" dataDxfId="17"/>
-    <tableColumn id="4" name="Directive" dataDxfId="16"/>
-    <tableColumn id="3" name="Factory" dataDxfId="15"/>
-    <tableColumn id="5" name="Service" dataDxfId="14"/>
+    <tableColumn id="1" name="Name" dataDxfId="6"/>
+    <tableColumn id="7" name="Dependencies" dataDxfId="5"/>
+    <tableColumn id="6" name="Route" dataDxfId="4"/>
+    <tableColumn id="2" name="Controller" dataDxfId="3"/>
+    <tableColumn id="4" name="Directive" dataDxfId="2"/>
+    <tableColumn id="3" name="Factory" dataDxfId="1"/>
+    <tableColumn id="5" name="Service" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project: Red" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4711,8 +4708,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:L46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4738,7 +4735,7 @@
       <c r="D2" s="23"/>
       <c r="E2" s="38"/>
       <c r="F2" s="22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -4754,7 +4751,7 @@
       </c>
       <c r="E3" s="39"/>
       <c r="F3" s="24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4764,12 +4761,10 @@
       <c r="C4" s="25">
         <v>2</v>
       </c>
-      <c r="D4" s="25" t="s">
-        <v>291</v>
-      </c>
+      <c r="D4" s="25"/>
       <c r="E4" s="39"/>
       <c r="F4" s="24" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4843,7 +4838,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>291</v>
+        <v>58</v>
       </c>
       <c r="E10" s="39"/>
       <c r="F10" s="39"/>
@@ -4909,9 +4904,7 @@
       <c r="C13" s="25">
         <v>1</v>
       </c>
-      <c r="D13" s="25" t="s">
-        <v>291</v>
-      </c>
+      <c r="D13" s="25"/>
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
     </row>
@@ -4922,9 +4915,7 @@
       <c r="C14" s="25">
         <v>1</v>
       </c>
-      <c r="D14" s="25" t="s">
-        <v>291</v>
-      </c>
+      <c r="D14" s="25"/>
       <c r="E14" s="39"/>
       <c r="F14" s="39"/>
     </row>
@@ -4935,9 +4926,7 @@
       <c r="C15" s="25">
         <v>4</v>
       </c>
-      <c r="D15" s="25" t="s">
-        <v>291</v>
-      </c>
+      <c r="D15" s="25"/>
       <c r="E15" s="39"/>
       <c r="F15" s="39"/>
     </row>
@@ -5098,9 +5087,7 @@
       <c r="C28" s="25">
         <v>5</v>
       </c>
-      <c r="D28" s="25" t="s">
-        <v>291</v>
-      </c>
+      <c r="D28" s="25"/>
       <c r="E28" s="39"/>
       <c r="F28" s="39"/>
     </row>
@@ -5111,9 +5098,7 @@
       <c r="C29" s="25">
         <v>1</v>
       </c>
-      <c r="D29" s="25" t="s">
-        <v>291</v>
-      </c>
+      <c r="D29" s="25"/>
       <c r="E29" s="39"/>
       <c r="F29" s="39"/>
     </row>
@@ -5124,9 +5109,7 @@
       <c r="C30" s="25">
         <v>2</v>
       </c>
-      <c r="D30" s="25" t="s">
-        <v>291</v>
-      </c>
+      <c r="D30" s="25"/>
       <c r="E30" s="39"/>
       <c r="F30" s="39"/>
     </row>
@@ -5148,9 +5131,7 @@
       <c r="C32" s="25">
         <v>5</v>
       </c>
-      <c r="D32" s="25" t="s">
-        <v>291</v>
-      </c>
+      <c r="D32" s="25"/>
       <c r="E32" s="39"/>
       <c r="F32" s="39"/>
     </row>
@@ -5162,7 +5143,7 @@
         <v>3</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="E33" s="39"/>
       <c r="F33" s="39"/>
@@ -5185,9 +5166,7 @@
       <c r="C35" s="25">
         <v>4</v>
       </c>
-      <c r="D35" s="25" t="s">
-        <v>291</v>
-      </c>
+      <c r="D35" s="25"/>
       <c r="E35" s="39"/>
       <c r="F35" s="39"/>
     </row>
@@ -5198,9 +5177,7 @@
       <c r="C36" s="25">
         <v>3</v>
       </c>
-      <c r="D36" s="25" t="s">
-        <v>291</v>
-      </c>
+      <c r="D36" s="25"/>
       <c r="E36" s="39"/>
       <c r="F36" s="39"/>
     </row>
@@ -5237,7 +5214,7 @@
       </c>
       <c r="D39" s="27">
         <f>SUMIF(D2:D38,"x",C2:C38)</f>
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E39" s="38"/>
       <c r="F39" s="38"/>
@@ -5430,22 +5407,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B25:C1048576 B1:C21">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="106" priority="1">
       <formula>$B1="Setup"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="105" priority="2">
       <formula>$B1="CSS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="104" priority="3">
       <formula>$B1="HTML"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="103" priority="4">
       <formula>$B1="JS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="102" priority="5">
       <formula>$B1="DB"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="101" priority="6">
       <formula>$B1="PHP"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5469,8 +5446,8 @@
   </sheetPr>
   <dimension ref="B2:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5566,7 +5543,10 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C8" s="15" t="s">
         <v>1</v>
       </c>
@@ -5818,36 +5798,48 @@
         <v>274</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C29" s="15" t="s">
         <v>128</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C30" s="15" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C31" s="15" t="s">
         <v>2</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C32" s="15" t="s">
         <v>128</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.25">
@@ -5865,29 +5857,29 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="C1:E1048576">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="CSS">
+    <cfRule type="containsText" dxfId="67" priority="2" operator="containsText" text="CSS">
       <formula>NOT(ISERROR(SEARCH("CSS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="HTML">
+    <cfRule type="containsText" dxfId="66" priority="3" operator="containsText" text="HTML">
       <formula>NOT(ISERROR(SEARCH("HTML",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="JS">
+    <cfRule type="containsText" dxfId="65" priority="4" operator="containsText" text="JS">
       <formula>NOT(ISERROR(SEARCH("JS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="DB">
+    <cfRule type="containsText" dxfId="64" priority="5" operator="containsText" text="DB">
       <formula>NOT(ISERROR(SEARCH("DB",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="PHP">
+    <cfRule type="containsText" dxfId="63" priority="6" operator="containsText" text="PHP">
       <formula>NOT(ISERROR(SEARCH("PHP",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Setup">
+    <cfRule type="containsText" dxfId="62" priority="1" operator="containsText" text="Setup">
       <formula>NOT(ISERROR(SEARCH("Setup",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F1048576">
-    <cfRule type="expression" dxfId="1" priority="9">
+    <cfRule type="expression" dxfId="61" priority="9">
       <formula>$B2="x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5915,8 +5907,8 @@
   </sheetPr>
   <dimension ref="B2:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5988,7 +5980,10 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="C8" s="4" t="s">
         <v>256</v>
       </c>
@@ -6069,7 +6064,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C17" s="4" t="s">
         <v>2</v>
       </c>
@@ -6077,7 +6072,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="18" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
         <v>250</v>
       </c>
@@ -6085,7 +6080,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
         <v>266</v>
       </c>
@@ -6093,7 +6088,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="20" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
         <v>277</v>
       </c>
@@ -6101,7 +6096,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
         <v>279</v>
       </c>
@@ -6109,7 +6104,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="22" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
         <v>279</v>
       </c>
@@ -6117,7 +6112,10 @@
         <v>282</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="C23" s="4" t="s">
         <v>284</v>
       </c>
@@ -6125,7 +6123,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
         <v>288</v>
       </c>
@@ -6133,17 +6131,17 @@
         <v>289</v>
       </c>
     </row>
-    <row r="25" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C25" s="4" t="s">
         <v>288</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="53" priority="1">
       <formula>$C5="x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6682,7 +6680,7 @@
   </sheetPr>
   <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
More work on collaboration, but ultimately unfinished. Calling it at ~3800 lines of code with comments removed.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -492,7 +492,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="302">
   <si>
     <t>Design</t>
   </si>
@@ -732,16 +732,6 @@
   </si>
   <si>
     <t>Conversation</t>
-  </si>
-  <si>
-    <t>&gt;&gt; Prompt client to enter old password and new password (twice)
-&lt;&lt; Enter old and new password
-&lt;&lt; Check that both password fields match
-&lt;&lt; If not, re-enter old and new password
-&lt;&lt; Else, send to server
-&gt;&gt; Hash old password and compare against the password in the database
-&gt;&gt; If password does not match, notify and reprompt client and do not continue
-&gt;&gt; Else, hash new password, replace old password, and notify client</t>
   </si>
   <si>
     <t>id PK AUTO_INCREMENT</t>
@@ -956,17 +946,6 @@
   <si>
     <t>&gt;&gt; Sanitize input
 &gt;&gt; If invalid input, notify client and do not continue</t>
-  </si>
-  <si>
-    <t>&gt;&gt; Prompt client for username, password (twice), and email address
-&lt;&lt; Enter credentials
-&lt;&lt; Check that both password fields match
-&lt;&lt;  If not, re-enter credentials
-&lt;&lt; Else, send to server
-&gt;&gt; Sanitize Input*
-&gt;&gt; Verify username is unique by comparing against database
-&gt;&gt; If username already exists, notify client
-&gt;&gt; Else, create user in database and notify client</t>
   </si>
   <si>
     <t>&gt;&gt; Prompt client to CRUD and enter information where applicable
@@ -1007,16 +986,6 @@
 &gt;&gt; Delete session cookie
 &gt;&gt; Delete session
 &lt;&lt; Delete cookie</t>
-  </si>
-  <si>
-    <t>&gt;&gt; Prompt client for credentials
-&lt;&lt; Enter username and password
-&gt;&gt; Sanitize Input*
-&gt;&gt; Compare username to users in database
-&gt;&gt; If no such username, notify and reprompt client and do not continue
-&gt;&gt; Else, hash the password and compare it against the password in the database
-&gt;&gt; If password does not match, notify and reprompt client
-&gt;&gt; Else, Start Session*</t>
   </si>
   <si>
     <t>&gt;&gt; Prompt client to logout
@@ -1435,9 +1404,6 @@
     <t>Recurrence changes are saved regardless of if submit is clicked or not</t>
   </si>
   <si>
-    <t xml:space="preserve">Other </t>
-  </si>
-  <si>
     <t>cacheService to share the activities between main controller and directives</t>
   </si>
   <si>
@@ -1447,13 +1413,56 @@
     <t>Sanitize input/files</t>
   </si>
   <si>
-    <t>Labels and calendars</t>
-  </si>
-  <si>
     <t>If error on query, create object in vm.x under x.summary that displays error message</t>
   </si>
   <si>
     <t>start and get session user id on query in php to reduce api calls</t>
+  </si>
+  <si>
+    <t>Extra (Not  in proposal)</t>
+  </si>
+  <si>
+    <t>Deny access to restricted areas</t>
+  </si>
+  <si>
+    <t>Validate input</t>
+  </si>
+  <si>
+    <t>&gt;&gt; Prompt client for username, password (twice), and email address
+&lt;&lt; Enter credentials
+&lt;&lt; Check that both password fields match
+&lt;&lt;  If not, re-enter credentials
+&lt;&lt; Send to server
+&gt;&gt; Sanitize Input*
+&gt;&gt; Verify username is unique by comparing against database
+&gt;&gt; If username already exists, notify client
+&gt;&gt; Create user in database and notify client</t>
+  </si>
+  <si>
+    <t>&gt;&gt; Prompt client for credentials
+&lt;&lt; Enter username and password
+&gt;&gt; Sanitize Input*
+&gt;&gt; Compare username to users in database
+&gt;&gt; If no such username, notify and reprompt client and do not continue
+&gt;&gt; Hash the password and compare it against the password in the database
+&gt;&gt; If password does not match, notify and reprompt client
+&gt;&gt; Start Session*</t>
+  </si>
+  <si>
+    <t>&gt;&gt; Prompt client to enter old password and new password (twice)
+&lt;&lt; Enter old and new password
+&lt;&lt; Check that both password fields match
+&lt;&lt; If not, re-enter old and new password
+&lt;&lt; Send to server
+&gt;&gt; Hash old password and compare against the password in the database
+&gt;&gt; If password does not match, notify and reprompt client and do not continue
+&gt;&gt; Hash new password, replace old password, and notify client</t>
+  </si>
+  <si>
+    <t>PHP unit tests</t>
+  </si>
+  <si>
+    <t>Labels (task groups) and calendars (event groups)</t>
   </si>
 </sst>
 </file>
@@ -1567,7 +1576,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1645,11 +1654,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF1F4E79"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF1F4E79"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF1F4E79"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF1F4E79"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF1F4E79"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1710,20 +1743,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1769,11 +1793,153 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="125">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1989,11 +2155,6 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2015,68 +2176,6 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2174,63 +2273,6 @@
     </dxf>
     <dxf>
       <alignment vertical="top" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3181,7 +3223,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -3325,7 +3367,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -3391,13 +3433,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -3855,6 +3897,46 @@
     <i/>
   </colItems>
   <formats count="33">
+    <format dxfId="106">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="105">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="104">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="103">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="102">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="101">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
     <format dxfId="100">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
@@ -3870,46 +3952,6 @@
       </pivotArea>
     </format>
     <format dxfId="99">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="98">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="97">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="96">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="95">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
-    </format>
-    <format dxfId="94">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="93">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3923,7 +3965,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="98">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3936,7 +3978,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="97">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3949,7 +3991,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="96">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3965,7 +4007,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="95">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3977,7 +4019,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="94">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3989,16 +4031,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="93">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="86">
+    <format dxfId="92">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="85">
+    <format dxfId="91">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="84">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -4012,7 +4054,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4026,7 +4068,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4039,7 +4081,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="87">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4052,7 +4094,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4068,7 +4110,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="85">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4080,7 +4122,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4092,10 +4134,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="83">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="76">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4104,7 +4146,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="81">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4113,7 +4155,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="80">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4122,7 +4164,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="79">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4131,7 +4173,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4140,7 +4182,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="77">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4152,7 +4194,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="76">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4165,7 +4207,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="75">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4178,7 +4220,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="74">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4330,7 +4372,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F36" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F36" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
   <autoFilter ref="B2:F36">
     <filterColumn colId="0">
       <filters blank="1"/>
@@ -4340,103 +4382,103 @@
     <sortCondition ref="C2:C30"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Done" dataDxfId="58"/>
-    <tableColumn id="3" name="Category" dataDxfId="57"/>
-    <tableColumn id="5" name="Remember" dataDxfId="56"/>
-    <tableColumn id="4" name="Look Into" dataDxfId="55"/>
-    <tableColumn id="2" name="Task" dataDxfId="54"/>
+    <tableColumn id="1" name="Done" dataDxfId="71"/>
+    <tableColumn id="3" name="Category" dataDxfId="70"/>
+    <tableColumn id="5" name="Remember" dataDxfId="69"/>
+    <tableColumn id="4" name="Look Into" dataDxfId="68"/>
+    <tableColumn id="2" name="Task" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:D31" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:D31" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="B2:D31">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="Done" dataDxfId="50"/>
-    <tableColumn id="2" name="File" dataDxfId="49"/>
-    <tableColumn id="3" name="Feature" dataDxfId="48"/>
+    <tableColumn id="1" name="Done" dataDxfId="64"/>
+    <tableColumn id="2" name="File" dataDxfId="63"/>
+    <tableColumn id="3" name="Feature" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q14" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q14" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="A1:Q14"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Name" dataDxfId="45"/>
-    <tableColumn id="2" name="Foreign Key1" dataDxfId="44"/>
-    <tableColumn id="3" name="Foreign Key2" dataDxfId="43"/>
-    <tableColumn id="4" name="Column1" dataDxfId="42"/>
-    <tableColumn id="5" name="Column2" dataDxfId="41"/>
-    <tableColumn id="6" name="Column3" dataDxfId="40"/>
-    <tableColumn id="7" name="Column4" dataDxfId="39"/>
-    <tableColumn id="8" name="Column5" dataDxfId="38"/>
-    <tableColumn id="9" name="Column6" dataDxfId="37"/>
-    <tableColumn id="13" name="Column7" dataDxfId="36"/>
-    <tableColumn id="12" name="Column8" dataDxfId="35"/>
-    <tableColumn id="11" name="Column9" dataDxfId="34"/>
-    <tableColumn id="17" name="Column10" dataDxfId="33"/>
-    <tableColumn id="16" name="Column11" dataDxfId="32"/>
-    <tableColumn id="15" name="Column12" dataDxfId="31"/>
-    <tableColumn id="14" name="Column13" dataDxfId="30"/>
-    <tableColumn id="10" name="Column14" dataDxfId="29"/>
+    <tableColumn id="1" name="Name" dataDxfId="59"/>
+    <tableColumn id="2" name="Foreign Key1" dataDxfId="58"/>
+    <tableColumn id="3" name="Foreign Key2" dataDxfId="57"/>
+    <tableColumn id="4" name="Column1" dataDxfId="56"/>
+    <tableColumn id="5" name="Column2" dataDxfId="55"/>
+    <tableColumn id="6" name="Column3" dataDxfId="54"/>
+    <tableColumn id="7" name="Column4" dataDxfId="53"/>
+    <tableColumn id="8" name="Column5" dataDxfId="52"/>
+    <tableColumn id="9" name="Column6" dataDxfId="51"/>
+    <tableColumn id="13" name="Column7" dataDxfId="50"/>
+    <tableColumn id="12" name="Column8" dataDxfId="49"/>
+    <tableColumn id="11" name="Column9" dataDxfId="48"/>
+    <tableColumn id="17" name="Column10" dataDxfId="47"/>
+    <tableColumn id="16" name="Column11" dataDxfId="46"/>
+    <tableColumn id="15" name="Column12" dataDxfId="45"/>
+    <tableColumn id="14" name="Column13" dataDxfId="44"/>
+    <tableColumn id="10" name="Column14" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="A2:L108"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Notes: Client" dataDxfId="26"/>
-    <tableColumn id="2" name="A:C" dataDxfId="25"/>
-    <tableColumn id="3" name="U" dataDxfId="24"/>
-    <tableColumn id="4" name="S" dataDxfId="23"/>
-    <tableColumn id="5" name="Use Case: Client" dataDxfId="22"/>
-    <tableColumn id="6" name="Conversation" dataDxfId="21"/>
-    <tableColumn id="8" name="Use Case: Server" dataDxfId="20"/>
-    <tableColumn id="13" name="G" dataDxfId="19"/>
-    <tableColumn id="9" name="A:S" dataDxfId="18"/>
-    <tableColumn id="10" name="D" dataDxfId="17"/>
-    <tableColumn id="11" name="C" dataDxfId="16"/>
-    <tableColumn id="12" name="Notes: Server" dataDxfId="15"/>
+    <tableColumn id="1" name="Notes: Client" dataDxfId="40"/>
+    <tableColumn id="2" name="A:C" dataDxfId="39"/>
+    <tableColumn id="3" name="U" dataDxfId="38"/>
+    <tableColumn id="4" name="S" dataDxfId="37"/>
+    <tableColumn id="5" name="Use Case: Client" dataDxfId="36"/>
+    <tableColumn id="6" name="Conversation" dataDxfId="35"/>
+    <tableColumn id="8" name="Use Case: Server" dataDxfId="34"/>
+    <tableColumn id="13" name="G" dataDxfId="33"/>
+    <tableColumn id="9" name="A:S" dataDxfId="32"/>
+    <tableColumn id="10" name="D" dataDxfId="31"/>
+    <tableColumn id="11" name="C" dataDxfId="30"/>
+    <tableColumn id="12" name="Notes: Server" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:D21"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Type" dataDxfId="12"/>
-    <tableColumn id="6" name="Name" dataDxfId="11"/>
-    <tableColumn id="2" name="Messages" dataDxfId="10"/>
-    <tableColumn id="3" name="Collaborators" dataDxfId="9"/>
+    <tableColumn id="1" name="Type" dataDxfId="26"/>
+    <tableColumn id="6" name="Name" dataDxfId="25"/>
+    <tableColumn id="2" name="Messages" dataDxfId="24"/>
+    <tableColumn id="3" name="Collaborators" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:G25"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Name" dataDxfId="6"/>
-    <tableColumn id="7" name="Dependencies" dataDxfId="5"/>
-    <tableColumn id="6" name="Route" dataDxfId="4"/>
-    <tableColumn id="2" name="Controller" dataDxfId="3"/>
-    <tableColumn id="4" name="Directive" dataDxfId="2"/>
-    <tableColumn id="3" name="Factory" dataDxfId="1"/>
-    <tableColumn id="5" name="Service" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="20"/>
+    <tableColumn id="7" name="Dependencies" dataDxfId="19"/>
+    <tableColumn id="6" name="Route" dataDxfId="18"/>
+    <tableColumn id="2" name="Controller" dataDxfId="17"/>
+    <tableColumn id="4" name="Directive" dataDxfId="16"/>
+    <tableColumn id="3" name="Factory" dataDxfId="15"/>
+    <tableColumn id="5" name="Service" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project: Red" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4706,534 +4748,706 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:L46"/>
+  <dimension ref="B1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="56.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="37"/>
-    <col min="6" max="6" width="43" style="37" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="2" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="34"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="22">
         <v>17</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="22" t="s">
-        <v>292</v>
-      </c>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="35"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="44"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="23">
         <v>5</v>
       </c>
-      <c r="D3" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="36"/>
+    </row>
+    <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="44"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="23">
+        <v>2</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="G4" s="36"/>
+    </row>
+    <row r="5" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="23">
+        <v>5</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="36"/>
+    </row>
+    <row r="6" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="44"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="23">
+        <v>5</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="G6" s="36"/>
+    </row>
+    <row r="7" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="41"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="24">
+        <v>15</v>
+      </c>
+      <c r="F7" s="24"/>
+      <c r="G7" s="35"/>
+    </row>
+    <row r="8" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="44"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="23">
+        <v>5</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="36"/>
+    </row>
+    <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="44"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="23">
+        <v>2</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="36"/>
+    </row>
+    <row r="10" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="44"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="23">
+        <v>5</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="36"/>
+    </row>
+    <row r="11" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="23">
+        <v>3</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="36"/>
+    </row>
+    <row r="12" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="41"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="24">
+        <v>6</v>
+      </c>
+      <c r="F12" s="24"/>
+      <c r="G12" s="35"/>
+    </row>
+    <row r="13" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="44"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="23">
+        <v>1</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="G13" s="36"/>
+    </row>
+    <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="44"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="23">
+        <v>1</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="G14" s="36"/>
+    </row>
+    <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="44"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="23">
+        <v>4</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" s="36"/>
+    </row>
+    <row r="16" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="24">
+        <v>24</v>
+      </c>
+      <c r="F16" s="24"/>
+      <c r="G16" s="35"/>
+    </row>
+    <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="23">
+        <v>5</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="36"/>
+    </row>
+    <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="44"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="23">
+        <v>1</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="36"/>
+    </row>
+    <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="44"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="23">
+        <v>1</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="36"/>
+    </row>
+    <row r="20" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="44"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="23">
+        <v>1</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="36"/>
+    </row>
+    <row r="21" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="44"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="23">
+        <v>1</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="36"/>
+    </row>
+    <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="44"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="23">
+        <v>5</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" s="36"/>
+    </row>
+    <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="44"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="23">
+        <v>5</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" s="36"/>
+    </row>
+    <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="44"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="23">
+        <v>5</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="36"/>
+    </row>
+    <row r="25" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="24">
+        <v>18</v>
+      </c>
+      <c r="F25" s="24"/>
+      <c r="G25" s="35"/>
+    </row>
+    <row r="26" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="44"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="23">
+        <v>5</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="36"/>
+    </row>
+    <row r="27" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="44"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="23">
+        <v>5</v>
+      </c>
+      <c r="F27" s="23"/>
+      <c r="G27" s="36"/>
+    </row>
+    <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="44"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="23">
+        <v>5</v>
+      </c>
+      <c r="F28" s="23"/>
+      <c r="G28" s="36"/>
+    </row>
+    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="44"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="23">
+        <v>1</v>
+      </c>
+      <c r="F29" s="23"/>
+      <c r="G29" s="36"/>
+    </row>
+    <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="44"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="23">
+        <v>2</v>
+      </c>
+      <c r="F30" s="23"/>
+      <c r="G30" s="36"/>
+    </row>
+    <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="41"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="24">
+        <v>8</v>
+      </c>
+      <c r="F31" s="24"/>
+      <c r="G31" s="35"/>
+    </row>
+    <row r="32" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="44"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="23">
+        <v>5</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" s="36"/>
+    </row>
+    <row r="33" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="44"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="23">
+        <v>3</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" s="36"/>
+    </row>
+    <row r="34" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="41"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="24">
+        <v>17</v>
+      </c>
+      <c r="F34" s="24"/>
+      <c r="G34" s="35"/>
+    </row>
+    <row r="35" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="44"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="23">
+        <v>4</v>
+      </c>
+      <c r="F35" s="23"/>
+      <c r="G35" s="36"/>
+    </row>
+    <row r="36" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="44"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="23">
+        <v>3</v>
+      </c>
+      <c r="F36" s="23"/>
+      <c r="G36" s="36"/>
+    </row>
+    <row r="37" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="44"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="23">
+        <v>5</v>
+      </c>
+      <c r="F37" s="23"/>
+      <c r="G37" s="36"/>
+    </row>
+    <row r="38" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="44"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="23">
+        <v>5</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="G38" s="36"/>
+    </row>
+    <row r="39" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="40" t="s">
+        <v>294</v>
+      </c>
+      <c r="C39" s="41"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="24">
+        <v>0</v>
+      </c>
+      <c r="F39" s="24"/>
+      <c r="G39" s="36"/>
+    </row>
+    <row r="40" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="43" t="s">
+        <v>291</v>
+      </c>
+      <c r="C40" s="44"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="23">
+        <v>0</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G40" s="36"/>
+    </row>
+    <row r="41" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="43" t="s">
+        <v>296</v>
+      </c>
+      <c r="C41" s="44"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="23">
+        <v>0</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G41" s="36"/>
+    </row>
+    <row r="42" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="43" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="25">
-        <v>2</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="24" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="25">
-        <v>5</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="24"/>
-    </row>
-    <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="25">
-        <v>5</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>283</v>
-      </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="24"/>
-    </row>
-    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="27">
-        <v>15</v>
-      </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-    </row>
-    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="25">
-        <v>5</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-    </row>
-    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="25">
-        <v>2</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-    </row>
-    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="25">
-        <v>5</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-    </row>
-    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="25">
-        <v>3</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="H11" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="K11" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="L11" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="27">
-        <v>6</v>
-      </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="H12" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12" s="25">
-        <v>84</v>
-      </c>
-      <c r="J12" s="25">
-        <v>74</v>
-      </c>
-      <c r="K12" s="25">
-        <v>64</v>
-      </c>
-      <c r="L12" s="25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="25">
-        <v>1</v>
-      </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-    </row>
-    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="25">
-        <v>1</v>
-      </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-    </row>
-    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="25">
-        <v>4</v>
-      </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-    </row>
-    <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="27">
-        <v>24</v>
-      </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-    </row>
-    <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="25">
-        <v>5</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-    </row>
-    <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="25">
-        <v>1</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-    </row>
-    <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="25">
-        <v>1</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-    </row>
-    <row r="20" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="25">
-        <v>1</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-    </row>
-    <row r="21" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="25">
-        <v>1</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-    </row>
-    <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="25">
-        <v>5</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-    </row>
-    <row r="23" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="25">
-        <v>5</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-    </row>
-    <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="25">
-        <v>5</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-    </row>
-    <row r="25" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="27">
-        <v>18</v>
-      </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-    </row>
-    <row r="26" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="25">
-        <v>5</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-    </row>
-    <row r="27" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="25">
-        <v>5</v>
-      </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-    </row>
-    <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="25">
-        <v>5</v>
-      </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-    </row>
-    <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="25">
-        <v>1</v>
-      </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-    </row>
-    <row r="30" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="25">
-        <v>2</v>
-      </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-    </row>
-    <row r="31" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="27">
-        <v>8</v>
-      </c>
-      <c r="D31" s="27"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-    </row>
-    <row r="32" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="25">
-        <v>5</v>
-      </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-    </row>
-    <row r="33" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="25">
-        <v>3</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>283</v>
-      </c>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-    </row>
-    <row r="34" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="27">
-        <v>17</v>
-      </c>
-      <c r="D34" s="27"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-    </row>
-    <row r="35" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="25">
-        <v>4</v>
-      </c>
-      <c r="D35" s="25"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-    </row>
-    <row r="36" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="25">
-        <v>3</v>
-      </c>
-      <c r="D36" s="25"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-    </row>
-    <row r="37" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="25">
-        <v>5</v>
-      </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
-    </row>
-    <row r="38" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="25">
-        <v>5</v>
-      </c>
-      <c r="D38" s="25" t="s">
-        <v>283</v>
-      </c>
-      <c r="E38" s="39"/>
-      <c r="F38" s="39"/>
-    </row>
-    <row r="39" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="26" t="s">
+      <c r="C42" s="44"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="23">
+        <v>0</v>
+      </c>
+      <c r="F42" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G42" s="36"/>
+    </row>
+    <row r="43" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="43" t="s">
+        <v>301</v>
+      </c>
+      <c r="C43" s="44"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="23">
+        <v>0</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G43" s="36"/>
+    </row>
+    <row r="44" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="43" t="s">
+        <v>300</v>
+      </c>
+      <c r="C44" s="44"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="23">
+        <v>0</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G44" s="36"/>
+    </row>
+    <row r="45" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="27">
+      <c r="C45" s="41"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="24">
         <v>105</v>
       </c>
-      <c r="D39" s="27">
-        <f>SUMIF(D2:D38,"x",C2:C38)</f>
-        <v>54</v>
-      </c>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="40"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="24">
+        <f>SUMIF(F2:F38,"x",E2:E38)</f>
+        <v>62</v>
+      </c>
+      <c r="G45" s="35"/>
+    </row>
+    <row r="46" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="40"/>
-      <c r="F46" s="40"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="37"/>
+    </row>
+    <row r="47" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F47" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" s="23">
+        <v>84</v>
+      </c>
+      <c r="D48" s="23">
+        <v>74</v>
+      </c>
+      <c r="E48" s="23">
+        <v>64</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="37"/>
     </row>
   </sheetData>
+  <mergeCells count="44">
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5275,7 +5489,7 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>34</v>
@@ -5283,26 +5497,26 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C3" s="18"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="13"/>
       <c r="C4" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
       <c r="C5" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="13"/>
       <c r="C6" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -5314,31 +5528,31 @@
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
       <c r="C9" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" s="18"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
       <c r="C12" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
@@ -5350,47 +5564,47 @@
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="13"/>
       <c r="C14" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
       <c r="C16" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="13"/>
       <c r="C17" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="13"/>
       <c r="C18" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C19" s="18"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C20" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C21" s="18"/>
     </row>
@@ -5407,22 +5621,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B25:C1048576 B1:C21">
-    <cfRule type="expression" dxfId="106" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>$B1="Setup"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>$B1="CSS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>$B1="HTML"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>$B1="JS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>$B1="DB"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>$B1="PHP"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5467,16 +5681,16 @@
   <sheetData>
     <row r="2" spans="2:6" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>124</v>
-      </c>
       <c r="D2" s="15" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>34</v>
@@ -5487,10 +5701,10 @@
         <v>58</v>
       </c>
       <c r="C3" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>125</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5498,13 +5712,13 @@
         <v>58</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>58</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5512,13 +5726,13 @@
         <v>58</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>58</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5529,7 +5743,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5540,7 +5754,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5551,10 +5765,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -5562,10 +5776,10 @@
         <v>1</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5576,10 +5790,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5593,7 +5807,7 @@
         <v>58</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5601,10 +5815,10 @@
         <v>58</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5612,13 +5826,13 @@
         <v>58</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>58</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5626,21 +5840,21 @@
         <v>58</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C15" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5648,10 +5862,10 @@
         <v>58</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5659,13 +5873,13 @@
         <v>58</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>58</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5676,7 +5890,7 @@
         <v>2</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5687,7 +5901,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5698,7 +5912,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5709,7 +5923,7 @@
         <v>2</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5720,7 +5934,7 @@
         <v>2</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5731,10 +5945,10 @@
         <v>2</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -5745,10 +5959,10 @@
         <v>2</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5759,10 +5973,10 @@
         <v>2</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5776,26 +5990,29 @@
         <v>58</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C27" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C28" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5803,10 +6020,10 @@
         <v>58</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="30" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5817,7 +6034,7 @@
         <v>2</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="31" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5828,7 +6045,7 @@
         <v>2</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="32" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5836,10 +6053,10 @@
         <v>58</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.25">
@@ -5857,29 +6074,29 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="C1:E1048576">
-    <cfRule type="containsText" dxfId="67" priority="2" operator="containsText" text="CSS">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="CSS">
       <formula>NOT(ISERROR(SEARCH("CSS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="3" operator="containsText" text="HTML">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="HTML">
       <formula>NOT(ISERROR(SEARCH("HTML",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="4" operator="containsText" text="JS">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="JS">
       <formula>NOT(ISERROR(SEARCH("JS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="5" operator="containsText" text="DB">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="DB">
       <formula>NOT(ISERROR(SEARCH("DB",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="6" operator="containsText" text="PHP">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="PHP">
       <formula>NOT(ISERROR(SEARCH("PHP",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="containsText" dxfId="62" priority="1" operator="containsText" text="Setup">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Setup">
       <formula>NOT(ISERROR(SEARCH("Setup",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F1048576">
-    <cfRule type="expression" dxfId="61" priority="9">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>$B2="x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5907,8 +6124,8 @@
   </sheetPr>
   <dimension ref="B2:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5922,21 +6139,21 @@
   <sheetData>
     <row r="2" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5944,18 +6161,18 @@
         <v>58</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -5963,10 +6180,10 @@
         <v>58</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
@@ -5977,7 +6194,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
@@ -5985,10 +6202,10 @@
         <v>58</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
@@ -5996,18 +6213,18 @@
         <v>58</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -6015,10 +6232,10 @@
         <v>58</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -6026,18 +6243,18 @@
         <v>58</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C13" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
@@ -6045,23 +6262,26 @@
         <v>2</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C15" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D15" s="12" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="4" t="s">
-        <v>270</v>
-      </c>
       <c r="D16" s="12" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -6069,47 +6289,47 @@
         <v>2</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>279</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="23" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
@@ -6117,31 +6337,31 @@
         <v>58</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C25" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>288</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>291</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="53" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$C5="x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6193,115 +6413,115 @@
         <v>50</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>93</v>
-      </c>
       <c r="D1" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="11" t="s">
-        <v>91</v>
-      </c>
       <c r="K1" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="O1" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="O1" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>118</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H2" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>108</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>109</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>51</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>148</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>149</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -6336,20 +6556,20 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -6368,22 +6588,22 @@
         <v>38</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -6398,17 +6618,17 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -6428,22 +6648,22 @@
         <v>37</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
@@ -6477,38 +6697,38 @@
     </row>
     <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
@@ -6518,51 +6738,51 @@
     </row>
     <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G11" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="H11" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>112</v>
-      </c>
       <c r="I11" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="L11" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="M11" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="N11" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="O11" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="M11" s="12" t="s">
+      <c r="P11" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="N11" s="12" t="s">
+      <c r="Q11" s="12" t="s">
         <v>208</v>
-      </c>
-      <c r="O11" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="P11" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q11" s="12" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -6586,19 +6806,19 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
@@ -6615,19 +6835,19 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>104</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>105</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -6654,10 +6874,10 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" t="s">
         <v>121</v>
-      </c>
-      <c r="B19" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -6680,8 +6900,8 @@
   </sheetPr>
   <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6697,22 +6917,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
       <c r="F1" s="10"/>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -6767,7 +6987,7 @@
         <v>63</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>63</v>
@@ -6784,7 +7004,7 @@
     </row>
     <row r="4" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
@@ -6797,7 +7017,7 @@
         <v>67</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>152</v>
+        <v>297</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>66</v>
@@ -6823,10 +7043,10 @@
         <v>74</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9" t="s">
@@ -6839,7 +7059,7 @@
         <v>58</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -6855,7 +7075,7 @@
         <v>75</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>75</v>
@@ -6871,7 +7091,7 @@
         <v>58</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="210" x14ac:dyDescent="0.25">
@@ -6889,7 +7109,7 @@
         <v>70</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>80</v>
+        <v>299</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>70</v>
@@ -6919,7 +7139,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>161</v>
+        <v>298</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>8</v>
@@ -6985,7 +7205,7 @@
         <v>65</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>65</v>
@@ -7012,13 +7232,13 @@
         <v>58</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -7045,7 +7265,7 @@
         <v>64</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>64</v>
@@ -7067,10 +7287,10 @@
       <c r="D13" s="9"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -7082,7 +7302,7 @@
     </row>
     <row r="14" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>58</v>
@@ -7094,13 +7314,13 @@
         <v>58</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -7124,13 +7344,13 @@
         <v>58</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
@@ -7154,13 +7374,13 @@
         <v>58</v>
       </c>
       <c r="E16" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>170</v>
-      </c>
       <c r="G16" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -7180,7 +7400,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
@@ -7204,11 +7424,11 @@
         <v>58</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -8507,185 +8727,185 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" style="36" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="34" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="31" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="31" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="31"/>
+    <col min="1" max="1" width="6" style="33" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="31" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="28" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="28" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="C13" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="B1" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>217</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>219</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>220</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>221</v>
-      </c>
-      <c r="D5" s="31" t="s">
+      <c r="D13" s="12" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>222</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>223</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="34" t="s">
-        <v>228</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="B14" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="34" t="s">
-        <v>227</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>230</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="34" t="s">
+      <c r="B15" s="31" t="s">
         <v>231</v>
       </c>
-      <c r="D11" s="31" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="C12" s="31" t="s">
+      <c r="D15" s="28" t="s">
         <v>225</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>232</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>229</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>233</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>234</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -8724,267 +8944,267 @@
         <v>50</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
         <v>184</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>187</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
+      <c r="D2" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
-        <v>176</v>
-      </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
+      <c r="A3" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="30"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="27"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
-        <v>215</v>
-      </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30" t="s">
+      <c r="A5" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30" t="s">
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
-        <v>177</v>
+      <c r="A7" s="29" t="s">
+        <v>174</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
+      <c r="D7" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="29" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
+      <c r="D8" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
-        <v>186</v>
+      <c r="A9" s="29" t="s">
+        <v>183</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
+      <c r="D9" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
-        <v>178</v>
+      <c r="A10" s="29" t="s">
+        <v>175</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
+      <c r="D10" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="29" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
+      <c r="D11" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
+      <c r="D12" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
+      <c r="D13" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
+      <c r="A14" s="29"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
+      <c r="A15" s="29"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
+      <c r="A16" s="29"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
+      <c r="A17" s="29"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
+      <c r="A18" s="29"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
+      <c r="A19" s="29"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
+      <c r="A20" s="29"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
+      <c r="A21" s="29"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
+      <c r="A22" s="29"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
+      <c r="A23" s="29"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
+      <c r="A24" s="29"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
+      <c r="A25" s="29"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bug fixes when adding activities and demo database created.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -492,7 +492,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="301">
   <si>
     <t>Design</t>
   </si>
@@ -1420,9 +1420,6 @@
   </si>
   <si>
     <t>Extra (Not  in proposal)</t>
-  </si>
-  <si>
-    <t>Deny access to restricted areas</t>
   </si>
   <si>
     <t>Validate input</t>
@@ -1787,11 +1784,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1802,14 +1802,11 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3223,7 +3220,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -3295,7 +3292,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -3361,13 +3358,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -3433,13 +3430,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -4748,10 +4745,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:I52"/>
+  <dimension ref="B1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:D44"/>
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4766,11 +4763,11 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="22">
         <v>17</v>
       </c>
@@ -4779,11 +4776,11 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="45"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="40"/>
       <c r="E3" s="23">
         <v>5</v>
       </c>
@@ -4793,11 +4790,11 @@
       <c r="G3" s="36"/>
     </row>
     <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="45"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="23">
         <v>2</v>
       </c>
@@ -4807,11 +4804,11 @@
       <c r="G4" s="36"/>
     </row>
     <row r="5" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="45"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
       <c r="E5" s="23">
         <v>5</v>
       </c>
@@ -4821,11 +4818,11 @@
       <c r="G5" s="36"/>
     </row>
     <row r="6" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="45"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="40"/>
       <c r="E6" s="23">
         <v>5</v>
       </c>
@@ -4835,11 +4832,11 @@
       <c r="G6" s="36"/>
     </row>
     <row r="7" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="43"/>
       <c r="E7" s="24">
         <v>15</v>
       </c>
@@ -4847,11 +4844,11 @@
       <c r="G7" s="35"/>
     </row>
     <row r="8" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="45"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="23">
         <v>5</v>
       </c>
@@ -4861,11 +4858,11 @@
       <c r="G8" s="36"/>
     </row>
     <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="45"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="40"/>
       <c r="E9" s="23">
         <v>2</v>
       </c>
@@ -4875,11 +4872,11 @@
       <c r="G9" s="36"/>
     </row>
     <row r="10" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="45"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="40"/>
       <c r="E10" s="23">
         <v>5</v>
       </c>
@@ -4889,11 +4886,11 @@
       <c r="G10" s="36"/>
     </row>
     <row r="11" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="45"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="40"/>
       <c r="E11" s="23">
         <v>3</v>
       </c>
@@ -4903,11 +4900,11 @@
       <c r="G11" s="36"/>
     </row>
     <row r="12" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="43"/>
       <c r="E12" s="24">
         <v>6</v>
       </c>
@@ -4915,11 +4912,11 @@
       <c r="G12" s="35"/>
     </row>
     <row r="13" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="45"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
       <c r="E13" s="23">
         <v>1</v>
       </c>
@@ -4929,11 +4926,11 @@
       <c r="G13" s="36"/>
     </row>
     <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="45"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="40"/>
       <c r="E14" s="23">
         <v>1</v>
       </c>
@@ -4943,11 +4940,11 @@
       <c r="G14" s="36"/>
     </row>
     <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="45"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
       <c r="E15" s="23">
         <v>4</v>
       </c>
@@ -4955,11 +4952,11 @@
       <c r="G15" s="36"/>
     </row>
     <row r="16" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="43"/>
       <c r="E16" s="24">
         <v>24</v>
       </c>
@@ -4967,11 +4964,11 @@
       <c r="G16" s="35"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="45"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
       <c r="E17" s="23">
         <v>5</v>
       </c>
@@ -4981,11 +4978,11 @@
       <c r="G17" s="36"/>
     </row>
     <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="45"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="40"/>
       <c r="E18" s="23">
         <v>1</v>
       </c>
@@ -4995,11 +4992,11 @@
       <c r="G18" s="36"/>
     </row>
     <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="44"/>
-      <c r="D19" s="45"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
       <c r="E19" s="23">
         <v>1</v>
       </c>
@@ -5009,11 +5006,11 @@
       <c r="G19" s="36"/>
     </row>
     <row r="20" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="45"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="40"/>
       <c r="E20" s="23">
         <v>1</v>
       </c>
@@ -5023,11 +5020,11 @@
       <c r="G20" s="36"/>
     </row>
     <row r="21" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="45"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
       <c r="E21" s="23">
         <v>1</v>
       </c>
@@ -5037,11 +5034,11 @@
       <c r="G21" s="36"/>
     </row>
     <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="45"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="40"/>
       <c r="E22" s="23">
         <v>5</v>
       </c>
@@ -5051,11 +5048,11 @@
       <c r="G22" s="36"/>
     </row>
     <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="45"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="40"/>
       <c r="E23" s="23">
         <v>5</v>
       </c>
@@ -5065,11 +5062,11 @@
       <c r="G23" s="36"/>
     </row>
     <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="45"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
       <c r="E24" s="23">
         <v>5</v>
       </c>
@@ -5079,11 +5076,11 @@
       <c r="G24" s="36"/>
     </row>
     <row r="25" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="43"/>
       <c r="E25" s="24">
         <v>18</v>
       </c>
@@ -5091,11 +5088,11 @@
       <c r="G25" s="35"/>
     </row>
     <row r="26" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="44"/>
-      <c r="D26" s="45"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="40"/>
       <c r="E26" s="23">
         <v>5</v>
       </c>
@@ -5105,11 +5102,11 @@
       <c r="G26" s="36"/>
     </row>
     <row r="27" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="44"/>
-      <c r="D27" s="45"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="40"/>
       <c r="E27" s="23">
         <v>5</v>
       </c>
@@ -5117,11 +5114,11 @@
       <c r="G27" s="36"/>
     </row>
     <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="44"/>
-      <c r="D28" s="45"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="40"/>
       <c r="E28" s="23">
         <v>5</v>
       </c>
@@ -5129,11 +5126,11 @@
       <c r="G28" s="36"/>
     </row>
     <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="44"/>
-      <c r="D29" s="45"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="40"/>
       <c r="E29" s="23">
         <v>1</v>
       </c>
@@ -5141,11 +5138,11 @@
       <c r="G29" s="36"/>
     </row>
     <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="43" t="s">
+      <c r="B30" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="44"/>
-      <c r="D30" s="45"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="40"/>
       <c r="E30" s="23">
         <v>2</v>
       </c>
@@ -5153,11 +5150,11 @@
       <c r="G30" s="36"/>
     </row>
     <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="41"/>
-      <c r="D31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="43"/>
       <c r="E31" s="24">
         <v>8</v>
       </c>
@@ -5165,11 +5162,11 @@
       <c r="G31" s="35"/>
     </row>
     <row r="32" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="45"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="40"/>
       <c r="E32" s="23">
         <v>5</v>
       </c>
@@ -5179,11 +5176,11 @@
       <c r="G32" s="36"/>
     </row>
     <row r="33" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="43" t="s">
+      <c r="B33" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="44"/>
-      <c r="D33" s="45"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="40"/>
       <c r="E33" s="23">
         <v>3</v>
       </c>
@@ -5193,11 +5190,11 @@
       <c r="G33" s="36"/>
     </row>
     <row r="34" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="41"/>
-      <c r="D34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="43"/>
       <c r="E34" s="24">
         <v>17</v>
       </c>
@@ -5205,11 +5202,11 @@
       <c r="G34" s="35"/>
     </row>
     <row r="35" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="45"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="40"/>
       <c r="E35" s="23">
         <v>4</v>
       </c>
@@ -5217,11 +5214,11 @@
       <c r="G35" s="36"/>
     </row>
     <row r="36" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="44"/>
-      <c r="D36" s="45"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="40"/>
       <c r="E36" s="23">
         <v>3</v>
       </c>
@@ -5229,11 +5226,11 @@
       <c r="G36" s="36"/>
     </row>
     <row r="37" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="43" t="s">
+      <c r="B37" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="44"/>
-      <c r="D37" s="45"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="40"/>
       <c r="E37" s="23">
         <v>5</v>
       </c>
@@ -5241,11 +5238,11 @@
       <c r="G37" s="36"/>
     </row>
     <row r="38" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="43" t="s">
+      <c r="B38" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="44"/>
-      <c r="D38" s="45"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="40"/>
       <c r="E38" s="23">
         <v>5</v>
       </c>
@@ -5255,11 +5252,11 @@
       <c r="G38" s="36"/>
     </row>
     <row r="39" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="41" t="s">
         <v>294</v>
       </c>
-      <c r="C39" s="41"/>
-      <c r="D39" s="42"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="43"/>
       <c r="E39" s="24">
         <v>0</v>
       </c>
@@ -5267,11 +5264,11 @@
       <c r="G39" s="36"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="43" t="s">
+      <c r="B40" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="C40" s="44"/>
-      <c r="D40" s="45"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="40"/>
       <c r="E40" s="23">
         <v>0</v>
       </c>
@@ -5281,11 +5278,11 @@
       <c r="G40" s="36"/>
     </row>
     <row r="41" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="43" t="s">
-        <v>296</v>
-      </c>
-      <c r="C41" s="44"/>
-      <c r="D41" s="45"/>
+      <c r="B41" s="38" t="s">
+        <v>295</v>
+      </c>
+      <c r="C41" s="39"/>
+      <c r="D41" s="40"/>
       <c r="E41" s="23">
         <v>0</v>
       </c>
@@ -5295,11 +5292,11 @@
       <c r="G41" s="36"/>
     </row>
     <row r="42" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="43" t="s">
-        <v>295</v>
-      </c>
-      <c r="C42" s="44"/>
-      <c r="D42" s="45"/>
+      <c r="B42" s="38" t="s">
+        <v>300</v>
+      </c>
+      <c r="C42" s="39"/>
+      <c r="D42" s="40"/>
       <c r="E42" s="23">
         <v>0</v>
       </c>
@@ -5309,11 +5306,11 @@
       <c r="G42" s="36"/>
     </row>
     <row r="43" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="43" t="s">
-        <v>301</v>
-      </c>
-      <c r="C43" s="44"/>
-      <c r="D43" s="45"/>
+      <c r="B43" s="38" t="s">
+        <v>299</v>
+      </c>
+      <c r="C43" s="39"/>
+      <c r="D43" s="40"/>
       <c r="E43" s="23">
         <v>0</v>
       </c>
@@ -5323,99 +5320,96 @@
       <c r="G43" s="36"/>
     </row>
     <row r="44" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="43" t="s">
-        <v>300</v>
-      </c>
-      <c r="C44" s="44"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="23">
-        <v>0</v>
-      </c>
-      <c r="F44" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="G44" s="36"/>
-    </row>
-    <row r="45" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="40" t="s">
+      <c r="B44" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C45" s="41"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="24">
+      <c r="C44" s="42"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="24">
         <v>105</v>
       </c>
-      <c r="F45" s="24">
+      <c r="F44" s="24">
         <f>SUMIF(F2:F38,"x",E2:E38)</f>
         <v>62</v>
       </c>
-      <c r="G45" s="35"/>
+      <c r="G44" s="35"/>
+    </row>
+    <row r="45" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="37"/>
     </row>
     <row r="46" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="37"/>
+      <c r="B46" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" s="22" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="47" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C47" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D47" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="E47" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="F47" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="26" t="s">
+      <c r="B47" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="23">
+      <c r="C47" s="23">
         <v>84</v>
       </c>
-      <c r="D48" s="23">
+      <c r="D47" s="23">
         <v>74</v>
       </c>
-      <c r="E48" s="23">
+      <c r="E47" s="23">
         <v>64</v>
       </c>
-      <c r="F48" s="23" t="s">
+      <c r="F47" s="23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="37"/>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
+  <mergeCells count="43">
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B27:D27"/>
@@ -5423,30 +5417,18 @@
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5771,7 +5753,10 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C9" s="15" t="s">
         <v>1</v>
       </c>
@@ -5846,7 +5831,10 @@
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C15" s="15" t="s">
         <v>127</v>
       </c>
@@ -5993,7 +5981,10 @@
         <v>137</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C27" s="15" t="s">
         <v>127</v>
       </c>
@@ -6917,22 +6908,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="10"/>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -7017,7 +7008,7 @@
         <v>67</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>66</v>
@@ -7109,7 +7100,7 @@
         <v>70</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>70</v>
@@ -7139,7 +7130,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Presentation PP and small fix to ConverArrayTest.
</commit_message>
<xml_diff>
--- a/doc/notes.xlsx
+++ b/doc/notes.xlsx
@@ -492,7 +492,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="301">
   <si>
     <t>Design</t>
   </si>
@@ -1814,130 +1814,6 @@
   </cellStyles>
   <dxfs count="125">
     <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8892BF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5382A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDDA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEF652A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF35A9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF76B64A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2152,6 +2028,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2173,6 +2054,68 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2270,6 +2213,63 @@
     </dxf>
     <dxf>
       <alignment vertical="top" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8892BF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5382A1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDDA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF652A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF35A9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B64A"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3894,46 +3894,6 @@
     <i/>
   </colItems>
   <formats count="33">
-    <format dxfId="106">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="105">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="104">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="103">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="102">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="101">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
-    </format>
     <format dxfId="100">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
@@ -3949,6 +3909,46 @@
       </pivotArea>
     </format>
     <format dxfId="99">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="98">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="97">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="96">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="95">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="94">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="93">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3962,7 +3962,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="98">
+    <format dxfId="92">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3975,7 +3975,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="97">
+    <format dxfId="91">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3988,7 +3988,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="96">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4004,7 +4004,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="95">
+    <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4016,7 +4016,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="94">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4028,16 +4028,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="93">
+    <format dxfId="87">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="92">
+    <format dxfId="86">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="91">
+    <format dxfId="85">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="90">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="6">
@@ -4051,7 +4051,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="83">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4065,7 +4065,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4078,7 +4078,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="81">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4091,7 +4091,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="80">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4107,7 +4107,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="79">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4119,7 +4119,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="84">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4131,10 +4131,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="77">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="82">
+    <format dxfId="76">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4143,7 +4143,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="75">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4152,7 +4152,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="74">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4161,7 +4161,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="73">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4170,7 +4170,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="72">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -4179,7 +4179,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="71">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4191,7 +4191,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="70">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4204,7 +4204,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="69">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4217,7 +4217,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="68">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -4369,7 +4369,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F36" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Task_List" displayName="Task_List" ref="B2:F36" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="B2:F36">
     <filterColumn colId="0">
       <filters blank="1"/>
@@ -4379,103 +4379,103 @@
     <sortCondition ref="C2:C30"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Done" dataDxfId="71"/>
-    <tableColumn id="3" name="Category" dataDxfId="70"/>
-    <tableColumn id="5" name="Remember" dataDxfId="69"/>
-    <tableColumn id="4" name="Look Into" dataDxfId="68"/>
-    <tableColumn id="2" name="Task" dataDxfId="67"/>
+    <tableColumn id="1" name="Done" dataDxfId="58"/>
+    <tableColumn id="3" name="Category" dataDxfId="57"/>
+    <tableColumn id="5" name="Remember" dataDxfId="56"/>
+    <tableColumn id="4" name="Look Into" dataDxfId="55"/>
+    <tableColumn id="2" name="Task" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:D31" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:D31" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="B2:D31">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="Done" dataDxfId="64"/>
-    <tableColumn id="2" name="File" dataDxfId="63"/>
-    <tableColumn id="3" name="Feature" dataDxfId="62"/>
+    <tableColumn id="1" name="Done" dataDxfId="50"/>
+    <tableColumn id="2" name="File" dataDxfId="49"/>
+    <tableColumn id="3" name="Feature" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q14" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Databases" displayName="Databases" ref="A1:Q14" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A1:Q14"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Name" dataDxfId="59"/>
-    <tableColumn id="2" name="Foreign Key1" dataDxfId="58"/>
-    <tableColumn id="3" name="Foreign Key2" dataDxfId="57"/>
-    <tableColumn id="4" name="Column1" dataDxfId="56"/>
-    <tableColumn id="5" name="Column2" dataDxfId="55"/>
-    <tableColumn id="6" name="Column3" dataDxfId="54"/>
-    <tableColumn id="7" name="Column4" dataDxfId="53"/>
-    <tableColumn id="8" name="Column5" dataDxfId="52"/>
-    <tableColumn id="9" name="Column6" dataDxfId="51"/>
-    <tableColumn id="13" name="Column7" dataDxfId="50"/>
-    <tableColumn id="12" name="Column8" dataDxfId="49"/>
-    <tableColumn id="11" name="Column9" dataDxfId="48"/>
-    <tableColumn id="17" name="Column10" dataDxfId="47"/>
-    <tableColumn id="16" name="Column11" dataDxfId="46"/>
-    <tableColumn id="15" name="Column12" dataDxfId="45"/>
-    <tableColumn id="14" name="Column13" dataDxfId="44"/>
-    <tableColumn id="10" name="Column14" dataDxfId="43"/>
+    <tableColumn id="1" name="Name" dataDxfId="45"/>
+    <tableColumn id="2" name="Foreign Key1" dataDxfId="44"/>
+    <tableColumn id="3" name="Foreign Key2" dataDxfId="43"/>
+    <tableColumn id="4" name="Column1" dataDxfId="42"/>
+    <tableColumn id="5" name="Column2" dataDxfId="41"/>
+    <tableColumn id="6" name="Column3" dataDxfId="40"/>
+    <tableColumn id="7" name="Column4" dataDxfId="39"/>
+    <tableColumn id="8" name="Column5" dataDxfId="38"/>
+    <tableColumn id="9" name="Column6" dataDxfId="37"/>
+    <tableColumn id="13" name="Column7" dataDxfId="36"/>
+    <tableColumn id="12" name="Column8" dataDxfId="35"/>
+    <tableColumn id="11" name="Column9" dataDxfId="34"/>
+    <tableColumn id="17" name="Column10" dataDxfId="33"/>
+    <tableColumn id="16" name="Column11" dataDxfId="32"/>
+    <tableColumn id="15" name="Column12" dataDxfId="31"/>
+    <tableColumn id="14" name="Column13" dataDxfId="30"/>
+    <tableColumn id="10" name="Column14" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Use_Cases" displayName="Use_Cases" ref="A2:L108" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A2:L108"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Notes: Client" dataDxfId="40"/>
-    <tableColumn id="2" name="A:C" dataDxfId="39"/>
-    <tableColumn id="3" name="U" dataDxfId="38"/>
-    <tableColumn id="4" name="S" dataDxfId="37"/>
-    <tableColumn id="5" name="Use Case: Client" dataDxfId="36"/>
-    <tableColumn id="6" name="Conversation" dataDxfId="35"/>
-    <tableColumn id="8" name="Use Case: Server" dataDxfId="34"/>
-    <tableColumn id="13" name="G" dataDxfId="33"/>
-    <tableColumn id="9" name="A:S" dataDxfId="32"/>
-    <tableColumn id="10" name="D" dataDxfId="31"/>
-    <tableColumn id="11" name="C" dataDxfId="30"/>
-    <tableColumn id="12" name="Notes: Server" dataDxfId="29"/>
+    <tableColumn id="1" name="Notes: Client" dataDxfId="26"/>
+    <tableColumn id="2" name="A:C" dataDxfId="25"/>
+    <tableColumn id="3" name="U" dataDxfId="24"/>
+    <tableColumn id="4" name="S" dataDxfId="23"/>
+    <tableColumn id="5" name="Use Case: Client" dataDxfId="22"/>
+    <tableColumn id="6" name="Conversation" dataDxfId="21"/>
+    <tableColumn id="8" name="Use Case: Server" dataDxfId="20"/>
+    <tableColumn id="13" name="G" dataDxfId="19"/>
+    <tableColumn id="9" name="A:S" dataDxfId="18"/>
+    <tableColumn id="10" name="D" dataDxfId="17"/>
+    <tableColumn id="11" name="C" dataDxfId="16"/>
+    <tableColumn id="12" name="Notes: Server" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:D21"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Type" dataDxfId="26"/>
-    <tableColumn id="6" name="Name" dataDxfId="25"/>
-    <tableColumn id="2" name="Messages" dataDxfId="24"/>
-    <tableColumn id="3" name="Collaborators" dataDxfId="23"/>
+    <tableColumn id="1" name="Type" dataDxfId="12"/>
+    <tableColumn id="6" name="Name" dataDxfId="11"/>
+    <tableColumn id="2" name="Messages" dataDxfId="10"/>
+    <tableColumn id="3" name="Collaborators" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G25" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G25"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Name" dataDxfId="20"/>
-    <tableColumn id="7" name="Dependencies" dataDxfId="19"/>
-    <tableColumn id="6" name="Route" dataDxfId="18"/>
-    <tableColumn id="2" name="Controller" dataDxfId="17"/>
-    <tableColumn id="4" name="Directive" dataDxfId="16"/>
-    <tableColumn id="3" name="Factory" dataDxfId="15"/>
-    <tableColumn id="5" name="Service" dataDxfId="14"/>
+    <tableColumn id="1" name="Name" dataDxfId="6"/>
+    <tableColumn id="7" name="Dependencies" dataDxfId="5"/>
+    <tableColumn id="6" name="Route" dataDxfId="4"/>
+    <tableColumn id="2" name="Controller" dataDxfId="3"/>
+    <tableColumn id="4" name="Directive" dataDxfId="2"/>
+    <tableColumn id="3" name="Factory" dataDxfId="1"/>
+    <tableColumn id="5" name="Service" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Senior Project: Red" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4747,8 +4747,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4920,9 +4920,7 @@
       <c r="E13" s="23">
         <v>1</v>
       </c>
-      <c r="F13" s="23" t="s">
-        <v>280</v>
-      </c>
+      <c r="F13" s="23"/>
       <c r="G13" s="36"/>
     </row>
     <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4934,9 +4932,7 @@
       <c r="E14" s="23">
         <v>1</v>
       </c>
-      <c r="F14" s="23" t="s">
-        <v>280</v>
-      </c>
+      <c r="F14" s="23"/>
       <c r="G14" s="36"/>
     </row>
     <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5386,6 +5382,37 @@
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B2:D2"/>
@@ -5398,37 +5425,6 @@
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5603,22 +5599,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B25:C1048576 B1:C21">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="106" priority="1">
       <formula>$B1="Setup"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="105" priority="2">
       <formula>$B1="CSS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="104" priority="3">
       <formula>$B1="HTML"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="103" priority="4">
       <formula>$B1="JS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="102" priority="5">
       <formula>$B1="DB"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="101" priority="6">
       <formula>$B1="PHP"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6065,29 +6061,29 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="C1:E1048576">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="CSS">
+    <cfRule type="containsText" dxfId="67" priority="2" operator="containsText" text="CSS">
       <formula>NOT(ISERROR(SEARCH("CSS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="HTML">
+    <cfRule type="containsText" dxfId="66" priority="3" operator="containsText" text="HTML">
       <formula>NOT(ISERROR(SEARCH("HTML",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="JS">
+    <cfRule type="containsText" dxfId="65" priority="4" operator="containsText" text="JS">
       <formula>NOT(ISERROR(SEARCH("JS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="DB">
+    <cfRule type="containsText" dxfId="64" priority="5" operator="containsText" text="DB">
       <formula>NOT(ISERROR(SEARCH("DB",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="PHP">
+    <cfRule type="containsText" dxfId="63" priority="6" operator="containsText" text="PHP">
       <formula>NOT(ISERROR(SEARCH("PHP",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Setup">
+    <cfRule type="containsText" dxfId="62" priority="1" operator="containsText" text="Setup">
       <formula>NOT(ISERROR(SEARCH("Setup",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F1048576">
-    <cfRule type="expression" dxfId="1" priority="9">
+    <cfRule type="expression" dxfId="61" priority="9">
       <formula>$B2="x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6352,7 +6348,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="53" priority="1">
       <formula>$C5="x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>